<commit_message>
Eliminate extraneous rows of commas from bldgs/BCEU
</commit_message>
<xml_diff>
--- a/InputData/bldgs/BCEU/BAU Components Energy Use.xlsx
+++ b/InputData/bldgs/BCEU/BAU Components Energy Use.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-1.5.0-us-wipJ\InputData\bldgs\BCEU\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="18195" windowHeight="4020" tabRatio="776" firstSheet="13" activeTab="19"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="18195" windowHeight="4020" tabRatio="776"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -33,7 +28,7 @@
     <sheet name="BCEU-commercial-appl" sheetId="16" r:id="rId19"/>
     <sheet name="BCEU-commercial-other" sheetId="17" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1965,15 +1960,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.000E+00"/>
     <numFmt numFmtId="167" formatCode="@*."/>
     <numFmt numFmtId="168" formatCode="#,##0.0"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="0.00000000000000000"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -2335,7 +2328,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2495,9 +2488,6 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2595,7 +2585,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2630,7 +2620,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2841,9 +2831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3327,7 +3315,7 @@
       </c>
       <c r="C2" s="67">
         <f t="shared" ref="C2:D2" si="0">TREND($E$2:$G$2,$E$1:$G$1,C1)</f>
-        <v>1607676980259447.8</v>
+        <v>1607676980259447.7</v>
       </c>
       <c r="D2" s="67">
         <f t="shared" si="0"/>
@@ -3335,11 +3323,11 @@
       </c>
       <c r="E2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(E$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(E$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>1606825855329949.3</v>
+        <v>1606825855329949.2</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(F$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(F$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>1607001314720812.3</v>
+        <v>1607001314720812.2</v>
       </c>
       <c r="G2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(G$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(G$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -3347,19 +3335,19 @@
       </c>
       <c r="H2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(H$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(H$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>1604837315566835.8</v>
+        <v>1604837315566835.7</v>
       </c>
       <c r="I2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(I$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(I$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>1603223730118443.3</v>
+        <v>1603223730118443.2</v>
       </c>
       <c r="J2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(J$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(J$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>1602208629441624.3</v>
+        <v>1602208629441624.2</v>
       </c>
       <c r="K2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(K$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(K$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>1610423974619289.3</v>
+        <v>1610423974619289.2</v>
       </c>
       <c r="L2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(L$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(L$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -3371,7 +3359,7 @@
       </c>
       <c r="N2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(N$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(N$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>1644842857868020.3</v>
+        <v>1644842857868020.2</v>
       </c>
       <c r="O2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(O$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(O$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -3383,7 +3371,7 @@
       </c>
       <c r="Q2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(Q$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(Q$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>1686129494077834.3</v>
+        <v>1686129494077834.2</v>
       </c>
       <c r="R2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(R$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(R$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -3391,7 +3379,7 @@
       </c>
       <c r="S2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(S$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(S$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>1718649570219966.3</v>
+        <v>1718649570219966.2</v>
       </c>
       <c r="T2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(T$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(T$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -3403,11 +3391,11 @@
       </c>
       <c r="V2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(V$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(V$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>1771186438240270.8</v>
+        <v>1771186438240270.7</v>
       </c>
       <c r="W2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(W$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(W$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>1788844543147208.3</v>
+        <v>1788844543147208.2</v>
       </c>
       <c r="X2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(X$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(X$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -3415,11 +3403,11 @@
       </c>
       <c r="Y2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(Y$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(Y$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>1825296031302876.3</v>
+        <v>1825296031302876.2</v>
       </c>
       <c r="Z2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(Z$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(Z$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>1842439775803722.8</v>
+        <v>1842439775803722.7</v>
       </c>
       <c r="AA2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(AA$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(AA$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -3439,11 +3427,11 @@
       </c>
       <c r="AE2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(AE$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(AE$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>1928205768189509.3</v>
+        <v>1928205768189509.2</v>
       </c>
       <c r="AF2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(AF$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(AF$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>1944690137901861.3</v>
+        <v>1944690137901861.2</v>
       </c>
       <c r="AG2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(AG$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(AG$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -3451,7 +3439,7 @@
       </c>
       <c r="AH2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(AH$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(AH$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>1976281641285956.3</v>
+        <v>1976281641285956.2</v>
       </c>
       <c r="AI2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(AI$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(AI$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -3603,7 +3591,7 @@
       </c>
       <c r="J4" s="9">
         <f>INDEX('AEO Table 4'!$C$56:$AJ$56,0,MATCH(J$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>178806739424703.88</v>
+        <v>178806739424703.87</v>
       </c>
       <c r="K4" s="9">
         <f>INDEX('AEO Table 4'!$C$56:$AJ$56,0,MATCH(K$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -3615,7 +3603,7 @@
       </c>
       <c r="M4" s="9">
         <f>INDEX('AEO Table 4'!$C$56:$AJ$56,0,MATCH(M$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>176208498307952.63</v>
+        <v>176208498307952.62</v>
       </c>
       <c r="N4" s="9">
         <f>INDEX('AEO Table 4'!$C$56:$AJ$56,0,MATCH(N$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -3627,7 +3615,7 @@
       </c>
       <c r="P4" s="9">
         <f>INDEX('AEO Table 4'!$C$56:$AJ$56,0,MATCH(P$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>172945274111675.13</v>
+        <v>172945274111675.12</v>
       </c>
       <c r="Q4" s="9">
         <f>INDEX('AEO Table 4'!$C$56:$AJ$56,0,MATCH(Q$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -3655,11 +3643,11 @@
       </c>
       <c r="W4" s="9">
         <f>INDEX('AEO Table 4'!$C$56:$AJ$56,0,MATCH(W$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>167916239424703.88</v>
+        <v>167916239424703.87</v>
       </c>
       <c r="X4" s="9">
         <f>INDEX('AEO Table 4'!$C$56:$AJ$56,0,MATCH(X$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>167284104906937.38</v>
+        <v>167284104906937.37</v>
       </c>
       <c r="Y4" s="9">
         <f>INDEX('AEO Table 4'!$C$56:$AJ$56,0,MATCH(Y$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -3699,7 +3687,7 @@
       </c>
       <c r="AH4" s="9">
         <f>INDEX('AEO Table 4'!$C$56:$AJ$56,0,MATCH(AH$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>160557360406091.38</v>
+        <v>160557360406091.37</v>
       </c>
       <c r="AI4" s="9">
         <f>INDEX('AEO Table 4'!$C$56:$AJ$56,0,MATCH(AI$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -3760,7 +3748,7 @@
       </c>
       <c r="N5" s="9">
         <f>INDEX('AEO Table 4'!$C$62:$AK$62,MATCH(N$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>5593068527918.7813</v>
+        <v>5593068527918.7812</v>
       </c>
       <c r="O5" s="9">
         <f>INDEX('AEO Table 4'!$C$62:$AK$62,MATCH(O$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -4409,7 +4397,7 @@
       </c>
       <c r="AH10" s="9">
         <f>INDEX('AEO Table 4'!$C$69:$AK$69,MATCH(AH$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>91507280033840.938</v>
+        <v>91507280033840.937</v>
       </c>
       <c r="AI10" s="9">
         <f>INDEX('AEO Table 4'!$C$69:$AK$69,MATCH(AI$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -4717,7 +4705,7 @@
       </c>
       <c r="O2" s="9">
         <f>INDEX('AEO Table 4'!$C$34:$AK$34,MATCH(O$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>114409412013536.38</v>
+        <v>114409412013536.37</v>
       </c>
       <c r="P2" s="9">
         <f>INDEX('AEO Table 4'!$C$34:$AK$34,MATCH(P$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -4769,7 +4757,7 @@
       </c>
       <c r="AB2" s="9">
         <f>INDEX('AEO Table 4'!$C$34:$AK$34,MATCH(AB$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>98826049069373.938</v>
+        <v>98826049069373.937</v>
       </c>
       <c r="AC2" s="9">
         <f>INDEX('AEO Table 4'!$C$34:$AK$34,MATCH(AC$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -4921,7 +4909,7 @@
       </c>
       <c r="D4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(D$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>706925528764805.38</v>
+        <v>706925528764805.37</v>
       </c>
       <c r="E4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(E$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -4929,31 +4917,31 @@
       </c>
       <c r="F4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(F$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>670331336717428.13</v>
+        <v>670331336717428.12</v>
       </c>
       <c r="G4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(G$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>666596983925549.88</v>
+        <v>666596983925549.87</v>
       </c>
       <c r="H4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(H$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>662432394247038.88</v>
+        <v>662432394247038.87</v>
       </c>
       <c r="I4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(I$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>657832000846023.63</v>
+        <v>657832000846023.62</v>
       </c>
       <c r="J4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(J$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>653308350253807.13</v>
+        <v>653308350253807.12</v>
       </c>
       <c r="K4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(K$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>649157081218274.13</v>
+        <v>649157081218274.12</v>
       </c>
       <c r="L4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(L$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>645603252961082.88</v>
+        <v>645603252961082.87</v>
       </c>
       <c r="M4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(M$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -4965,7 +4953,7 @@
       </c>
       <c r="O4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(O$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>635323494077834.13</v>
+        <v>635323494077834.12</v>
       </c>
       <c r="P4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(P$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -4989,11 +4977,11 @@
       </c>
       <c r="U4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(U$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>619232157360406.13</v>
+        <v>619232157360406.12</v>
       </c>
       <c r="V4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(V$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>617003236040609.13</v>
+        <v>617003236040609.12</v>
       </c>
       <c r="W4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(W$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -5005,7 +4993,7 @@
       </c>
       <c r="Y4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(Y$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>611293849407783.38</v>
+        <v>611293849407783.37</v>
       </c>
       <c r="Z4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(Z$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -5017,7 +5005,7 @@
       </c>
       <c r="AB4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(AB$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>605960423011844.38</v>
+        <v>605960423011844.37</v>
       </c>
       <c r="AC4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(AC$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -5029,11 +5017,11 @@
       </c>
       <c r="AE4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(AE$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>600392195431472.13</v>
+        <v>600392195431472.12</v>
       </c>
       <c r="AF4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(AF$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>598554543147208.13</v>
+        <v>598554543147208.12</v>
       </c>
       <c r="AG4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(AG$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -5041,7 +5029,7 @@
       </c>
       <c r="AH4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(AH$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>594326928934010.13</v>
+        <v>594326928934010.12</v>
       </c>
       <c r="AI4" s="9">
         <f>INDEX('AEO Table 4'!$C$51:$AK$51,MATCH(AI$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -5070,7 +5058,7 @@
       </c>
       <c r="F5" s="9">
         <f>INDEX('AEO Table 4'!$C$60:$AK$60,MATCH(F$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>71548950930626.063</v>
+        <v>71548950930626.062</v>
       </c>
       <c r="G5" s="9">
         <f>INDEX('AEO Table 4'!$C$60:$AK$60,MATCH(G$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -5142,11 +5130,11 @@
       </c>
       <c r="X5" s="9">
         <f>INDEX('AEO Table 4'!$C$60:$AK$60,MATCH(X$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>46257821489001.688</v>
+        <v>46257821489001.687</v>
       </c>
       <c r="Y5" s="9">
         <f>INDEX('AEO Table 4'!$C$60:$AK$60,MATCH(Y$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>45284818104906.938</v>
+        <v>45284818104906.937</v>
       </c>
       <c r="Z5" s="9">
         <f>INDEX('AEO Table 4'!$C$60:$AK$60,MATCH(Z$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -5306,7 +5294,7 @@
       </c>
       <c r="C7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(C$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>87349818104906.938</v>
+        <v>87349818104906.937</v>
       </c>
       <c r="D7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(D$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -5314,7 +5302,7 @@
       </c>
       <c r="E7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(E$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>86830909475465.313</v>
+        <v>86830909475465.312</v>
       </c>
       <c r="F7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(F$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -5334,7 +5322,7 @@
       </c>
       <c r="J7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(J$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>83237914551607.438</v>
+        <v>83237914551607.437</v>
       </c>
       <c r="K7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(K$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -5402,11 +5390,11 @@
       </c>
       <c r="AA7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(AA$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>73319005922165.813</v>
+        <v>73319005922165.812</v>
       </c>
       <c r="AB7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(AB$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>72648997461928.938</v>
+        <v>72648997461928.937</v>
       </c>
       <c r="AC7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(AC$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -5681,7 +5669,7 @@
       </c>
       <c r="H10">
         <f>INDEX('AEO Table 4'!$C$66:$AK$66,MATCH(H$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>57534043993231.813</v>
+        <v>57534043993231.812</v>
       </c>
       <c r="I10">
         <f>INDEX('AEO Table 4'!$C$66:$AK$66,MATCH(I$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -5773,7 +5761,7 @@
       </c>
       <c r="AE10">
         <f>INDEX('AEO Table 4'!$C$66:$AK$66,MATCH(AE$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>43421319796954.313</v>
+        <v>43421319796954.312</v>
       </c>
       <c r="AF10">
         <f>INDEX('AEO Table 4'!$C$66:$AK$66,MATCH(AF$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -6069,7 +6057,7 @@
       </c>
       <c r="I2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(I$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(I$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>156017136209813.88</v>
+        <v>156017136209813.87</v>
       </c>
       <c r="J2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(J$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(J$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -6077,11 +6065,11 @@
       </c>
       <c r="K2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(K$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(K$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>157850812182741.13</v>
+        <v>157850812182741.12</v>
       </c>
       <c r="L2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(L$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(L$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>159053646362098.13</v>
+        <v>159053646362098.12</v>
       </c>
       <c r="M2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(M$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(M$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -6093,7 +6081,7 @@
       </c>
       <c r="O2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(O$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(O$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>163545287648054.13</v>
+        <v>163545287648054.12</v>
       </c>
       <c r="P2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(P$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(P$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -7431,7 +7419,7 @@
       </c>
       <c r="AE2" s="9">
         <f>INDEX('AEO Table 4'!$C$41:$AK$41,MATCH(AE$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>37797821489001.688</v>
+        <v>37797821489001.687</v>
       </c>
       <c r="AF2" s="9">
         <f>INDEX('AEO Table 4'!$C$41:$AK$41,MATCH(AF$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -8564,7 +8552,7 @@
       </c>
       <c r="C2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(C$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(C$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
-        <v>254169001692047.38</v>
+        <v>254169001692047.37</v>
       </c>
       <c r="D2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(D$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(D$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
@@ -8576,11 +8564,11 @@
       </c>
       <c r="F2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(F$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(F$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
-        <v>256979657360406.13</v>
+        <v>256979657360406.12</v>
       </c>
       <c r="G2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(G$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(G$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
-        <v>257538925549915.38</v>
+        <v>257538925549915.37</v>
       </c>
       <c r="H2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(H$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(H$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
@@ -8604,7 +8592,7 @@
       </c>
       <c r="M2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(M$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(M$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
-        <v>256701315566835.88</v>
+        <v>256701315566835.87</v>
       </c>
       <c r="N2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(N$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(N$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
@@ -8632,7 +8620,7 @@
       </c>
       <c r="T2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(T$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(T$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
-        <v>260242021996615.88</v>
+        <v>260242021996615.87</v>
       </c>
       <c r="U2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(U$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(U$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
@@ -8640,7 +8628,7 @@
       </c>
       <c r="V2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(V$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(V$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
-        <v>262586852791878.13</v>
+        <v>262586852791878.12</v>
       </c>
       <c r="W2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(W$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(W$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
@@ -8652,7 +8640,7 @@
       </c>
       <c r="Y2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(Y$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(Y$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
-        <v>266762377326565.13</v>
+        <v>266762377326565.12</v>
       </c>
       <c r="Z2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(Z$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(Z$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
@@ -8820,7 +8808,7 @@
       </c>
       <c r="E4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(E$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
-        <v>225538367174280.88</v>
+        <v>225538367174280.87</v>
       </c>
       <c r="F4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(F$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
@@ -8832,7 +8820,7 @@
       </c>
       <c r="H4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(H$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
-        <v>225786687817258.88</v>
+        <v>225786687817258.87</v>
       </c>
       <c r="I4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(I$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
@@ -8840,7 +8828,7 @@
       </c>
       <c r="J4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(J$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
-        <v>226952542301184.38</v>
+        <v>226952542301184.37</v>
       </c>
       <c r="K4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(K$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
@@ -8880,7 +8868,7 @@
       </c>
       <c r="T4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(T$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
-        <v>244536785109983.13</v>
+        <v>244536785109983.12</v>
       </c>
       <c r="U4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(U$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
@@ -8892,7 +8880,7 @@
       </c>
       <c r="W4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(W$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
-        <v>250141594754653.13</v>
+        <v>250141594754653.12</v>
       </c>
       <c r="X4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(X$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
@@ -9614,7 +9602,7 @@
       </c>
       <c r="Z10">
         <f>SUM(INDEX('AEO Table 4'!$C$67:$AJ$68,0,MATCH(Z$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
-        <v>8741522842639.5938</v>
+        <v>8741522842639.5937</v>
       </c>
       <c r="AA10">
         <f>SUM(INDEX('AEO Table 4'!$C$67:$AJ$68,0,MATCH(AA$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69</f>
@@ -9927,7 +9915,7 @@
       </c>
       <c r="H2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(H$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(H$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>398243684433164.13</v>
+        <v>398243684433164.12</v>
       </c>
       <c r="I2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(I$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(I$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -9935,11 +9923,11 @@
       </c>
       <c r="J2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(J$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(J$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>397591370558375.63</v>
+        <v>397591370558375.62</v>
       </c>
       <c r="K2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(K$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(K$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>399630025380710.63</v>
+        <v>399630025380710.62</v>
       </c>
       <c r="L2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(L$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(L$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -9947,7 +9935,7 @@
       </c>
       <c r="M2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(M$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(M$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>405061070219966.13</v>
+        <v>405061070219966.12</v>
       </c>
       <c r="N2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(N$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(N$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -9955,7 +9943,7 @@
       </c>
       <c r="O2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(O$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(O$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>411389767343485.63</v>
+        <v>411389767343485.62</v>
       </c>
       <c r="P2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(P$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(P$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -9967,7 +9955,7 @@
       </c>
       <c r="R2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(R$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(R$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>421978286802030.38</v>
+        <v>421978286802030.37</v>
       </c>
       <c r="S2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(S$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(S$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -9987,7 +9975,7 @@
       </c>
       <c r="W2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(W$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(W$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>443905456852791.88</v>
+        <v>443905456852791.87</v>
       </c>
       <c r="X2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$44:$AJ$45,0,MATCH(X$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$69+INDEX('AEO Table 4'!$C$47:$AJ$47,MATCH(X$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
@@ -10283,7 +10271,7 @@
       </c>
       <c r="AI4" s="9">
         <f>INDEX('AEO Table 4'!$C$56:$AJ$56,0,MATCH(AI$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$69</f>
-        <v>39667681895093.063</v>
+        <v>39667681895093.062</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -11114,14 +11102,14 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AK24"/>
+  <dimension ref="A1:AK11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M41" sqref="M41"/>
       <selection pane="topRight" activeCell="M41" sqref="M41"/>
       <selection pane="bottomLeft" activeCell="M41" sqref="M41"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11782,7 +11770,7 @@
       </c>
       <c r="C6" s="9">
         <f>'District Heat'!C9</f>
-        <v>375086476892834.88</v>
+        <v>375086476892834.87</v>
       </c>
       <c r="D6" s="9">
         <f>'District Heat'!D9</f>
@@ -11826,7 +11814,7 @@
       </c>
       <c r="N6" s="9">
         <f>'District Heat'!N9</f>
-        <v>335953845875489.13</v>
+        <v>335953845875489.12</v>
       </c>
       <c r="O6" s="9">
         <f>'District Heat'!O9</f>
@@ -11850,7 +11838,7 @@
       </c>
       <c r="T6" s="9">
         <f>'District Heat'!T9</f>
-        <v>326534871984644.38</v>
+        <v>326534871984644.37</v>
       </c>
       <c r="U6" s="9">
         <f>'District Heat'!U9</f>
@@ -12244,7 +12232,7 @@
       </c>
       <c r="C10">
         <f>(INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(C$1,'AEO Table 5'!$C$1:$AK$1,0))*(1-About!$C$50))*INDEX('AEO Table 5'!$C$52:$AK$52,MATCH(C$1,'AEO Table 5'!$C$1:$AK$1,0))/INDEX('AEO Table 5'!$C$55:$AK$55,MATCH(C$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15</f>
-        <v>364266499418248.63</v>
+        <v>364266499418248.62</v>
       </c>
       <c r="D10">
         <f>(INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(D$1,'AEO Table 5'!$C$1:$AK$1,0))*(1-About!$C$50))*INDEX('AEO Table 5'!$C$52:$AK$52,MATCH(D$1,'AEO Table 5'!$C$1:$AK$1,0))/INDEX('AEO Table 5'!$C$55:$AK$55,MATCH(D$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15</f>
@@ -12272,7 +12260,7 @@
       </c>
       <c r="J10">
         <f>(INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(J$1,'AEO Table 5'!$C$1:$AK$1,0))*(1-About!$C$50))*INDEX('AEO Table 5'!$C$52:$AK$52,MATCH(J$1,'AEO Table 5'!$C$1:$AK$1,0))/INDEX('AEO Table 5'!$C$55:$AK$55,MATCH(J$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15</f>
-        <v>332344541212124.88</v>
+        <v>332344541212124.87</v>
       </c>
       <c r="K10">
         <f>(INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(K$1,'AEO Table 5'!$C$1:$AK$1,0))*(1-About!$C$50))*INDEX('AEO Table 5'!$C$52:$AK$52,MATCH(K$1,'AEO Table 5'!$C$1:$AK$1,0))/INDEX('AEO Table 5'!$C$55:$AK$55,MATCH(K$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15</f>
@@ -12280,11 +12268,11 @@
       </c>
       <c r="L10">
         <f>(INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(L$1,'AEO Table 5'!$C$1:$AK$1,0))*(1-About!$C$50))*INDEX('AEO Table 5'!$C$52:$AK$52,MATCH(L$1,'AEO Table 5'!$C$1:$AK$1,0))/INDEX('AEO Table 5'!$C$55:$AK$55,MATCH(L$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15</f>
-        <v>327454683292015.63</v>
+        <v>327454683292015.62</v>
       </c>
       <c r="M10">
         <f>(INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(M$1,'AEO Table 5'!$C$1:$AK$1,0))*(1-About!$C$50))*INDEX('AEO Table 5'!$C$52:$AK$52,MATCH(M$1,'AEO Table 5'!$C$1:$AK$1,0))/INDEX('AEO Table 5'!$C$55:$AK$55,MATCH(M$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15</f>
-        <v>326778697874473.63</v>
+        <v>326778697874473.62</v>
       </c>
       <c r="N10">
         <f>(INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(N$1,'AEO Table 5'!$C$1:$AK$1,0))*(1-About!$C$50))*INDEX('AEO Table 5'!$C$52:$AK$52,MATCH(N$1,'AEO Table 5'!$C$1:$AK$1,0))/INDEX('AEO Table 5'!$C$55:$AK$55,MATCH(N$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15</f>
@@ -12292,7 +12280,7 @@
       </c>
       <c r="O10">
         <f>(INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(O$1,'AEO Table 5'!$C$1:$AK$1,0))*(1-About!$C$50))*INDEX('AEO Table 5'!$C$52:$AK$52,MATCH(O$1,'AEO Table 5'!$C$1:$AK$1,0))/INDEX('AEO Table 5'!$C$55:$AK$55,MATCH(O$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15</f>
-        <v>326078188440129.38</v>
+        <v>326078188440129.37</v>
       </c>
       <c r="P10">
         <f>(INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(P$1,'AEO Table 5'!$C$1:$AK$1,0))*(1-About!$C$50))*INDEX('AEO Table 5'!$C$52:$AK$52,MATCH(P$1,'AEO Table 5'!$C$1:$AK$1,0))/INDEX('AEO Table 5'!$C$55:$AK$55,MATCH(P$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15</f>
@@ -12352,7 +12340,7 @@
       </c>
       <c r="AD10">
         <f>(INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(AD$1,'AEO Table 5'!$C$1:$AK$1,0))*(1-About!$C$50))*INDEX('AEO Table 5'!$C$52:$AK$52,MATCH(AD$1,'AEO Table 5'!$C$1:$AK$1,0))/INDEX('AEO Table 5'!$C$55:$AK$55,MATCH(AD$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15</f>
-        <v>322641245121938.38</v>
+        <v>322641245121938.37</v>
       </c>
       <c r="AE10">
         <f>(INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(AE$1,'AEO Table 5'!$C$1:$AK$1,0))*(1-About!$C$50))*INDEX('AEO Table 5'!$C$52:$AK$52,MATCH(AE$1,'AEO Table 5'!$C$1:$AK$1,0))/INDEX('AEO Table 5'!$C$55:$AK$55,MATCH(AE$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15</f>
@@ -12481,63 +12469,6 @@
       <c r="AI11" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="71"/>
-    </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="E15" s="70"/>
-      <c r="G15" s="71"/>
-    </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="71"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="71"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="E18" s="70"/>
-      <c r="G18" s="71"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="E19" s="70"/>
-      <c r="G19" s="71"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="E20" s="70"/>
-      <c r="G20" s="71"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="E21" s="70"/>
-      <c r="G21" s="71"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="E22" s="69"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="71"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="E23" s="70"/>
-      <c r="G23" s="71"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G24" s="70"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16315,7 +16246,7 @@
       </c>
       <c r="AD10">
         <f>(INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(AD$1,'AEO Table 5'!$C$1:$AK$1,0))*(1-About!$C$50))*INDEX('AEO Table 5'!$C$53:$AK$53,MATCH(AD$1,'AEO Table 5'!$C$1:$AK$1,0))/INDEX('AEO Table 5'!$C$55:$AK$55,MATCH(AD$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15</f>
-        <v>11208390649743.313</v>
+        <v>11208390649743.312</v>
       </c>
       <c r="AE10">
         <f>(INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(AE$1,'AEO Table 5'!$C$1:$AK$1,0))*(1-About!$C$50))*INDEX('AEO Table 5'!$C$53:$AK$53,MATCH(AE$1,'AEO Table 5'!$C$1:$AK$1,0))/INDEX('AEO Table 5'!$C$55:$AK$55,MATCH(AE$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15</f>
@@ -27913,44 +27844,44 @@
       </c>
     </row>
     <row r="141" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B141" s="72" t="s">
+      <c r="B141" s="69" t="s">
         <v>102</v>
       </c>
-      <c r="C141" s="72"/>
-      <c r="D141" s="72"/>
-      <c r="E141" s="72"/>
-      <c r="F141" s="72"/>
-      <c r="G141" s="72"/>
-      <c r="H141" s="72"/>
-      <c r="I141" s="72"/>
-      <c r="J141" s="72"/>
-      <c r="K141" s="72"/>
-      <c r="L141" s="72"/>
-      <c r="M141" s="72"/>
-      <c r="N141" s="72"/>
-      <c r="O141" s="72"/>
-      <c r="P141" s="72"/>
-      <c r="Q141" s="72"/>
-      <c r="R141" s="72"/>
-      <c r="S141" s="72"/>
-      <c r="T141" s="72"/>
-      <c r="U141" s="72"/>
-      <c r="V141" s="72"/>
-      <c r="W141" s="72"/>
-      <c r="X141" s="72"/>
-      <c r="Y141" s="72"/>
-      <c r="Z141" s="72"/>
-      <c r="AA141" s="72"/>
-      <c r="AB141" s="72"/>
-      <c r="AC141" s="72"/>
-      <c r="AD141" s="72"/>
-      <c r="AE141" s="72"/>
-      <c r="AF141" s="72"/>
-      <c r="AG141" s="72"/>
-      <c r="AH141" s="72"/>
-      <c r="AI141" s="72"/>
-      <c r="AJ141" s="72"/>
-      <c r="AK141" s="72"/>
+      <c r="C141" s="69"/>
+      <c r="D141" s="69"/>
+      <c r="E141" s="69"/>
+      <c r="F141" s="69"/>
+      <c r="G141" s="69"/>
+      <c r="H141" s="69"/>
+      <c r="I141" s="69"/>
+      <c r="J141" s="69"/>
+      <c r="K141" s="69"/>
+      <c r="L141" s="69"/>
+      <c r="M141" s="69"/>
+      <c r="N141" s="69"/>
+      <c r="O141" s="69"/>
+      <c r="P141" s="69"/>
+      <c r="Q141" s="69"/>
+      <c r="R141" s="69"/>
+      <c r="S141" s="69"/>
+      <c r="T141" s="69"/>
+      <c r="U141" s="69"/>
+      <c r="V141" s="69"/>
+      <c r="W141" s="69"/>
+      <c r="X141" s="69"/>
+      <c r="Y141" s="69"/>
+      <c r="Z141" s="69"/>
+      <c r="AA141" s="69"/>
+      <c r="AB141" s="69"/>
+      <c r="AC141" s="69"/>
+      <c r="AD141" s="69"/>
+      <c r="AE141" s="69"/>
+      <c r="AF141" s="69"/>
+      <c r="AG141" s="69"/>
+      <c r="AH141" s="69"/>
+      <c r="AI141" s="69"/>
+      <c r="AJ141" s="69"/>
+      <c r="AK141" s="69"/>
     </row>
     <row r="142" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B142" s="44" t="s">
@@ -28071,14 +28002,14 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AK46"/>
+  <dimension ref="A1:AK11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M41" sqref="M41"/>
       <selection pane="topRight" activeCell="M41" sqref="M41"/>
       <selection pane="bottomLeft" activeCell="M41" sqref="M41"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10:AI10"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28206,7 +28137,7 @@
       </c>
       <c r="C2" s="9">
         <f>SUM(INDEX('AEO Table 5'!$C$38:$AJ$40,0,MATCH(C$1,'AEO Table 5'!$C$1:$AK$1,0)))*10^15</f>
-        <v>2249710000000000.3</v>
+        <v>2249710000000000.2</v>
       </c>
       <c r="D2" s="9">
         <f>SUM(INDEX('AEO Table 5'!$C$38:$AJ$40,0,MATCH(D$1,'AEO Table 5'!$C$1:$AK$1,0)))*10^15</f>
@@ -29218,7 +29149,7 @@
       </c>
       <c r="H10">
         <f>(1-About!$C50)*INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(H$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15-SUM('BCEU-commercial-heating'!H10,'BCEU-commercial-appl'!H10)</f>
-        <v>189455859771331.88</v>
+        <v>189455859771331.87</v>
       </c>
       <c r="I10">
         <f>(1-About!$C50)*INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(I$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15-SUM('BCEU-commercial-heating'!I10,'BCEU-commercial-appl'!I10)</f>
@@ -29234,11 +29165,11 @@
       </c>
       <c r="L10">
         <f>(1-About!$C50)*INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(L$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15-SUM('BCEU-commercial-heating'!L10,'BCEU-commercial-appl'!L10)</f>
-        <v>192987382780569.38</v>
+        <v>192987382780569.37</v>
       </c>
       <c r="M10">
         <f>(1-About!$C50)*INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(M$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15-SUM('BCEU-commercial-heating'!M10,'BCEU-commercial-appl'!M10)</f>
-        <v>195156767282935.63</v>
+        <v>195156767282935.62</v>
       </c>
       <c r="N10">
         <f>(1-About!$C50)*INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(N$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15-SUM('BCEU-commercial-heating'!N10,'BCEU-commercial-appl'!N10)</f>
@@ -29254,7 +29185,7 @@
       </c>
       <c r="Q10">
         <f>(1-About!$C50)*INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(Q$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15-SUM('BCEU-commercial-heating'!Q10,'BCEU-commercial-appl'!Q10)</f>
-        <v>203070732440389.13</v>
+        <v>203070732440389.12</v>
       </c>
       <c r="R10">
         <f>(1-About!$C50)*INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(R$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15-SUM('BCEU-commercial-heating'!R10,'BCEU-commercial-appl'!R10)</f>
@@ -29274,11 +29205,11 @@
       </c>
       <c r="V10">
         <f>(1-About!$C50)*INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(V$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15-SUM('BCEU-commercial-heating'!V10,'BCEU-commercial-appl'!V10)</f>
-        <v>215467900274182.63</v>
+        <v>215467900274182.62</v>
       </c>
       <c r="W10">
         <f>(1-About!$C50)*INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(W$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15-SUM('BCEU-commercial-heating'!W10,'BCEU-commercial-appl'!W10)</f>
-        <v>218101537333770.63</v>
+        <v>218101537333770.62</v>
       </c>
       <c r="X10">
         <f>(1-About!$C50)*INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(X$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15-SUM('BCEU-commercial-heating'!X10,'BCEU-commercial-appl'!X10)</f>
@@ -29286,7 +29217,7 @@
       </c>
       <c r="Y10">
         <f>(1-About!$C50)*INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(Y$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15-SUM('BCEU-commercial-heating'!Y10,'BCEU-commercial-appl'!Y10)</f>
-        <v>223384935070649.38</v>
+        <v>223384935070649.37</v>
       </c>
       <c r="Z10">
         <f>(1-About!$C50)*INDEX('AEO Table 5'!$C$58:$AK$58,MATCH(Z$1,'AEO Table 5'!$C$1:$AK$1,0))*10^15-SUM('BCEU-commercial-heating'!Z10,'BCEU-commercial-appl'!Z10)</f>
@@ -29436,7 +29367,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -38506,44 +38436,44 @@
     </row>
     <row r="117" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="118" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B118" s="72" t="s">
+      <c r="B118" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="C118" s="72"/>
-      <c r="D118" s="72"/>
-      <c r="E118" s="72"/>
-      <c r="F118" s="72"/>
-      <c r="G118" s="72"/>
-      <c r="H118" s="72"/>
-      <c r="I118" s="72"/>
-      <c r="J118" s="72"/>
-      <c r="K118" s="72"/>
-      <c r="L118" s="72"/>
-      <c r="M118" s="72"/>
-      <c r="N118" s="72"/>
-      <c r="O118" s="72"/>
-      <c r="P118" s="72"/>
-      <c r="Q118" s="72"/>
-      <c r="R118" s="72"/>
-      <c r="S118" s="72"/>
-      <c r="T118" s="72"/>
-      <c r="U118" s="72"/>
-      <c r="V118" s="72"/>
-      <c r="W118" s="72"/>
-      <c r="X118" s="72"/>
-      <c r="Y118" s="72"/>
-      <c r="Z118" s="72"/>
-      <c r="AA118" s="72"/>
-      <c r="AB118" s="72"/>
-      <c r="AC118" s="72"/>
-      <c r="AD118" s="72"/>
-      <c r="AE118" s="72"/>
-      <c r="AF118" s="72"/>
-      <c r="AG118" s="72"/>
-      <c r="AH118" s="72"/>
-      <c r="AI118" s="72"/>
-      <c r="AJ118" s="72"/>
-      <c r="AK118" s="72"/>
+      <c r="C118" s="69"/>
+      <c r="D118" s="69"/>
+      <c r="E118" s="69"/>
+      <c r="F118" s="69"/>
+      <c r="G118" s="69"/>
+      <c r="H118" s="69"/>
+      <c r="I118" s="69"/>
+      <c r="J118" s="69"/>
+      <c r="K118" s="69"/>
+      <c r="L118" s="69"/>
+      <c r="M118" s="69"/>
+      <c r="N118" s="69"/>
+      <c r="O118" s="69"/>
+      <c r="P118" s="69"/>
+      <c r="Q118" s="69"/>
+      <c r="R118" s="69"/>
+      <c r="S118" s="69"/>
+      <c r="T118" s="69"/>
+      <c r="U118" s="69"/>
+      <c r="V118" s="69"/>
+      <c r="W118" s="69"/>
+      <c r="X118" s="69"/>
+      <c r="Y118" s="69"/>
+      <c r="Z118" s="69"/>
+      <c r="AA118" s="69"/>
+      <c r="AB118" s="69"/>
+      <c r="AC118" s="69"/>
+      <c r="AD118" s="69"/>
+      <c r="AE118" s="69"/>
+      <c r="AF118" s="69"/>
+      <c r="AG118" s="69"/>
+      <c r="AH118" s="69"/>
+      <c r="AI118" s="69"/>
+      <c r="AJ118" s="69"/>
+      <c r="AK118" s="69"/>
     </row>
     <row r="119" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="44" t="s">
@@ -38831,7 +38761,7 @@
       </c>
       <c r="C9" s="9">
         <f>$B$3*('AEO Table 5'!D61/'AEO Table 5'!$C61)</f>
-        <v>375086476892834.88</v>
+        <v>375086476892834.87</v>
       </c>
       <c r="D9" s="9">
         <f>$B$3*('AEO Table 5'!E61/'AEO Table 5'!$C61)</f>
@@ -38875,7 +38805,7 @@
       </c>
       <c r="N9" s="9">
         <f>$B$3*('AEO Table 5'!O61/'AEO Table 5'!$C61)</f>
-        <v>335953845875489.13</v>
+        <v>335953845875489.12</v>
       </c>
       <c r="O9" s="9">
         <f>$B$3*('AEO Table 5'!P61/'AEO Table 5'!$C61)</f>
@@ -38899,7 +38829,7 @@
       </c>
       <c r="T9" s="9">
         <f>$B$3*('AEO Table 5'!U61/'AEO Table 5'!$C61)</f>
-        <v>326534871984644.38</v>
+        <v>326534871984644.37</v>
       </c>
       <c r="U9" s="9">
         <f>$B$3*('AEO Table 5'!V61/'AEO Table 5'!$C61)</f>
@@ -39117,37 +39047,37 @@
       <c r="G1"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="70" t="s">
         <v>439</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
     </row>
     <row r="3" spans="1:7" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="46"/>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="72" t="s">
         <v>440</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="76"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="73"/>
     </row>
     <row r="4" spans="1:7" s="12" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46"/>
       <c r="B4" s="47"/>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="74" t="s">
         <v>441</v>
       </c>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
     </row>
     <row r="5" spans="1:7" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="48"/>
@@ -45608,158 +45538,158 @@
       <c r="G303" s="13"/>
     </row>
     <row r="304" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A304" s="78" t="s">
+      <c r="A304" s="75" t="s">
         <v>241</v>
       </c>
-      <c r="B304" s="78"/>
-      <c r="C304" s="78"/>
-      <c r="D304" s="78"/>
-      <c r="E304" s="78"/>
-      <c r="F304" s="78"/>
-      <c r="G304" s="78"/>
+      <c r="B304" s="75"/>
+      <c r="C304" s="75"/>
+      <c r="D304" s="75"/>
+      <c r="E304" s="75"/>
+      <c r="F304" s="75"/>
+      <c r="G304" s="75"/>
       <c r="H304" s="28"/>
       <c r="I304" s="28"/>
     </row>
     <row r="305" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A305" s="78"/>
-      <c r="B305" s="78"/>
-      <c r="C305" s="78"/>
-      <c r="D305" s="78"/>
-      <c r="E305" s="78"/>
-      <c r="F305" s="78"/>
-      <c r="G305" s="78"/>
+      <c r="A305" s="75"/>
+      <c r="B305" s="75"/>
+      <c r="C305" s="75"/>
+      <c r="D305" s="75"/>
+      <c r="E305" s="75"/>
+      <c r="F305" s="75"/>
+      <c r="G305" s="75"/>
       <c r="H305" s="28"/>
       <c r="I305" s="28"/>
     </row>
     <row r="306" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A306" s="78"/>
-      <c r="B306" s="78"/>
-      <c r="C306" s="78"/>
-      <c r="D306" s="78"/>
-      <c r="E306" s="78"/>
-      <c r="F306" s="78"/>
-      <c r="G306" s="78"/>
+      <c r="A306" s="75"/>
+      <c r="B306" s="75"/>
+      <c r="C306" s="75"/>
+      <c r="D306" s="75"/>
+      <c r="E306" s="75"/>
+      <c r="F306" s="75"/>
+      <c r="G306" s="75"/>
       <c r="H306" s="28"/>
       <c r="I306" s="28"/>
     </row>
     <row r="307" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A307" s="78"/>
-      <c r="B307" s="78"/>
-      <c r="C307" s="78"/>
-      <c r="D307" s="78"/>
-      <c r="E307" s="78"/>
-      <c r="F307" s="78"/>
-      <c r="G307" s="78"/>
+      <c r="A307" s="75"/>
+      <c r="B307" s="75"/>
+      <c r="C307" s="75"/>
+      <c r="D307" s="75"/>
+      <c r="E307" s="75"/>
+      <c r="F307" s="75"/>
+      <c r="G307" s="75"/>
       <c r="H307" s="28"/>
       <c r="I307" s="28"/>
     </row>
     <row r="308" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A308" s="78"/>
-      <c r="B308" s="78"/>
-      <c r="C308" s="78"/>
-      <c r="D308" s="78"/>
-      <c r="E308" s="78"/>
-      <c r="F308" s="78"/>
-      <c r="G308" s="78"/>
+      <c r="A308" s="75"/>
+      <c r="B308" s="75"/>
+      <c r="C308" s="75"/>
+      <c r="D308" s="75"/>
+      <c r="E308" s="75"/>
+      <c r="F308" s="75"/>
+      <c r="G308" s="75"/>
       <c r="H308" s="28"/>
       <c r="I308" s="28"/>
     </row>
     <row r="309" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A309" s="78"/>
-      <c r="B309" s="78"/>
-      <c r="C309" s="78"/>
-      <c r="D309" s="78"/>
-      <c r="E309" s="78"/>
-      <c r="F309" s="78"/>
-      <c r="G309" s="78"/>
+      <c r="A309" s="75"/>
+      <c r="B309" s="75"/>
+      <c r="C309" s="75"/>
+      <c r="D309" s="75"/>
+      <c r="E309" s="75"/>
+      <c r="F309" s="75"/>
+      <c r="G309" s="75"/>
       <c r="H309" s="28"/>
       <c r="I309" s="28"/>
     </row>
     <row r="310" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A310" s="78"/>
-      <c r="B310" s="78"/>
-      <c r="C310" s="78"/>
-      <c r="D310" s="78"/>
-      <c r="E310" s="78"/>
-      <c r="F310" s="78"/>
-      <c r="G310" s="78"/>
+      <c r="A310" s="75"/>
+      <c r="B310" s="75"/>
+      <c r="C310" s="75"/>
+      <c r="D310" s="75"/>
+      <c r="E310" s="75"/>
+      <c r="F310" s="75"/>
+      <c r="G310" s="75"/>
       <c r="H310" s="28"/>
       <c r="I310" s="28"/>
     </row>
     <row r="311" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A311" s="78"/>
-      <c r="B311" s="78"/>
-      <c r="C311" s="78"/>
-      <c r="D311" s="78"/>
-      <c r="E311" s="78"/>
-      <c r="F311" s="78"/>
-      <c r="G311" s="78"/>
+      <c r="A311" s="75"/>
+      <c r="B311" s="75"/>
+      <c r="C311" s="75"/>
+      <c r="D311" s="75"/>
+      <c r="E311" s="75"/>
+      <c r="F311" s="75"/>
+      <c r="G311" s="75"/>
       <c r="H311" s="28"/>
       <c r="I311" s="28"/>
     </row>
     <row r="312" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A312" s="78"/>
-      <c r="B312" s="78"/>
-      <c r="C312" s="78"/>
-      <c r="D312" s="78"/>
-      <c r="E312" s="78"/>
-      <c r="F312" s="78"/>
-      <c r="G312" s="78"/>
+      <c r="A312" s="75"/>
+      <c r="B312" s="75"/>
+      <c r="C312" s="75"/>
+      <c r="D312" s="75"/>
+      <c r="E312" s="75"/>
+      <c r="F312" s="75"/>
+      <c r="G312" s="75"/>
       <c r="H312" s="28"/>
       <c r="I312" s="28"/>
     </row>
     <row r="313" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A313" s="78"/>
-      <c r="B313" s="78"/>
-      <c r="C313" s="78"/>
-      <c r="D313" s="78"/>
-      <c r="E313" s="78"/>
-      <c r="F313" s="78"/>
-      <c r="G313" s="78"/>
+      <c r="A313" s="75"/>
+      <c r="B313" s="75"/>
+      <c r="C313" s="75"/>
+      <c r="D313" s="75"/>
+      <c r="E313" s="75"/>
+      <c r="F313" s="75"/>
+      <c r="G313" s="75"/>
       <c r="H313" s="28"/>
       <c r="I313" s="28"/>
     </row>
     <row r="314" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A314" s="78"/>
-      <c r="B314" s="78"/>
-      <c r="C314" s="78"/>
-      <c r="D314" s="78"/>
-      <c r="E314" s="78"/>
-      <c r="F314" s="78"/>
-      <c r="G314" s="78"/>
+      <c r="A314" s="75"/>
+      <c r="B314" s="75"/>
+      <c r="C314" s="75"/>
+      <c r="D314" s="75"/>
+      <c r="E314" s="75"/>
+      <c r="F314" s="75"/>
+      <c r="G314" s="75"/>
       <c r="H314" s="28"/>
       <c r="I314" s="28"/>
     </row>
     <row r="315" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A315" s="78"/>
-      <c r="B315" s="78"/>
-      <c r="C315" s="78"/>
-      <c r="D315" s="78"/>
-      <c r="E315" s="78"/>
-      <c r="F315" s="78"/>
-      <c r="G315" s="78"/>
+      <c r="A315" s="75"/>
+      <c r="B315" s="75"/>
+      <c r="C315" s="75"/>
+      <c r="D315" s="75"/>
+      <c r="E315" s="75"/>
+      <c r="F315" s="75"/>
+      <c r="G315" s="75"/>
       <c r="H315" s="28"/>
       <c r="I315" s="28"/>
     </row>
     <row r="316" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A316" s="78"/>
-      <c r="B316" s="78"/>
-      <c r="C316" s="78"/>
-      <c r="D316" s="78"/>
-      <c r="E316" s="78"/>
-      <c r="F316" s="78"/>
-      <c r="G316" s="78"/>
+      <c r="A316" s="75"/>
+      <c r="B316" s="75"/>
+      <c r="C316" s="75"/>
+      <c r="D316" s="75"/>
+      <c r="E316" s="75"/>
+      <c r="F316" s="75"/>
+      <c r="G316" s="75"/>
       <c r="H316" s="28"/>
       <c r="I316" s="28"/>
     </row>
     <row r="317" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A317" s="78"/>
-      <c r="B317" s="78"/>
-      <c r="C317" s="78"/>
-      <c r="D317" s="78"/>
-      <c r="E317" s="78"/>
-      <c r="F317" s="78"/>
-      <c r="G317" s="78"/>
+      <c r="A317" s="75"/>
+      <c r="B317" s="75"/>
+      <c r="C317" s="75"/>
+      <c r="D317" s="75"/>
+      <c r="E317" s="75"/>
+      <c r="F317" s="75"/>
+      <c r="G317" s="75"/>
       <c r="H317" s="28"/>
       <c r="I317" s="28"/>
     </row>
@@ -45998,7 +45928,7 @@
       </c>
       <c r="O2" s="9">
         <f>INDEX('AEO Table 4'!$C$34:$AK$34,MATCH(O$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>461045587986463.63</v>
+        <v>461045587986463.62</v>
       </c>
       <c r="P2" s="9">
         <f>INDEX('AEO Table 4'!$C$34:$AK$34,MATCH(P$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -46014,7 +45944,7 @@
       </c>
       <c r="S2" s="9">
         <f>INDEX('AEO Table 4'!$C$34:$AK$34,MATCH(S$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>439798176818950.88</v>
+        <v>439798176818950.87</v>
       </c>
       <c r="T2" s="9">
         <f>INDEX('AEO Table 4'!$C$34:$AK$34,MATCH(T$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -46042,7 +45972,7 @@
       </c>
       <c r="Z2" s="9">
         <f>INDEX('AEO Table 4'!$C$34:$AK$34,MATCH(Z$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>406870297800338.38</v>
+        <v>406870297800338.37</v>
       </c>
       <c r="AA2" s="9">
         <f>INDEX('AEO Table 4'!$C$34:$AK$34,MATCH(AA$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -46070,7 +46000,7 @@
       </c>
       <c r="AG2" s="9">
         <f>INDEX('AEO Table 4'!$C$34:$AK$34,MATCH(AG$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>377079857021996.63</v>
+        <v>377079857021996.62</v>
       </c>
       <c r="AH2" s="9">
         <f>INDEX('AEO Table 4'!$C$34:$AK$34,MATCH(AH$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -46336,11 +46266,11 @@
       </c>
       <c r="B5" s="9">
         <f>INDEX('AEO Table 4'!$C$60:$AK$60,MATCH(B$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>320735760575296.13</v>
+        <v>320735760575296.12</v>
       </c>
       <c r="C5" s="9">
         <f>INDEX('AEO Table 4'!$C$60:$AK$60,MATCH(C$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>332862488155668.38</v>
+        <v>332862488155668.37</v>
       </c>
       <c r="D5" s="9">
         <f>INDEX('AEO Table 4'!$C$60:$AK$60,MATCH(D$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -46360,15 +46290,15 @@
       </c>
       <c r="H5" s="9">
         <f>INDEX('AEO Table 4'!$C$60:$AK$60,MATCH(H$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>274166915397631.13</v>
+        <v>274166915397631.12</v>
       </c>
       <c r="I5" s="9">
         <f>INDEX('AEO Table 4'!$C$60:$AK$60,MATCH(I$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>266539639593908.63</v>
+        <v>266539639593908.62</v>
       </c>
       <c r="J5" s="9">
         <f>INDEX('AEO Table 4'!$C$60:$AK$60,MATCH(J$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>259173549915397.63</v>
+        <v>259173549915397.62</v>
       </c>
       <c r="K5" s="9">
         <f>INDEX('AEO Table 4'!$C$60:$AK$60,MATCH(K$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -46444,7 +46374,7 @@
       </c>
       <c r="AC5" s="9">
         <f>INDEX('AEO Table 4'!$C$60:$AK$60,MATCH(AC$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>167634222504230.13</v>
+        <v>167634222504230.12</v>
       </c>
       <c r="AD5" s="9">
         <f>INDEX('AEO Table 4'!$C$60:$AK$60,MATCH(AD$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -46632,15 +46562,15 @@
       </c>
       <c r="N7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(N$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>331493263959390.88</v>
+        <v>331493263959390.87</v>
       </c>
       <c r="O7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(O$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>329074488155668.38</v>
+        <v>329074488155668.37</v>
       </c>
       <c r="P7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(P$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>326433784263959.38</v>
+        <v>326433784263959.37</v>
       </c>
       <c r="Q7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(Q$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -46648,7 +46578,7 @@
       </c>
       <c r="R7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(R$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>321447212351945.88</v>
+        <v>321447212351945.87</v>
       </c>
       <c r="S7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(S$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -46656,11 +46586,11 @@
       </c>
       <c r="T7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(T$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>315391860406091.38</v>
+        <v>315391860406091.37</v>
       </c>
       <c r="U7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(U$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>312924212351945.88</v>
+        <v>312924212351945.87</v>
       </c>
       <c r="V7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(V$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -46668,7 +46598,7 @@
       </c>
       <c r="W7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(W$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>306505122673434.88</v>
+        <v>306505122673434.87</v>
       </c>
       <c r="X7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(X$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -46676,11 +46606,11 @@
       </c>
       <c r="Y7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(Y$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>300806297800338.38</v>
+        <v>300806297800338.37</v>
       </c>
       <c r="Z7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(Z$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>297944467005076.13</v>
+        <v>297944467005076.12</v>
       </c>
       <c r="AA7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(AA$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -46708,7 +46638,7 @@
       </c>
       <c r="AG7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(AG$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>278953191201353.63</v>
+        <v>278953191201353.62</v>
       </c>
       <c r="AH7" s="9">
         <f>INDEX('AEO Table 4'!$C$72:$AK$72,MATCH(AH$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -46975,7 +46905,7 @@
       </c>
       <c r="K10" s="9">
         <f>INDEX('AEO Table 4'!$C$66:$AK$66,MATCH(K$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>219425187817258.88</v>
+        <v>219425187817258.87</v>
       </c>
       <c r="L10" s="9">
         <f>INDEX('AEO Table 4'!$C$66:$AK$66,MATCH(L$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -46987,7 +46917,7 @@
       </c>
       <c r="N10" s="9">
         <f>INDEX('AEO Table 4'!$C$66:$AK$66,MATCH(N$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>208987357021996.63</v>
+        <v>208987357021996.62</v>
       </c>
       <c r="O10" s="9">
         <f>INDEX('AEO Table 4'!$C$66:$AK$66,MATCH(O$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -46999,7 +46929,7 @@
       </c>
       <c r="Q10" s="9">
         <f>INDEX('AEO Table 4'!$C$66:$AK$66,MATCH(Q$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>200933049915397.63</v>
+        <v>200933049915397.62</v>
       </c>
       <c r="R10" s="9">
         <f>INDEX('AEO Table 4'!$C$66:$AK$66,MATCH(R$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -47063,7 +46993,7 @@
       </c>
       <c r="AG10" s="9">
         <f>INDEX('AEO Table 4'!$C$66:$AK$66,MATCH(AG$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>172182546531302.88</v>
+        <v>172182546531302.87</v>
       </c>
       <c r="AH10" s="9">
         <f>INDEX('AEO Table 4'!$C$66:$AK$66,MATCH(AH$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -47339,7 +47269,7 @@
       </c>
       <c r="F2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(F$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(F$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>611319746192893.38</v>
+        <v>611319746192893.37</v>
       </c>
       <c r="G2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(G$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(G$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -47351,23 +47281,23 @@
       </c>
       <c r="I2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(I$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(I$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>628715863790186.13</v>
+        <v>628715863790186.12</v>
       </c>
       <c r="J2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(J$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(J$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>632233864636209.88</v>
+        <v>632233864636209.87</v>
       </c>
       <c r="K2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(K$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(K$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>636105187817258.88</v>
+        <v>636105187817258.87</v>
       </c>
       <c r="L2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(L$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(L$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>640952353637901.88</v>
+        <v>640952353637901.87</v>
       </c>
       <c r="M2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(M$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(M$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>646444472927241.88</v>
+        <v>646444472927241.87</v>
       </c>
       <c r="N2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(N$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(N$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -47375,11 +47305,11 @@
       </c>
       <c r="O2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(O$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(O$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>659052712351945.88</v>
+        <v>659052712351945.87</v>
       </c>
       <c r="P2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(P$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(P$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>665825925549915.38</v>
+        <v>665825925549915.37</v>
       </c>
       <c r="Q2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(Q$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(Q$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -47399,7 +47329,7 @@
       </c>
       <c r="U2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(U$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(U$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>700417864636209.88</v>
+        <v>700417864636209.87</v>
       </c>
       <c r="V2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(V$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(V$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -47435,7 +47365,7 @@
       </c>
       <c r="AD2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(AD$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(AD$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>773671759729272.38</v>
+        <v>773671759729272.37</v>
       </c>
       <c r="AE2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(AE$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(AE$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -47447,15 +47377,15 @@
       </c>
       <c r="AG2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(AG$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(AG$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>798634263113367.13</v>
+        <v>798634263113367.12</v>
       </c>
       <c r="AH2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(AH$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(AH$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>806767887478849.38</v>
+        <v>806767887478849.37</v>
       </c>
       <c r="AI2" s="9">
         <f>INDEX('AEO Table 4'!$C$35:$AK$35,MATCH(AI$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68+INDEX('AEO Table 4'!$C$46:$AK$46,MATCH(AI$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>815796434856175.88</v>
+        <v>815796434856175.87</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -47579,7 +47509,7 @@
       </c>
       <c r="D4" s="9">
         <f>INDEX('AEO Table 4'!$C$52:$AK$52,MATCH(D$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>41725685279187.813</v>
+        <v>41725685279187.812</v>
       </c>
       <c r="E4" s="9">
         <f>INDEX('AEO Table 4'!$C$52:$AK$52,MATCH(E$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -47599,7 +47529,7 @@
       </c>
       <c r="I4" s="9">
         <f>INDEX('AEO Table 4'!$C$52:$AK$52,MATCH(I$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>44858316412859.563</v>
+        <v>44858316412859.562</v>
       </c>
       <c r="J4" s="9">
         <f>INDEX('AEO Table 4'!$C$52:$AK$52,MATCH(J$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -47651,7 +47581,7 @@
       </c>
       <c r="V4" s="9">
         <f>INDEX('AEO Table 4'!$C$52:$AK$52,MATCH(V$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>41620730118443.313</v>
+        <v>41620730118443.312</v>
       </c>
       <c r="W4" s="9">
         <f>INDEX('AEO Table 4'!$C$52:$AK$52,MATCH(W$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -47699,7 +47629,7 @@
       </c>
       <c r="AH4" s="9">
         <f>INDEX('AEO Table 4'!$C$52:$AK$52,MATCH(AH$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>41595092216582.063</v>
+        <v>41595092216582.062</v>
       </c>
       <c r="AI4" s="9">
         <f>INDEX('AEO Table 4'!$C$52:$AK$52,MATCH(AI$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -48605,7 +48535,7 @@
       </c>
       <c r="D2" s="9">
         <f>INDEX('AEO Table 4'!$C$41:$AK$41,MATCH(D$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>235237363790186.13</v>
+        <v>235237363790186.12</v>
       </c>
       <c r="E2" s="9">
         <f>INDEX('AEO Table 4'!$C$41:$AK$41,MATCH(E$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -48633,7 +48563,7 @@
       </c>
       <c r="K2" s="9">
         <f>INDEX('AEO Table 4'!$C$41:$AK$41,MATCH(K$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>152636049915397.63</v>
+        <v>152636049915397.62</v>
       </c>
       <c r="L2" s="9">
         <f>INDEX('AEO Table 4'!$C$41:$AK$41,MATCH(L$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -48653,7 +48583,7 @@
       </c>
       <c r="P2" s="9">
         <f>INDEX('AEO Table 4'!$C$41:$AK$41,MATCH(P$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>152605604906937.38</v>
+        <v>152605604906937.37</v>
       </c>
       <c r="Q2" s="9">
         <f>INDEX('AEO Table 4'!$C$41:$AK$41,MATCH(Q$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -49840,7 +49770,7 @@
       </c>
       <c r="B2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(B$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(B$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>1018004169204737.8</v>
+        <v>1018004169204737.7</v>
       </c>
       <c r="C2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(C$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(C$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
@@ -49868,19 +49798,19 @@
       </c>
       <c r="I2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(I$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(I$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>1038569772419627.8</v>
+        <v>1038569772419627.7</v>
       </c>
       <c r="J2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(J$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(J$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>1037396838409475.3</v>
+        <v>1037396838409475.2</v>
       </c>
       <c r="K2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(K$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(K$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>1035782451776649.8</v>
+        <v>1035782451776649.7</v>
       </c>
       <c r="L2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(L$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(L$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>1034809813874788.8</v>
+        <v>1034809813874788.7</v>
       </c>
       <c r="M2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(M$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(M$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
@@ -49888,15 +49818,15 @@
       </c>
       <c r="N2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(N$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(N$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>1034885926395939.3</v>
+        <v>1034885926395939.2</v>
       </c>
       <c r="O2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(O$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(O$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>1035758416243654.8</v>
+        <v>1035758416243654.7</v>
       </c>
       <c r="P2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(P$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(P$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>1037298292724196.3</v>
+        <v>1037298292724196.2</v>
       </c>
       <c r="Q2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(Q$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(Q$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
@@ -49904,11 +49834,11 @@
       </c>
       <c r="R2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(R$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(R$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>1041297805414551.8</v>
+        <v>1041297805414551.7</v>
       </c>
       <c r="S2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(S$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(S$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>1044559427241962.8</v>
+        <v>1044559427241962.7</v>
       </c>
       <c r="T2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(T$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(T$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
@@ -49928,7 +49858,7 @@
       </c>
       <c r="X2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(X$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(X$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>1068946680203045.8</v>
+        <v>1068946680203045.7</v>
       </c>
       <c r="Y2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(Y$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(Y$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
@@ -49956,15 +49886,15 @@
       </c>
       <c r="AE2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(AE$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(AE$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>1113470902707275.8</v>
+        <v>1113470902707275.7</v>
       </c>
       <c r="AF2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(AF$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(AF$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>1120082276649746.3</v>
+        <v>1120082276649746.2</v>
       </c>
       <c r="AG2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(AG$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(AG$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>1126663205583756.3</v>
+        <v>1126663205583756.2</v>
       </c>
       <c r="AH2" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$36:$AJ$40,0,MATCH(AH$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68+SUM(INDEX('AEO Table 4'!$C$42:$AJ$43,0,MATCH(AH$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
@@ -50092,7 +50022,7 @@
       </c>
       <c r="C4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(C$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>910909846023688.63</v>
+        <v>910909846023688.62</v>
       </c>
       <c r="D4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(D$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
@@ -50100,7 +50030,7 @@
       </c>
       <c r="E4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(E$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>908871632825719.13</v>
+        <v>908871632825719.12</v>
       </c>
       <c r="F4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(F$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
@@ -50112,15 +50042,15 @@
       </c>
       <c r="H4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(H$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>909872312182741.13</v>
+        <v>909872312182741.12</v>
       </c>
       <c r="I4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(I$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>911733463620981.38</v>
+        <v>911733463620981.37</v>
       </c>
       <c r="J4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(J$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>914570457698815.38</v>
+        <v>914570457698815.37</v>
       </c>
       <c r="K4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(K$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
@@ -50128,11 +50058,11 @@
       </c>
       <c r="L4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(L$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>924597280879864.63</v>
+        <v>924597280879864.62</v>
       </c>
       <c r="M4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(M$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>931447407783418.13</v>
+        <v>931447407783418.12</v>
       </c>
       <c r="N4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(N$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
@@ -50140,11 +50070,11 @@
       </c>
       <c r="O4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(O$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>945031489847715.88</v>
+        <v>945031489847715.87</v>
       </c>
       <c r="P4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(P$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>953186746192893.38</v>
+        <v>953186746192893.37</v>
       </c>
       <c r="Q4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(Q$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
@@ -50152,7 +50082,7 @@
       </c>
       <c r="R4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(R$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>969173580372250.38</v>
+        <v>969173580372250.37</v>
       </c>
       <c r="S4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(S$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
@@ -50160,7 +50090,7 @@
       </c>
       <c r="T4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(T$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>985431214890017.13</v>
+        <v>985431214890017.12</v>
       </c>
       <c r="U4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(U$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
@@ -50176,15 +50106,15 @@
       </c>
       <c r="X4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(X$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>1015195216582064.3</v>
+        <v>1015195216582064.2</v>
       </c>
       <c r="Y4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(Y$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>1022201574450084.8</v>
+        <v>1022201574450084.7</v>
       </c>
       <c r="Z4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(Z$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>1029304875634517.8</v>
+        <v>1029304875634517.7</v>
       </c>
       <c r="AA4" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$53:$AJ$55,0,MATCH(AA$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
@@ -50277,7 +50207,7 @@
       </c>
       <c r="N5" s="9">
         <f>INDEX('AEO Table 4'!$C$61:$AJ$61,MATCH(N$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>25969592216582.063</v>
+        <v>25969592216582.062</v>
       </c>
       <c r="O5" s="9">
         <f>INDEX('AEO Table 4'!$C$61:$AJ$61,MATCH(O$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -50305,11 +50235,11 @@
       </c>
       <c r="U5" s="9">
         <f>INDEX('AEO Table 4'!$C$61:$AJ$61,MATCH(U$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>22813726734348.563</v>
+        <v>22813726734348.562</v>
       </c>
       <c r="V5" s="9">
         <f>INDEX('AEO Table 4'!$C$61:$AJ$61,MATCH(V$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>22353045685279.188</v>
+        <v>22353045685279.187</v>
       </c>
       <c r="W5" s="9">
         <f>INDEX('AEO Table 4'!$C$61:$AJ$61,MATCH(W$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -50333,7 +50263,7 @@
       </c>
       <c r="AB5" s="9">
         <f>INDEX('AEO Table 4'!$C$61:$AJ$61,MATCH(AB$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
-        <v>19801273265651.438</v>
+        <v>19801273265651.437</v>
       </c>
       <c r="AC5" s="9">
         <f>INDEX('AEO Table 4'!$C$61:$AJ$61,MATCH(AC$1,'AEO Table 4'!$C$1:$AK$1,0))*10^15*About!$A$68</f>
@@ -50810,7 +50740,7 @@
       </c>
       <c r="E10" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$67:$AJ$68,0,MATCH(E$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>61034230118443.313</v>
+        <v>61034230118443.312</v>
       </c>
       <c r="F10" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$67:$AJ$68,0,MATCH(F$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
@@ -50886,7 +50816,7 @@
       </c>
       <c r="X10" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$67:$AJ$68,0,MATCH(X$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>
-        <v>36547630287648.063</v>
+        <v>36547630287648.062</v>
       </c>
       <c r="Y10" s="9">
         <f>SUM(INDEX('AEO Table 4'!$C$67:$AJ$68,0,MATCH(Y$1,'AEO Table 4'!$C$1:$AK$1,0)))*10^15*About!$A$68</f>

</xml_diff>

<commit_message>
Revert "AEO 2020 update"
This reverts commit 4a215b59cca46e5d6cb5d520de174a22f7c7f0f7.
</commit_message>
<xml_diff>
--- a/InputData/bldgs/BCEU/BAU Components Energy Use.xlsx
+++ b/InputData/bldgs/BCEU/BAU Components Energy Use.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\United States\Model\InputData\bldgs\BCEU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE79BA0-476A-44DB-91E5-C60E84D4EB79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B011FA31-D94A-48DD-B5AE-D997E957F583}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="14107" windowHeight="10200" firstSheet="2" activeTab="5" xr2:uid="{62DBD58C-909E-4480-AEA4-2C1D8430F11A}"/>
+    <workbookView xWindow="9172" yWindow="240" windowWidth="10021" windowHeight="9683" firstSheet="16" activeTab="16" xr2:uid="{62DBD58C-909E-4480-AEA4-2C1D8430F11A}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2604,7 +2604,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="17" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="9">
       <alignment wrapText="1"/>
     </xf>
@@ -2626,6 +2625,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -13832,7 +13832,7 @@
   </sheetPr>
   <dimension ref="A1:AI11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -14619,131 +14619,131 @@
       </c>
       <c r="B7" s="9">
         <f>Calculations!J139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="C7" s="9">
         <f>Calculations!K139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="D7" s="9">
         <f>Calculations!L139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="E7" s="9">
         <f>Calculations!M139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="F7" s="9">
         <f>Calculations!N139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="G7" s="9">
         <f>Calculations!O139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="H7" s="9">
         <f>Calculations!P139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="I7" s="9">
         <f>Calculations!Q139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="J7" s="9">
         <f>Calculations!R139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="K7" s="9">
         <f>Calculations!S139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="L7" s="9">
         <f>Calculations!T139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="M7" s="9">
         <f>Calculations!U139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="N7" s="9">
         <f>Calculations!V139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="O7" s="9">
         <f>Calculations!W139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="P7" s="9">
         <f>Calculations!X139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="9">
         <f>Calculations!Y139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="R7" s="9">
         <f>Calculations!Z139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="S7" s="9">
         <f>Calculations!AA139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="T7" s="9">
         <f>Calculations!AB139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="U7" s="9">
         <f>Calculations!AC139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="V7" s="9">
         <f>Calculations!AD139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="W7" s="9">
         <f>Calculations!AE139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="X7" s="9">
         <f>Calculations!AF139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="Y7" s="9">
         <f>Calculations!AG139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="Z7" s="9">
         <f>Calculations!AH139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="AA7" s="9">
         <f>Calculations!AI139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="AB7" s="9">
         <f>Calculations!AJ139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="AC7" s="9">
         <f>Calculations!AK139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="AD7" s="9">
         <f>Calculations!AL139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="AE7" s="9">
         <f>Calculations!AM139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="AF7" s="9">
         <f>Calculations!AN139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
       <c r="AG7" s="9">
         <f>Calculations!AO139</f>
-        <v>130720000000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.45">
@@ -29281,42 +29281,42 @@
     </row>
     <row r="140" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="141" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B141" s="79" t="s">
+      <c r="B141" s="78" t="s">
         <v>529</v>
       </c>
-      <c r="C141" s="79"/>
-      <c r="D141" s="79"/>
-      <c r="E141" s="79"/>
-      <c r="F141" s="79"/>
-      <c r="G141" s="79"/>
-      <c r="H141" s="79"/>
-      <c r="I141" s="79"/>
-      <c r="J141" s="79"/>
-      <c r="K141" s="79"/>
-      <c r="L141" s="79"/>
-      <c r="M141" s="79"/>
-      <c r="N141" s="79"/>
-      <c r="O141" s="79"/>
-      <c r="P141" s="79"/>
-      <c r="Q141" s="79"/>
-      <c r="R141" s="79"/>
-      <c r="S141" s="79"/>
-      <c r="T141" s="79"/>
-      <c r="U141" s="79"/>
-      <c r="V141" s="79"/>
-      <c r="W141" s="79"/>
-      <c r="X141" s="79"/>
-      <c r="Y141" s="79"/>
-      <c r="Z141" s="79"/>
-      <c r="AA141" s="79"/>
-      <c r="AB141" s="79"/>
-      <c r="AC141" s="79"/>
-      <c r="AD141" s="79"/>
-      <c r="AE141" s="79"/>
-      <c r="AF141" s="79"/>
-      <c r="AG141" s="79"/>
-      <c r="AH141" s="79"/>
-      <c r="AI141" s="79"/>
+      <c r="C141" s="78"/>
+      <c r="D141" s="78"/>
+      <c r="E141" s="78"/>
+      <c r="F141" s="78"/>
+      <c r="G141" s="78"/>
+      <c r="H141" s="78"/>
+      <c r="I141" s="78"/>
+      <c r="J141" s="78"/>
+      <c r="K141" s="78"/>
+      <c r="L141" s="78"/>
+      <c r="M141" s="78"/>
+      <c r="N141" s="78"/>
+      <c r="O141" s="78"/>
+      <c r="P141" s="78"/>
+      <c r="Q141" s="78"/>
+      <c r="R141" s="78"/>
+      <c r="S141" s="78"/>
+      <c r="T141" s="78"/>
+      <c r="U141" s="78"/>
+      <c r="V141" s="78"/>
+      <c r="W141" s="78"/>
+      <c r="X141" s="78"/>
+      <c r="Y141" s="78"/>
+      <c r="Z141" s="78"/>
+      <c r="AA141" s="78"/>
+      <c r="AB141" s="78"/>
+      <c r="AC141" s="78"/>
+      <c r="AD141" s="78"/>
+      <c r="AE141" s="78"/>
+      <c r="AF141" s="78"/>
+      <c r="AG141" s="78"/>
+      <c r="AH141" s="78"/>
+      <c r="AI141" s="78"/>
     </row>
     <row r="142" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B142" s="30" t="s">
@@ -32336,8 +32336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AI134"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView topLeftCell="T1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -33395,7 +33395,7 @@
       </c>
     </row>
     <row r="31" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="69" t="s">
+      <c r="A31" s="14" t="s">
         <v>537</v>
       </c>
       <c r="B31" s="57" t="s">
@@ -33502,7 +33502,7 @@
       </c>
     </row>
     <row r="32" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="69" t="s">
+      <c r="A32" s="14" t="s">
         <v>538</v>
       </c>
       <c r="B32" s="57" t="s">
@@ -33609,7 +33609,7 @@
       </c>
     </row>
     <row r="33" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="69" t="s">
+      <c r="A33" s="67" t="s">
         <v>539</v>
       </c>
       <c r="B33" s="57" t="s">
@@ -33716,7 +33716,7 @@
       </c>
     </row>
     <row r="34" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="69" t="s">
+      <c r="A34" s="14" t="s">
         <v>540</v>
       </c>
       <c r="B34" s="57" t="s">
@@ -33823,7 +33823,7 @@
       </c>
     </row>
     <row r="35" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="69" t="s">
+      <c r="A35" s="67" t="s">
         <v>541</v>
       </c>
       <c r="B35" s="57" t="s">
@@ -33930,7 +33930,7 @@
       </c>
     </row>
     <row r="36" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="69" t="s">
+      <c r="A36" s="14" t="s">
         <v>542</v>
       </c>
       <c r="B36" s="57" t="s">
@@ -34037,7 +34037,7 @@
       </c>
     </row>
     <row r="37" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="69" t="s">
+      <c r="A37" s="67" t="s">
         <v>543</v>
       </c>
       <c r="B37" s="57" t="s">
@@ -34144,7 +34144,7 @@
       </c>
     </row>
     <row r="38" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="69" t="s">
+      <c r="A38" s="14" t="s">
         <v>544</v>
       </c>
       <c r="B38" s="57" t="s">
@@ -41092,42 +41092,42 @@
     </row>
     <row r="117" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="118" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B118" s="79" t="s">
+      <c r="B118" s="78" t="s">
         <v>607</v>
       </c>
-      <c r="C118" s="79"/>
-      <c r="D118" s="79"/>
-      <c r="E118" s="79"/>
-      <c r="F118" s="79"/>
-      <c r="G118" s="79"/>
-      <c r="H118" s="79"/>
-      <c r="I118" s="79"/>
-      <c r="J118" s="79"/>
-      <c r="K118" s="79"/>
-      <c r="L118" s="79"/>
-      <c r="M118" s="79"/>
-      <c r="N118" s="79"/>
-      <c r="O118" s="79"/>
-      <c r="P118" s="79"/>
-      <c r="Q118" s="79"/>
-      <c r="R118" s="79"/>
-      <c r="S118" s="79"/>
-      <c r="T118" s="79"/>
-      <c r="U118" s="79"/>
-      <c r="V118" s="79"/>
-      <c r="W118" s="79"/>
-      <c r="X118" s="79"/>
-      <c r="Y118" s="79"/>
-      <c r="Z118" s="79"/>
-      <c r="AA118" s="79"/>
-      <c r="AB118" s="79"/>
-      <c r="AC118" s="79"/>
-      <c r="AD118" s="79"/>
-      <c r="AE118" s="79"/>
-      <c r="AF118" s="79"/>
-      <c r="AG118" s="79"/>
-      <c r="AH118" s="79"/>
-      <c r="AI118" s="79"/>
+      <c r="C118" s="78"/>
+      <c r="D118" s="78"/>
+      <c r="E118" s="78"/>
+      <c r="F118" s="78"/>
+      <c r="G118" s="78"/>
+      <c r="H118" s="78"/>
+      <c r="I118" s="78"/>
+      <c r="J118" s="78"/>
+      <c r="K118" s="78"/>
+      <c r="L118" s="78"/>
+      <c r="M118" s="78"/>
+      <c r="N118" s="78"/>
+      <c r="O118" s="78"/>
+      <c r="P118" s="78"/>
+      <c r="Q118" s="78"/>
+      <c r="R118" s="78"/>
+      <c r="S118" s="78"/>
+      <c r="T118" s="78"/>
+      <c r="U118" s="78"/>
+      <c r="V118" s="78"/>
+      <c r="W118" s="78"/>
+      <c r="X118" s="78"/>
+      <c r="Y118" s="78"/>
+      <c r="Z118" s="78"/>
+      <c r="AA118" s="78"/>
+      <c r="AB118" s="78"/>
+      <c r="AC118" s="78"/>
+      <c r="AD118" s="78"/>
+      <c r="AE118" s="78"/>
+      <c r="AF118" s="78"/>
+      <c r="AG118" s="78"/>
+      <c r="AH118" s="78"/>
+      <c r="AI118" s="78"/>
     </row>
     <row r="119" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B119" s="30" t="s">
@@ -41679,37 +41679,37 @@
       <c r="G1"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="79" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
     </row>
     <row r="3" spans="1:7" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="32"/>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="81" t="s">
         <v>255</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="83"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="82"/>
     </row>
     <row r="4" spans="1:7" s="12" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A4" s="32"/>
       <c r="B4" s="33"/>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="83" t="s">
         <v>256</v>
       </c>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
     </row>
     <row r="5" spans="1:7" ht="40.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="34"/>
@@ -48170,158 +48170,158 @@
       <c r="G303" s="13"/>
     </row>
     <row r="304" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A304" s="85" t="s">
+      <c r="A304" s="84" t="s">
         <v>234</v>
       </c>
-      <c r="B304" s="85"/>
-      <c r="C304" s="85"/>
-      <c r="D304" s="85"/>
-      <c r="E304" s="85"/>
-      <c r="F304" s="85"/>
-      <c r="G304" s="85"/>
+      <c r="B304" s="84"/>
+      <c r="C304" s="84"/>
+      <c r="D304" s="84"/>
+      <c r="E304" s="84"/>
+      <c r="F304" s="84"/>
+      <c r="G304" s="84"/>
       <c r="H304" s="28"/>
       <c r="I304" s="28"/>
     </row>
     <row r="305" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A305" s="85"/>
-      <c r="B305" s="85"/>
-      <c r="C305" s="85"/>
-      <c r="D305" s="85"/>
-      <c r="E305" s="85"/>
-      <c r="F305" s="85"/>
-      <c r="G305" s="85"/>
+      <c r="A305" s="84"/>
+      <c r="B305" s="84"/>
+      <c r="C305" s="84"/>
+      <c r="D305" s="84"/>
+      <c r="E305" s="84"/>
+      <c r="F305" s="84"/>
+      <c r="G305" s="84"/>
       <c r="H305" s="28"/>
       <c r="I305" s="28"/>
     </row>
     <row r="306" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A306" s="85"/>
-      <c r="B306" s="85"/>
-      <c r="C306" s="85"/>
-      <c r="D306" s="85"/>
-      <c r="E306" s="85"/>
-      <c r="F306" s="85"/>
-      <c r="G306" s="85"/>
+      <c r="A306" s="84"/>
+      <c r="B306" s="84"/>
+      <c r="C306" s="84"/>
+      <c r="D306" s="84"/>
+      <c r="E306" s="84"/>
+      <c r="F306" s="84"/>
+      <c r="G306" s="84"/>
       <c r="H306" s="28"/>
       <c r="I306" s="28"/>
     </row>
     <row r="307" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A307" s="85"/>
-      <c r="B307" s="85"/>
-      <c r="C307" s="85"/>
-      <c r="D307" s="85"/>
-      <c r="E307" s="85"/>
-      <c r="F307" s="85"/>
-      <c r="G307" s="85"/>
+      <c r="A307" s="84"/>
+      <c r="B307" s="84"/>
+      <c r="C307" s="84"/>
+      <c r="D307" s="84"/>
+      <c r="E307" s="84"/>
+      <c r="F307" s="84"/>
+      <c r="G307" s="84"/>
       <c r="H307" s="28"/>
       <c r="I307" s="28"/>
     </row>
     <row r="308" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A308" s="85"/>
-      <c r="B308" s="85"/>
-      <c r="C308" s="85"/>
-      <c r="D308" s="85"/>
-      <c r="E308" s="85"/>
-      <c r="F308" s="85"/>
-      <c r="G308" s="85"/>
+      <c r="A308" s="84"/>
+      <c r="B308" s="84"/>
+      <c r="C308" s="84"/>
+      <c r="D308" s="84"/>
+      <c r="E308" s="84"/>
+      <c r="F308" s="84"/>
+      <c r="G308" s="84"/>
       <c r="H308" s="28"/>
       <c r="I308" s="28"/>
     </row>
     <row r="309" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A309" s="85"/>
-      <c r="B309" s="85"/>
-      <c r="C309" s="85"/>
-      <c r="D309" s="85"/>
-      <c r="E309" s="85"/>
-      <c r="F309" s="85"/>
-      <c r="G309" s="85"/>
+      <c r="A309" s="84"/>
+      <c r="B309" s="84"/>
+      <c r="C309" s="84"/>
+      <c r="D309" s="84"/>
+      <c r="E309" s="84"/>
+      <c r="F309" s="84"/>
+      <c r="G309" s="84"/>
       <c r="H309" s="28"/>
       <c r="I309" s="28"/>
     </row>
     <row r="310" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A310" s="85"/>
-      <c r="B310" s="85"/>
-      <c r="C310" s="85"/>
-      <c r="D310" s="85"/>
-      <c r="E310" s="85"/>
-      <c r="F310" s="85"/>
-      <c r="G310" s="85"/>
+      <c r="A310" s="84"/>
+      <c r="B310" s="84"/>
+      <c r="C310" s="84"/>
+      <c r="D310" s="84"/>
+      <c r="E310" s="84"/>
+      <c r="F310" s="84"/>
+      <c r="G310" s="84"/>
       <c r="H310" s="28"/>
       <c r="I310" s="28"/>
     </row>
     <row r="311" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A311" s="85"/>
-      <c r="B311" s="85"/>
-      <c r="C311" s="85"/>
-      <c r="D311" s="85"/>
-      <c r="E311" s="85"/>
-      <c r="F311" s="85"/>
-      <c r="G311" s="85"/>
+      <c r="A311" s="84"/>
+      <c r="B311" s="84"/>
+      <c r="C311" s="84"/>
+      <c r="D311" s="84"/>
+      <c r="E311" s="84"/>
+      <c r="F311" s="84"/>
+      <c r="G311" s="84"/>
       <c r="H311" s="28"/>
       <c r="I311" s="28"/>
     </row>
     <row r="312" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A312" s="85"/>
-      <c r="B312" s="85"/>
-      <c r="C312" s="85"/>
-      <c r="D312" s="85"/>
-      <c r="E312" s="85"/>
-      <c r="F312" s="85"/>
-      <c r="G312" s="85"/>
+      <c r="A312" s="84"/>
+      <c r="B312" s="84"/>
+      <c r="C312" s="84"/>
+      <c r="D312" s="84"/>
+      <c r="E312" s="84"/>
+      <c r="F312" s="84"/>
+      <c r="G312" s="84"/>
       <c r="H312" s="28"/>
       <c r="I312" s="28"/>
     </row>
     <row r="313" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A313" s="85"/>
-      <c r="B313" s="85"/>
-      <c r="C313" s="85"/>
-      <c r="D313" s="85"/>
-      <c r="E313" s="85"/>
-      <c r="F313" s="85"/>
-      <c r="G313" s="85"/>
+      <c r="A313" s="84"/>
+      <c r="B313" s="84"/>
+      <c r="C313" s="84"/>
+      <c r="D313" s="84"/>
+      <c r="E313" s="84"/>
+      <c r="F313" s="84"/>
+      <c r="G313" s="84"/>
       <c r="H313" s="28"/>
       <c r="I313" s="28"/>
     </row>
     <row r="314" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A314" s="85"/>
-      <c r="B314" s="85"/>
-      <c r="C314" s="85"/>
-      <c r="D314" s="85"/>
-      <c r="E314" s="85"/>
-      <c r="F314" s="85"/>
-      <c r="G314" s="85"/>
+      <c r="A314" s="84"/>
+      <c r="B314" s="84"/>
+      <c r="C314" s="84"/>
+      <c r="D314" s="84"/>
+      <c r="E314" s="84"/>
+      <c r="F314" s="84"/>
+      <c r="G314" s="84"/>
       <c r="H314" s="28"/>
       <c r="I314" s="28"/>
     </row>
     <row r="315" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A315" s="85"/>
-      <c r="B315" s="85"/>
-      <c r="C315" s="85"/>
-      <c r="D315" s="85"/>
-      <c r="E315" s="85"/>
-      <c r="F315" s="85"/>
-      <c r="G315" s="85"/>
+      <c r="A315" s="84"/>
+      <c r="B315" s="84"/>
+      <c r="C315" s="84"/>
+      <c r="D315" s="84"/>
+      <c r="E315" s="84"/>
+      <c r="F315" s="84"/>
+      <c r="G315" s="84"/>
       <c r="H315" s="28"/>
       <c r="I315" s="28"/>
     </row>
     <row r="316" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A316" s="85"/>
-      <c r="B316" s="85"/>
-      <c r="C316" s="85"/>
-      <c r="D316" s="85"/>
-      <c r="E316" s="85"/>
-      <c r="F316" s="85"/>
-      <c r="G316" s="85"/>
+      <c r="A316" s="84"/>
+      <c r="B316" s="84"/>
+      <c r="C316" s="84"/>
+      <c r="D316" s="84"/>
+      <c r="E316" s="84"/>
+      <c r="F316" s="84"/>
+      <c r="G316" s="84"/>
       <c r="H316" s="28"/>
       <c r="I316" s="28"/>
     </row>
     <row r="317" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A317" s="85"/>
-      <c r="B317" s="85"/>
-      <c r="C317" s="85"/>
-      <c r="D317" s="85"/>
-      <c r="E317" s="85"/>
-      <c r="F317" s="85"/>
-      <c r="G317" s="85"/>
+      <c r="A317" s="84"/>
+      <c r="B317" s="84"/>
+      <c r="C317" s="84"/>
+      <c r="D317" s="84"/>
+      <c r="E317" s="84"/>
+      <c r="F317" s="84"/>
+      <c r="G317" s="84"/>
       <c r="H317" s="28"/>
       <c r="I317" s="28"/>
     </row>
@@ -48373,14 +48373,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1A7FE6B-E04E-4776-A8FC-22EB4ECE4947}">
   <dimension ref="A1:AO195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="F131" sqref="F131"/>
-    </sheetView>
+    <sheetView topLeftCell="G172" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="7" width="9.06640625" customWidth="1"/>
+    <col min="2" max="7" width="0" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="15.796875" customWidth="1"/>
     <col min="9" max="9" width="20.53125" customWidth="1"/>
     <col min="10" max="10" width="12.06640625" bestFit="1" customWidth="1"/>
@@ -60790,7 +60788,9 @@
       <c r="C131" s="66"/>
       <c r="D131" s="66"/>
       <c r="E131" s="66"/>
-      <c r="F131" s="66"/>
+      <c r="F131" s="66" t="s">
+        <v>104</v>
+      </c>
       <c r="G131" s="66"/>
     </row>
     <row r="132" spans="1:41" x14ac:dyDescent="0.45">
@@ -61412,269 +61412,234 @@
       <c r="I138" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J138" s="78">
+      <c r="J138" s="85">
         <f>'District Heat'!D9</f>
         <v>328342916402388.69</v>
       </c>
-      <c r="K138" s="78">
+      <c r="K138" s="85">
         <f>'District Heat'!E9</f>
         <v>328289571366317.06</v>
       </c>
-      <c r="L138" s="78">
+      <c r="L138" s="85">
         <f>'District Heat'!F9</f>
         <v>327742106631717.31</v>
       </c>
-      <c r="M138" s="78">
+      <c r="M138" s="85">
         <f>'District Heat'!G9</f>
         <v>326788074362311.63</v>
       </c>
-      <c r="N138" s="78">
+      <c r="N138" s="85">
         <f>'District Heat'!H9</f>
         <v>325041551853638.19</v>
       </c>
-      <c r="O138" s="78">
+      <c r="O138" s="85">
         <f>'District Heat'!I9</f>
         <v>323040510232182.13</v>
       </c>
-      <c r="P138" s="78">
+      <c r="P138" s="85">
         <f>'District Heat'!J9</f>
         <v>321299261950238.88</v>
       </c>
-      <c r="Q138" s="78">
+      <c r="Q138" s="85">
         <f>'District Heat'!K9</f>
         <v>319985979494407.19</v>
       </c>
-      <c r="R138" s="78">
+      <c r="R138" s="85">
         <f>'District Heat'!L9</f>
         <v>319192886486370.13</v>
       </c>
-      <c r="S138" s="78">
+      <c r="S138" s="85">
         <f>'District Heat'!M9</f>
         <v>318491414331247.19</v>
       </c>
-      <c r="T138" s="78">
+      <c r="T138" s="85">
         <f>'District Heat'!N9</f>
         <v>318220921846081.63</v>
       </c>
-      <c r="U138" s="78">
+      <c r="U138" s="85">
         <f>'District Heat'!O9</f>
         <v>318044009212329.88</v>
       </c>
-      <c r="V138" s="78">
+      <c r="V138" s="85">
         <f>'District Heat'!P9</f>
         <v>317512668542305.5</v>
       </c>
-      <c r="W138" s="78">
+      <c r="W138" s="85">
         <f>'District Heat'!Q9</f>
         <v>316836663367680</v>
       </c>
-      <c r="X138" s="78">
+      <c r="X138" s="85">
         <f>'District Heat'!R9</f>
         <v>316400861547569.25</v>
       </c>
-      <c r="Y138" s="78">
+      <c r="Y138" s="85">
         <f>'District Heat'!S9</f>
         <v>316265690651082.56</v>
       </c>
-      <c r="Z138" s="78">
+      <c r="Z138" s="85">
         <f>'District Heat'!T9</f>
         <v>315943812128345.19</v>
       </c>
-      <c r="AA138" s="78">
+      <c r="AA138" s="85">
         <f>'District Heat'!U9</f>
         <v>315549601353307.25</v>
       </c>
-      <c r="AB138" s="78">
+      <c r="AB138" s="85">
         <f>'District Heat'!V9</f>
         <v>315172870872575.25</v>
       </c>
-      <c r="AC138" s="78">
+      <c r="AC138" s="85">
         <f>'District Heat'!W9</f>
         <v>315013890609706.31</v>
       </c>
-      <c r="AD138" s="78">
+      <c r="AD138" s="85">
         <f>'District Heat'!X9</f>
         <v>314824621216186.56</v>
       </c>
-      <c r="AE138" s="78">
+      <c r="AE138" s="85">
         <f>'District Heat'!Y9</f>
         <v>314581705402210.63</v>
       </c>
-      <c r="AF138" s="78">
+      <c r="AF138" s="85">
         <f>'District Heat'!Z9</f>
         <v>314416848143842.25</v>
       </c>
-      <c r="AG138" s="78">
+      <c r="AG138" s="85">
         <f>'District Heat'!AA9</f>
         <v>314327638366004.94</v>
       </c>
-      <c r="AH138" s="78">
+      <c r="AH138" s="85">
         <f>'District Heat'!AB9</f>
         <v>314165041490521</v>
       </c>
-      <c r="AI138" s="78">
+      <c r="AI138" s="85">
         <f>'District Heat'!AC9</f>
         <v>313989183702115.31</v>
       </c>
-      <c r="AJ138" s="78">
+      <c r="AJ138" s="85">
         <f>'District Heat'!AD9</f>
         <v>313771885560829.06</v>
       </c>
-      <c r="AK138" s="78">
+      <c r="AK138" s="85">
         <f>'District Heat'!AE9</f>
         <v>313654044266456.13</v>
       </c>
-      <c r="AL138" s="78">
+      <c r="AL138" s="85">
         <f>'District Heat'!AF9</f>
         <v>313551272191312.44</v>
       </c>
-      <c r="AM138" s="78">
+      <c r="AM138" s="85">
         <f>'District Heat'!AG9</f>
         <v>313457541647706.38</v>
       </c>
-      <c r="AN138" s="78">
+      <c r="AN138" s="85">
         <f>'District Heat'!AH9</f>
         <v>-342221968696.93982</v>
       </c>
-      <c r="AO138" s="78">
+      <c r="AO138" s="85">
         <f>'District Heat'!AI9</f>
         <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:41" x14ac:dyDescent="0.45">
-      <c r="H139" s="14" t="s">
-        <v>558</v>
-      </c>
       <c r="I139" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="J139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(J$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="K139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(K$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="L139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(L$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="M139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(M$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="N139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(N$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="O139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(O$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="P139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(P$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="Q139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(Q$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="R139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(R$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="S139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(S$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="T139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(T$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="U139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(U$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="V139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(V$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="W139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(W$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="X139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(X$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="Y139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(Y$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="Z139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(Z$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="AA139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(AA$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="AB139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(AB$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="AC139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(AC$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="AD139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(AD$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="AE139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(AE$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="AF139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(AF$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="AG139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(AG$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="AH139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(AH$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="AI139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(AI$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="AJ139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(AJ$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="AK139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(AK$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="AL139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(AL$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="AM139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(AM$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="AN139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(AN$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
-      </c>
-      <c r="AO139" s="76">
-        <f>INDEX(Table5,MATCH($H139,'AEO Table 5'!$A$31:$A$58,0),MATCH(AO$133,'AEO Table 5'!$C$13:$AI$13,0))*quadrillion</f>
-        <v>130720000000000</v>
+      <c r="J139" s="9">
+        <v>0</v>
+      </c>
+      <c r="K139" s="9">
+        <v>0</v>
+      </c>
+      <c r="L139" s="9">
+        <v>0</v>
+      </c>
+      <c r="M139" s="9">
+        <v>0</v>
+      </c>
+      <c r="N139" s="9">
+        <v>0</v>
+      </c>
+      <c r="O139" s="9">
+        <v>0</v>
+      </c>
+      <c r="P139" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q139" s="9">
+        <v>0</v>
+      </c>
+      <c r="R139" s="9">
+        <v>0</v>
+      </c>
+      <c r="S139" s="9">
+        <v>0</v>
+      </c>
+      <c r="T139" s="9">
+        <v>0</v>
+      </c>
+      <c r="U139" s="9">
+        <v>0</v>
+      </c>
+      <c r="V139" s="9">
+        <v>0</v>
+      </c>
+      <c r="W139" s="9">
+        <v>0</v>
+      </c>
+      <c r="X139" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y139" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z139" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA139" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB139" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC139" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD139" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE139" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF139" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG139" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH139" s="9">
+        <v>0</v>
+      </c>
+      <c r="AI139" s="9">
+        <v>0</v>
+      </c>
+      <c r="AJ139" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK139" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL139" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM139" s="9">
+        <v>0</v>
+      </c>
+      <c r="AN139" s="9">
+        <v>0</v>
+      </c>
+      <c r="AO139" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:41" x14ac:dyDescent="0.45">
@@ -67117,9 +67082,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="J138" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Prevent bldgs/BCEU from being a mixed-type variable so VDF2TAB doesn't produce extra time axes when used on this variable (#86)
</commit_message>
<xml_diff>
--- a/InputData/bldgs/BCEU/BAU Components Energy Use.xlsx
+++ b/InputData/bldgs/BCEU/BAU Components Energy Use.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\bldgs\BCEU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\bldgs\BCEU\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9C7DAD-2B7D-41E3-BA06-7BF25D77A021}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9165" yWindow="240" windowWidth="10020" windowHeight="9690" firstSheet="13" activeTab="16"/>
+    <workbookView xWindow="2940" yWindow="900" windowWidth="23955" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -33,16 +34,17 @@
     <sheet name="BCEU-commercial-lighting" sheetId="15" r:id="rId19"/>
     <sheet name="BCEU-commercial-appl" sheetId="16" r:id="rId20"/>
     <sheet name="BCEU-commercial-other" sheetId="17" r:id="rId21"/>
+    <sheet name="BCEU-all-envelope" sheetId="31" r:id="rId22"/>
   </sheets>
   <definedNames>
     <definedName name="Fraction_coal">About!$C$50</definedName>
-    <definedName name="Percent_rural">About!$A$69</definedName>
-    <definedName name="Percent_urban">About!$A$68</definedName>
-    <definedName name="quadrillion">About!$B$71</definedName>
+    <definedName name="Percent_rural">About!$A$77</definedName>
+    <definedName name="Percent_urban">About!$A$76</definedName>
+    <definedName name="quadrillion">About!$B$79</definedName>
     <definedName name="Table4">'AEO Table 4'!$C$34:$AI$72</definedName>
     <definedName name="Table5">'AEO Table 5'!$C$31:$AI$58</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -57,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1836" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1854" uniqueCount="616">
   <si>
     <t>Sources:</t>
   </si>
@@ -2016,11 +2018,32 @@
   <si>
     <t>Quadrillion</t>
   </si>
+  <si>
+    <t>Note on Envelope</t>
+  </si>
+  <si>
+    <t>Envelope does not use energy itself, so it must always have zero in this variable.  We export</t>
+  </si>
+  <si>
+    <t>only one envelope CSV file, which is read by all building types.  (We need to export a CSV</t>
+  </si>
+  <si>
+    <t>file for envelope, instead of hard-coding the zero value in Vensim, because Vensim's VDF2TAB</t>
+  </si>
+  <si>
+    <t>export function inserts extra "Time" rows for variables of mixed type - data for some</t>
+  </si>
+  <si>
+    <t>subscript elements, constand for others - and we wish to avoid extra time rows when</t>
+  </si>
+  <si>
+    <t>VDF2TAB is used on BCEU BAU Components Energy Use.)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
@@ -2428,7 +2451,7 @@
     </xf>
     <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2625,26 +2648,27 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="18">
-    <cellStyle name="Body: normal cell" xfId="4"/>
-    <cellStyle name="Body: normal cell 2" xfId="11"/>
+    <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Body: normal cell 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Comma" xfId="17" builtinId="3"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="1"/>
-    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="13"/>
-    <cellStyle name="Footnotes: top row" xfId="6"/>
-    <cellStyle name="Footnotes: top row 2" xfId="9"/>
-    <cellStyle name="Header: bottom row" xfId="2"/>
-    <cellStyle name="Header: bottom row 2" xfId="12"/>
-    <cellStyle name="Header: top rows" xfId="16"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="13" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Footnotes: top row 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Header: bottom row" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Header: bottom row 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Header: top rows" xfId="16" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="8"/>
-    <cellStyle name="Parent row" xfId="5"/>
-    <cellStyle name="Parent row 2" xfId="10"/>
+    <cellStyle name="Normal 2" xfId="8" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Parent row" xfId="5" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Parent row 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="Percent" xfId="15" builtinId="5"/>
-    <cellStyle name="Table title" xfId="3"/>
-    <cellStyle name="Table title 2" xfId="14"/>
+    <cellStyle name="Table title" xfId="3" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Table title 2" xfId="14" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
   </cellStyles>
   <dxfs count="29">
     <dxf>
@@ -3026,6 +3050,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3061,6 +3102,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3236,12 +3294,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3553,41 +3609,76 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="51">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="51">
         <f>'RECS HC2.1'!B24/('RECS HC2.1'!B24+'RECS HC2.1'!B27)</f>
         <v>0.80118443316412857</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B76" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="51">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="51">
         <f>'RECS HC2.1'!B27/('RECS HC2.1'!B27+'RECS HC2.1'!B24)</f>
         <v>0.1988155668358714</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B77" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>608</v>
       </c>
-      <c r="B71" s="75">
+      <c r="B79" s="75">
         <f>10^15</f>
         <v>1000000000000000</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B21" r:id="rId1" display="http://www.euroheat.org/United-States-156.aspx"/>
-    <hyperlink ref="B7" r:id="rId2"/>
-    <hyperlink ref="B14" r:id="rId3"/>
+    <hyperlink ref="B21" r:id="rId1" display="http://www.euroheat.org/United-States-156.aspx" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B14" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
@@ -3595,7 +3686,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -5052,7 +5143,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -6508,7 +6599,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -7964,7 +8055,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -9420,7 +9511,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -10876,7 +10967,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -12335,7 +12426,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -13791,13 +13882,13 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AI11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -15250,7 +15341,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -16706,7 +16797,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -18162,7 +18253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AI159"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -29386,7 +29477,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -30842,7 +30933,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -32297,8 +32388,1142 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3425169B-F9CD-4E65-A74E-F6E3167B281E}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:AI11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="2" max="33" width="9.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2023</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2027</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2028</v>
+      </c>
+      <c r="L1" s="1">
+        <v>2029</v>
+      </c>
+      <c r="M1" s="1">
+        <v>2030</v>
+      </c>
+      <c r="N1" s="1">
+        <v>2031</v>
+      </c>
+      <c r="O1" s="1">
+        <v>2032</v>
+      </c>
+      <c r="P1" s="1">
+        <v>2033</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>2034</v>
+      </c>
+      <c r="R1" s="1">
+        <v>2035</v>
+      </c>
+      <c r="S1" s="1">
+        <v>2036</v>
+      </c>
+      <c r="T1" s="1">
+        <v>2037</v>
+      </c>
+      <c r="U1" s="1">
+        <v>2038</v>
+      </c>
+      <c r="V1" s="1">
+        <v>2039</v>
+      </c>
+      <c r="W1" s="1">
+        <v>2040</v>
+      </c>
+      <c r="X1" s="1">
+        <v>2041</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>2042</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>2043</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>2044</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>2045</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>2046</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>2047</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>2048</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>2049</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>2050</v>
+      </c>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="86">
+        <v>0</v>
+      </c>
+      <c r="C2" s="86">
+        <v>0</v>
+      </c>
+      <c r="D2" s="86">
+        <v>0</v>
+      </c>
+      <c r="E2" s="86">
+        <v>0</v>
+      </c>
+      <c r="F2" s="86">
+        <v>0</v>
+      </c>
+      <c r="G2" s="86">
+        <v>0</v>
+      </c>
+      <c r="H2" s="86">
+        <v>0</v>
+      </c>
+      <c r="I2" s="86">
+        <v>0</v>
+      </c>
+      <c r="J2" s="86">
+        <v>0</v>
+      </c>
+      <c r="K2" s="86">
+        <v>0</v>
+      </c>
+      <c r="L2" s="86">
+        <v>0</v>
+      </c>
+      <c r="M2" s="86">
+        <v>0</v>
+      </c>
+      <c r="N2" s="86">
+        <v>0</v>
+      </c>
+      <c r="O2" s="86">
+        <v>0</v>
+      </c>
+      <c r="P2" s="86">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="86">
+        <v>0</v>
+      </c>
+      <c r="R2" s="86">
+        <v>0</v>
+      </c>
+      <c r="S2" s="86">
+        <v>0</v>
+      </c>
+      <c r="T2" s="86">
+        <v>0</v>
+      </c>
+      <c r="U2" s="86">
+        <v>0</v>
+      </c>
+      <c r="V2" s="86">
+        <v>0</v>
+      </c>
+      <c r="W2" s="86">
+        <v>0</v>
+      </c>
+      <c r="X2" s="86">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="86">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="86">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="86">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="86">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="86">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="86">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="86">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="86">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="86">
+        <v>0</v>
+      </c>
+      <c r="C3" s="86">
+        <v>0</v>
+      </c>
+      <c r="D3" s="86">
+        <v>0</v>
+      </c>
+      <c r="E3" s="86">
+        <v>0</v>
+      </c>
+      <c r="F3" s="86">
+        <v>0</v>
+      </c>
+      <c r="G3" s="86">
+        <v>0</v>
+      </c>
+      <c r="H3" s="86">
+        <v>0</v>
+      </c>
+      <c r="I3" s="86">
+        <v>0</v>
+      </c>
+      <c r="J3" s="86">
+        <v>0</v>
+      </c>
+      <c r="K3" s="86">
+        <v>0</v>
+      </c>
+      <c r="L3" s="86">
+        <v>0</v>
+      </c>
+      <c r="M3" s="86">
+        <v>0</v>
+      </c>
+      <c r="N3" s="86">
+        <v>0</v>
+      </c>
+      <c r="O3" s="86">
+        <v>0</v>
+      </c>
+      <c r="P3" s="86">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="86">
+        <v>0</v>
+      </c>
+      <c r="R3" s="86">
+        <v>0</v>
+      </c>
+      <c r="S3" s="86">
+        <v>0</v>
+      </c>
+      <c r="T3" s="86">
+        <v>0</v>
+      </c>
+      <c r="U3" s="86">
+        <v>0</v>
+      </c>
+      <c r="V3" s="86">
+        <v>0</v>
+      </c>
+      <c r="W3" s="86">
+        <v>0</v>
+      </c>
+      <c r="X3" s="86">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="86">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="86">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="86">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="86">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="86">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="86">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="86">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="86">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="86">
+        <v>0</v>
+      </c>
+      <c r="C4" s="86">
+        <v>0</v>
+      </c>
+      <c r="D4" s="86">
+        <v>0</v>
+      </c>
+      <c r="E4" s="86">
+        <v>0</v>
+      </c>
+      <c r="F4" s="86">
+        <v>0</v>
+      </c>
+      <c r="G4" s="86">
+        <v>0</v>
+      </c>
+      <c r="H4" s="86">
+        <v>0</v>
+      </c>
+      <c r="I4" s="86">
+        <v>0</v>
+      </c>
+      <c r="J4" s="86">
+        <v>0</v>
+      </c>
+      <c r="K4" s="86">
+        <v>0</v>
+      </c>
+      <c r="L4" s="86">
+        <v>0</v>
+      </c>
+      <c r="M4" s="86">
+        <v>0</v>
+      </c>
+      <c r="N4" s="86">
+        <v>0</v>
+      </c>
+      <c r="O4" s="86">
+        <v>0</v>
+      </c>
+      <c r="P4" s="86">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="86">
+        <v>0</v>
+      </c>
+      <c r="R4" s="86">
+        <v>0</v>
+      </c>
+      <c r="S4" s="86">
+        <v>0</v>
+      </c>
+      <c r="T4" s="86">
+        <v>0</v>
+      </c>
+      <c r="U4" s="86">
+        <v>0</v>
+      </c>
+      <c r="V4" s="86">
+        <v>0</v>
+      </c>
+      <c r="W4" s="86">
+        <v>0</v>
+      </c>
+      <c r="X4" s="86">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="86">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="86">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="86">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="86">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="86">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="86">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="86">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="86">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="86">
+        <v>0</v>
+      </c>
+      <c r="C5" s="86">
+        <v>0</v>
+      </c>
+      <c r="D5" s="86">
+        <v>0</v>
+      </c>
+      <c r="E5" s="86">
+        <v>0</v>
+      </c>
+      <c r="F5" s="86">
+        <v>0</v>
+      </c>
+      <c r="G5" s="86">
+        <v>0</v>
+      </c>
+      <c r="H5" s="86">
+        <v>0</v>
+      </c>
+      <c r="I5" s="86">
+        <v>0</v>
+      </c>
+      <c r="J5" s="86">
+        <v>0</v>
+      </c>
+      <c r="K5" s="86">
+        <v>0</v>
+      </c>
+      <c r="L5" s="86">
+        <v>0</v>
+      </c>
+      <c r="M5" s="86">
+        <v>0</v>
+      </c>
+      <c r="N5" s="86">
+        <v>0</v>
+      </c>
+      <c r="O5" s="86">
+        <v>0</v>
+      </c>
+      <c r="P5" s="86">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="86">
+        <v>0</v>
+      </c>
+      <c r="R5" s="86">
+        <v>0</v>
+      </c>
+      <c r="S5" s="86">
+        <v>0</v>
+      </c>
+      <c r="T5" s="86">
+        <v>0</v>
+      </c>
+      <c r="U5" s="86">
+        <v>0</v>
+      </c>
+      <c r="V5" s="86">
+        <v>0</v>
+      </c>
+      <c r="W5" s="86">
+        <v>0</v>
+      </c>
+      <c r="X5" s="86">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="86">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="86">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="86">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="86">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="86">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="86">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="86">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="86">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="86">
+        <v>0</v>
+      </c>
+      <c r="C6" s="86">
+        <v>0</v>
+      </c>
+      <c r="D6" s="86">
+        <v>0</v>
+      </c>
+      <c r="E6" s="86">
+        <v>0</v>
+      </c>
+      <c r="F6" s="86">
+        <v>0</v>
+      </c>
+      <c r="G6" s="86">
+        <v>0</v>
+      </c>
+      <c r="H6" s="86">
+        <v>0</v>
+      </c>
+      <c r="I6" s="86">
+        <v>0</v>
+      </c>
+      <c r="J6" s="86">
+        <v>0</v>
+      </c>
+      <c r="K6" s="86">
+        <v>0</v>
+      </c>
+      <c r="L6" s="86">
+        <v>0</v>
+      </c>
+      <c r="M6" s="86">
+        <v>0</v>
+      </c>
+      <c r="N6" s="86">
+        <v>0</v>
+      </c>
+      <c r="O6" s="86">
+        <v>0</v>
+      </c>
+      <c r="P6" s="86">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="86">
+        <v>0</v>
+      </c>
+      <c r="R6" s="86">
+        <v>0</v>
+      </c>
+      <c r="S6" s="86">
+        <v>0</v>
+      </c>
+      <c r="T6" s="86">
+        <v>0</v>
+      </c>
+      <c r="U6" s="86">
+        <v>0</v>
+      </c>
+      <c r="V6" s="86">
+        <v>0</v>
+      </c>
+      <c r="W6" s="86">
+        <v>0</v>
+      </c>
+      <c r="X6" s="86">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="86">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="86">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="86">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="86">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="86">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="86">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="86">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="86">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B7" s="86">
+        <v>0</v>
+      </c>
+      <c r="C7" s="86">
+        <v>0</v>
+      </c>
+      <c r="D7" s="86">
+        <v>0</v>
+      </c>
+      <c r="E7" s="86">
+        <v>0</v>
+      </c>
+      <c r="F7" s="86">
+        <v>0</v>
+      </c>
+      <c r="G7" s="86">
+        <v>0</v>
+      </c>
+      <c r="H7" s="86">
+        <v>0</v>
+      </c>
+      <c r="I7" s="86">
+        <v>0</v>
+      </c>
+      <c r="J7" s="86">
+        <v>0</v>
+      </c>
+      <c r="K7" s="86">
+        <v>0</v>
+      </c>
+      <c r="L7" s="86">
+        <v>0</v>
+      </c>
+      <c r="M7" s="86">
+        <v>0</v>
+      </c>
+      <c r="N7" s="86">
+        <v>0</v>
+      </c>
+      <c r="O7" s="86">
+        <v>0</v>
+      </c>
+      <c r="P7" s="86">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="86">
+        <v>0</v>
+      </c>
+      <c r="R7" s="86">
+        <v>0</v>
+      </c>
+      <c r="S7" s="86">
+        <v>0</v>
+      </c>
+      <c r="T7" s="86">
+        <v>0</v>
+      </c>
+      <c r="U7" s="86">
+        <v>0</v>
+      </c>
+      <c r="V7" s="86">
+        <v>0</v>
+      </c>
+      <c r="W7" s="86">
+        <v>0</v>
+      </c>
+      <c r="X7" s="86">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="86">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="86">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="86">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="86">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="86">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="86">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="86">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="86">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B8" s="86">
+        <v>0</v>
+      </c>
+      <c r="C8" s="86">
+        <v>0</v>
+      </c>
+      <c r="D8" s="86">
+        <v>0</v>
+      </c>
+      <c r="E8" s="86">
+        <v>0</v>
+      </c>
+      <c r="F8" s="86">
+        <v>0</v>
+      </c>
+      <c r="G8" s="86">
+        <v>0</v>
+      </c>
+      <c r="H8" s="86">
+        <v>0</v>
+      </c>
+      <c r="I8" s="86">
+        <v>0</v>
+      </c>
+      <c r="J8" s="86">
+        <v>0</v>
+      </c>
+      <c r="K8" s="86">
+        <v>0</v>
+      </c>
+      <c r="L8" s="86">
+        <v>0</v>
+      </c>
+      <c r="M8" s="86">
+        <v>0</v>
+      </c>
+      <c r="N8" s="86">
+        <v>0</v>
+      </c>
+      <c r="O8" s="86">
+        <v>0</v>
+      </c>
+      <c r="P8" s="86">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="86">
+        <v>0</v>
+      </c>
+      <c r="R8" s="86">
+        <v>0</v>
+      </c>
+      <c r="S8" s="86">
+        <v>0</v>
+      </c>
+      <c r="T8" s="86">
+        <v>0</v>
+      </c>
+      <c r="U8" s="86">
+        <v>0</v>
+      </c>
+      <c r="V8" s="86">
+        <v>0</v>
+      </c>
+      <c r="W8" s="86">
+        <v>0</v>
+      </c>
+      <c r="X8" s="86">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="86">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="86">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="86">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="86">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="86">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="86">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="86">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="86">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B9" s="86">
+        <v>0</v>
+      </c>
+      <c r="C9" s="86">
+        <v>0</v>
+      </c>
+      <c r="D9" s="86">
+        <v>0</v>
+      </c>
+      <c r="E9" s="86">
+        <v>0</v>
+      </c>
+      <c r="F9" s="86">
+        <v>0</v>
+      </c>
+      <c r="G9" s="86">
+        <v>0</v>
+      </c>
+      <c r="H9" s="86">
+        <v>0</v>
+      </c>
+      <c r="I9" s="86">
+        <v>0</v>
+      </c>
+      <c r="J9" s="86">
+        <v>0</v>
+      </c>
+      <c r="K9" s="86">
+        <v>0</v>
+      </c>
+      <c r="L9" s="86">
+        <v>0</v>
+      </c>
+      <c r="M9" s="86">
+        <v>0</v>
+      </c>
+      <c r="N9" s="86">
+        <v>0</v>
+      </c>
+      <c r="O9" s="86">
+        <v>0</v>
+      </c>
+      <c r="P9" s="86">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="86">
+        <v>0</v>
+      </c>
+      <c r="R9" s="86">
+        <v>0</v>
+      </c>
+      <c r="S9" s="86">
+        <v>0</v>
+      </c>
+      <c r="T9" s="86">
+        <v>0</v>
+      </c>
+      <c r="U9" s="86">
+        <v>0</v>
+      </c>
+      <c r="V9" s="86">
+        <v>0</v>
+      </c>
+      <c r="W9" s="86">
+        <v>0</v>
+      </c>
+      <c r="X9" s="86">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="86">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="86">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="86">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="86">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="86">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="86">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="86">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="86">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B10" s="86">
+        <v>0</v>
+      </c>
+      <c r="C10" s="86">
+        <v>0</v>
+      </c>
+      <c r="D10" s="86">
+        <v>0</v>
+      </c>
+      <c r="E10" s="86">
+        <v>0</v>
+      </c>
+      <c r="F10" s="86">
+        <v>0</v>
+      </c>
+      <c r="G10" s="86">
+        <v>0</v>
+      </c>
+      <c r="H10" s="86">
+        <v>0</v>
+      </c>
+      <c r="I10" s="86">
+        <v>0</v>
+      </c>
+      <c r="J10" s="86">
+        <v>0</v>
+      </c>
+      <c r="K10" s="86">
+        <v>0</v>
+      </c>
+      <c r="L10" s="86">
+        <v>0</v>
+      </c>
+      <c r="M10" s="86">
+        <v>0</v>
+      </c>
+      <c r="N10" s="86">
+        <v>0</v>
+      </c>
+      <c r="O10" s="86">
+        <v>0</v>
+      </c>
+      <c r="P10" s="86">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="86">
+        <v>0</v>
+      </c>
+      <c r="R10" s="86">
+        <v>0</v>
+      </c>
+      <c r="S10" s="86">
+        <v>0</v>
+      </c>
+      <c r="T10" s="86">
+        <v>0</v>
+      </c>
+      <c r="U10" s="86">
+        <v>0</v>
+      </c>
+      <c r="V10" s="86">
+        <v>0</v>
+      </c>
+      <c r="W10" s="86">
+        <v>0</v>
+      </c>
+      <c r="X10" s="86">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="86">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="86">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="86">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="86">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="86">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="86">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="86">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="86">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B11" s="86">
+        <v>0</v>
+      </c>
+      <c r="C11" s="86">
+        <v>0</v>
+      </c>
+      <c r="D11" s="86">
+        <v>0</v>
+      </c>
+      <c r="E11" s="86">
+        <v>0</v>
+      </c>
+      <c r="F11" s="86">
+        <v>0</v>
+      </c>
+      <c r="G11" s="86">
+        <v>0</v>
+      </c>
+      <c r="H11" s="86">
+        <v>0</v>
+      </c>
+      <c r="I11" s="86">
+        <v>0</v>
+      </c>
+      <c r="J11" s="86">
+        <v>0</v>
+      </c>
+      <c r="K11" s="86">
+        <v>0</v>
+      </c>
+      <c r="L11" s="86">
+        <v>0</v>
+      </c>
+      <c r="M11" s="86">
+        <v>0</v>
+      </c>
+      <c r="N11" s="86">
+        <v>0</v>
+      </c>
+      <c r="O11" s="86">
+        <v>0</v>
+      </c>
+      <c r="P11" s="86">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="86">
+        <v>0</v>
+      </c>
+      <c r="R11" s="86">
+        <v>0</v>
+      </c>
+      <c r="S11" s="86">
+        <v>0</v>
+      </c>
+      <c r="T11" s="86">
+        <v>0</v>
+      </c>
+      <c r="U11" s="86">
+        <v>0</v>
+      </c>
+      <c r="V11" s="86">
+        <v>0</v>
+      </c>
+      <c r="W11" s="86">
+        <v>0</v>
+      </c>
+      <c r="X11" s="86">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="86">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="86">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="86">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="86">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="86">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="86">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="86">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="86">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="86">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AI134"/>
   <sheetViews>
     <sheetView topLeftCell="T1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -41184,7 +42409,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AI9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -41495,7 +42720,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J320"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -48335,7 +49560,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AO195"/>
   <sheetViews>
     <sheetView topLeftCell="I118" workbookViewId="0">
@@ -67055,7 +68280,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -68515,7 +69740,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -69971,7 +71196,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>

</xml_diff>

<commit_message>
advance start year .mdl, ccamc, IT, update gdpgr to take out covid recession, fix bug in comm heat
</commit_message>
<xml_diff>
--- a/InputData/bldgs/BCEU/BAU Components Energy Use.xlsx
+++ b/InputData/bldgs/BCEU/BAU Components Energy Use.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\US_EPS\InputData\bldgs\BCEU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\us-eps\InputData\bldgs\BCEU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CDBC84-7227-4E6A-B580-C2BB8AE7DDB6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8A3C73-8E87-4BA5-99D6-66566EC6D3D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="1155" windowWidth="13215" windowHeight="15810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="840" windowWidth="28005" windowHeight="15645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2720,6 +2720,7 @@
     <xf numFmtId="168" fontId="3" fillId="0" borderId="3" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="5">
       <alignment wrapText="1"/>
     </xf>
@@ -2733,7 +2734,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="4" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3409,7 +3409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -12544,7 +12544,7 @@
   <dimension ref="A1:AI11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13999,7 +13999,9 @@
   </sheetPr>
   <dimension ref="A1:AI11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14007,7 +14009,8 @@
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="33" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="32" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
@@ -14655,127 +14658,127 @@
       </c>
       <c r="C6" s="9">
         <f>Calculations!K138</f>
-        <v>348233022820383.44</v>
+        <v>336352809191520</v>
       </c>
       <c r="D6" s="9">
         <f>Calculations!L138</f>
-        <v>347221008177414</v>
+        <v>348233022820383.44</v>
       </c>
       <c r="E6" s="9">
         <f>Calculations!M138</f>
-        <v>347869235071709.25</v>
+        <v>347221008177414</v>
       </c>
       <c r="F6" s="9">
         <f>Calculations!N138</f>
-        <v>350786576050082.56</v>
+        <v>347869235071709.25</v>
       </c>
       <c r="G6" s="9">
         <f>Calculations!O138</f>
-        <v>352843560602611.69</v>
+        <v>350786576050082.56</v>
       </c>
       <c r="H6" s="9">
         <f>Calculations!P138</f>
-        <v>353347488222806.69</v>
+        <v>352843560602611.69</v>
       </c>
       <c r="I6" s="9">
         <f>Calculations!Q138</f>
-        <v>352608394379854</v>
+        <v>353347488222806.69</v>
       </c>
       <c r="J6" s="9">
         <f>Calculations!R138</f>
-        <v>351575582723987.81</v>
+        <v>352608394379854</v>
       </c>
       <c r="K6" s="9">
         <f>Calculations!S138</f>
-        <v>349976132455191.19</v>
+        <v>351575582723987.81</v>
       </c>
       <c r="L6" s="9">
         <f>Calculations!T138</f>
-        <v>347839159391519.88</v>
+        <v>349976132455191.19</v>
       </c>
       <c r="M6" s="9">
         <f>Calculations!U138</f>
-        <v>346373289936330.5</v>
+        <v>347839159391519.88</v>
       </c>
       <c r="N6" s="9">
         <f>Calculations!V138</f>
-        <v>345300484024893.13</v>
+        <v>346373289936330.5</v>
       </c>
       <c r="O6" s="9">
         <f>Calculations!W138</f>
-        <v>344274711358007.38</v>
+        <v>345300484024893.13</v>
       </c>
       <c r="P6" s="9">
         <f>Calculations!X138</f>
-        <v>343328607248219.06</v>
+        <v>344274711358007.38</v>
       </c>
       <c r="Q6" s="9">
         <f>Calculations!Y138</f>
-        <v>342625668212302.69</v>
+        <v>343328607248219.06</v>
       </c>
       <c r="R6" s="9">
         <f>Calculations!Z138</f>
-        <v>341985280192099.31</v>
+        <v>342625668212302.69</v>
       </c>
       <c r="S6" s="9">
         <f>Calculations!AA138</f>
-        <v>341153399676221.88</v>
+        <v>341985280192099.31</v>
       </c>
       <c r="T6" s="9">
         <f>Calculations!AB138</f>
-        <v>340303281779804</v>
+        <v>341153399676221.88</v>
       </c>
       <c r="U6" s="9">
         <f>Calculations!AC138</f>
-        <v>339511715473542.25</v>
+        <v>340303281779804</v>
       </c>
       <c r="V6" s="9">
         <f>Calculations!AD138</f>
-        <v>338614084401506</v>
+        <v>339511715473542.25</v>
       </c>
       <c r="W6" s="9">
         <f>Calculations!AE138</f>
-        <v>337634545094060.38</v>
+        <v>338614084401506</v>
       </c>
       <c r="X6" s="9">
         <f>Calculations!AF138</f>
-        <v>336460633704539.5</v>
+        <v>337634545094060.38</v>
       </c>
       <c r="Y6" s="9">
         <f>Calculations!AG138</f>
-        <v>335200334722985.19</v>
+        <v>336460633704539.5</v>
       </c>
       <c r="Z6" s="9">
         <f>Calculations!AH138</f>
-        <v>333844849413171.81</v>
+        <v>335200334722985.19</v>
       </c>
       <c r="AA6" s="9">
         <f>Calculations!AI138</f>
-        <v>332403136488347.38</v>
+        <v>333844849413171.81</v>
       </c>
       <c r="AB6" s="9">
         <f>Calculations!AJ138</f>
-        <v>331004937313584.13</v>
+        <v>332403136488347.38</v>
       </c>
       <c r="AC6" s="9">
         <f>Calculations!AK138</f>
-        <v>329646412440347.31</v>
+        <v>331004937313584.13</v>
       </c>
       <c r="AD6" s="9">
         <f>Calculations!AL138</f>
-        <v>328457943141798.63</v>
+        <v>329646412440347.31</v>
       </c>
       <c r="AE6" s="9">
         <f>Calculations!AM138</f>
-        <v>327133493374308.38</v>
+        <v>328457943141798.63</v>
       </c>
       <c r="AF6" s="9">
         <f>Calculations!AN138</f>
-        <v>325590674971400.31</v>
+        <v>327133493374308.38</v>
       </c>
       <c r="AG6" s="9">
         <f>Calculations!AO138</f>
-        <v>-173255115133.70282</v>
+        <v>325590674971400.31</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
@@ -26797,103 +26800,103 @@
       <c r="A112" s="14" t="s">
         <v>447</v>
       </c>
-      <c r="B112" s="90" t="s">
+      <c r="B112" s="91" t="s">
         <v>592</v>
       </c>
-      <c r="C112" s="91">
+      <c r="C112" s="92">
         <v>21.012035000000001</v>
       </c>
-      <c r="D112" s="91">
+      <c r="D112" s="92">
         <v>21.043247000000001</v>
       </c>
-      <c r="E112" s="91">
+      <c r="E112" s="92">
         <v>21.216681999999999</v>
       </c>
-      <c r="F112" s="91">
+      <c r="F112" s="92">
         <v>21.018280000000001</v>
       </c>
-      <c r="G112" s="91">
+      <c r="G112" s="92">
         <v>20.85379</v>
       </c>
-      <c r="H112" s="91">
+      <c r="H112" s="92">
         <v>20.627789</v>
       </c>
-      <c r="I112" s="91">
+      <c r="I112" s="92">
         <v>20.385228999999999</v>
       </c>
-      <c r="J112" s="91">
+      <c r="J112" s="92">
         <v>20.220219</v>
       </c>
-      <c r="K112" s="91">
+      <c r="K112" s="92">
         <v>20.168883999999998</v>
       </c>
-      <c r="L112" s="91">
+      <c r="L112" s="92">
         <v>20.144856999999998</v>
       </c>
-      <c r="M112" s="91">
+      <c r="M112" s="92">
         <v>20.183903000000001</v>
       </c>
-      <c r="N112" s="91">
+      <c r="N112" s="92">
         <v>20.200790000000001</v>
       </c>
-      <c r="O112" s="91">
+      <c r="O112" s="92">
         <v>20.210455</v>
       </c>
-      <c r="P112" s="91">
+      <c r="P112" s="92">
         <v>20.251712999999999</v>
       </c>
-      <c r="Q112" s="91">
+      <c r="Q112" s="92">
         <v>20.298100000000002</v>
       </c>
-      <c r="R112" s="91">
+      <c r="R112" s="92">
         <v>20.374268000000001</v>
       </c>
-      <c r="S112" s="91">
+      <c r="S112" s="92">
         <v>20.453151999999999</v>
       </c>
-      <c r="T112" s="91">
+      <c r="T112" s="92">
         <v>20.522358000000001</v>
       </c>
-      <c r="U112" s="91">
+      <c r="U112" s="92">
         <v>20.597715000000001</v>
       </c>
-      <c r="V112" s="91">
+      <c r="V112" s="92">
         <v>20.691054999999999</v>
       </c>
-      <c r="W112" s="91">
+      <c r="W112" s="92">
         <v>20.79027</v>
       </c>
-      <c r="X112" s="91">
+      <c r="X112" s="92">
         <v>20.887352</v>
       </c>
-      <c r="Y112" s="91">
+      <c r="Y112" s="92">
         <v>20.988150000000001</v>
       </c>
-      <c r="Z112" s="91">
+      <c r="Z112" s="92">
         <v>21.068726000000002</v>
       </c>
-      <c r="AA112" s="91">
+      <c r="AA112" s="92">
         <v>21.118212</v>
       </c>
-      <c r="AB112" s="91">
+      <c r="AB112" s="92">
         <v>21.216028000000001</v>
       </c>
-      <c r="AC112" s="91">
+      <c r="AC112" s="92">
         <v>21.321000999999999</v>
       </c>
-      <c r="AD112" s="91">
+      <c r="AD112" s="92">
         <v>21.423819999999999</v>
       </c>
-      <c r="AE112" s="91">
+      <c r="AE112" s="92">
         <v>21.530754000000002</v>
       </c>
-      <c r="AF112" s="91">
+      <c r="AF112" s="92">
         <v>21.665205</v>
       </c>
-      <c r="AG112" s="91">
+      <c r="AG112" s="92">
         <v>21.802175999999999</v>
       </c>
-      <c r="AH112" s="92">
+      <c r="AH112" s="93">
         <v>1.2310000000000001E-3</v>
       </c>
     </row>
@@ -29722,40 +29725,40 @@
     </row>
     <row r="146" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="147" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B147" s="93" t="s">
+      <c r="B147" s="94" t="s">
         <v>598</v>
       </c>
-      <c r="C147" s="94"/>
-      <c r="D147" s="94"/>
-      <c r="E147" s="94"/>
-      <c r="F147" s="94"/>
-      <c r="G147" s="94"/>
-      <c r="H147" s="94"/>
-      <c r="I147" s="94"/>
-      <c r="J147" s="94"/>
-      <c r="K147" s="94"/>
-      <c r="L147" s="94"/>
-      <c r="M147" s="94"/>
-      <c r="N147" s="94"/>
-      <c r="O147" s="94"/>
-      <c r="P147" s="94"/>
-      <c r="Q147" s="94"/>
-      <c r="R147" s="94"/>
-      <c r="S147" s="94"/>
-      <c r="T147" s="94"/>
-      <c r="U147" s="94"/>
-      <c r="V147" s="94"/>
-      <c r="W147" s="94"/>
-      <c r="X147" s="94"/>
-      <c r="Y147" s="94"/>
-      <c r="Z147" s="94"/>
-      <c r="AA147" s="94"/>
-      <c r="AB147" s="94"/>
-      <c r="AC147" s="94"/>
-      <c r="AD147" s="94"/>
-      <c r="AE147" s="94"/>
-      <c r="AF147" s="94"/>
-      <c r="AG147" s="94"/>
+      <c r="C147" s="95"/>
+      <c r="D147" s="95"/>
+      <c r="E147" s="95"/>
+      <c r="F147" s="95"/>
+      <c r="G147" s="95"/>
+      <c r="H147" s="95"/>
+      <c r="I147" s="95"/>
+      <c r="J147" s="95"/>
+      <c r="K147" s="95"/>
+      <c r="L147" s="95"/>
+      <c r="M147" s="95"/>
+      <c r="N147" s="95"/>
+      <c r="O147" s="95"/>
+      <c r="P147" s="95"/>
+      <c r="Q147" s="95"/>
+      <c r="R147" s="95"/>
+      <c r="S147" s="95"/>
+      <c r="T147" s="95"/>
+      <c r="U147" s="95"/>
+      <c r="V147" s="95"/>
+      <c r="W147" s="95"/>
+      <c r="X147" s="95"/>
+      <c r="Y147" s="95"/>
+      <c r="Z147" s="95"/>
+      <c r="AA147" s="95"/>
+      <c r="AB147" s="95"/>
+      <c r="AC147" s="95"/>
+      <c r="AD147" s="95"/>
+      <c r="AE147" s="95"/>
+      <c r="AF147" s="95"/>
+      <c r="AG147" s="95"/>
       <c r="AH147" s="77"/>
     </row>
     <row r="148" spans="1:34" x14ac:dyDescent="0.25">
@@ -29859,693 +29862,693 @@
       </c>
     </row>
     <row r="308" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B308" s="95"/>
-      <c r="C308" s="95"/>
-      <c r="D308" s="95"/>
-      <c r="E308" s="95"/>
-      <c r="F308" s="95"/>
-      <c r="G308" s="95"/>
-      <c r="H308" s="95"/>
-      <c r="I308" s="95"/>
-      <c r="J308" s="95"/>
-      <c r="K308" s="95"/>
-      <c r="L308" s="95"/>
-      <c r="M308" s="95"/>
-      <c r="N308" s="95"/>
-      <c r="O308" s="95"/>
-      <c r="P308" s="95"/>
-      <c r="Q308" s="95"/>
-      <c r="R308" s="95"/>
-      <c r="S308" s="95"/>
-      <c r="T308" s="95"/>
-      <c r="U308" s="95"/>
-      <c r="V308" s="95"/>
-      <c r="W308" s="95"/>
-      <c r="X308" s="95"/>
-      <c r="Y308" s="95"/>
-      <c r="Z308" s="95"/>
-      <c r="AA308" s="95"/>
-      <c r="AB308" s="95"/>
-      <c r="AC308" s="95"/>
-      <c r="AD308" s="95"/>
-      <c r="AE308" s="95"/>
-      <c r="AF308" s="95"/>
-      <c r="AG308" s="95"/>
-      <c r="AH308" s="95"/>
+      <c r="B308" s="90"/>
+      <c r="C308" s="90"/>
+      <c r="D308" s="90"/>
+      <c r="E308" s="90"/>
+      <c r="F308" s="90"/>
+      <c r="G308" s="90"/>
+      <c r="H308" s="90"/>
+      <c r="I308" s="90"/>
+      <c r="J308" s="90"/>
+      <c r="K308" s="90"/>
+      <c r="L308" s="90"/>
+      <c r="M308" s="90"/>
+      <c r="N308" s="90"/>
+      <c r="O308" s="90"/>
+      <c r="P308" s="90"/>
+      <c r="Q308" s="90"/>
+      <c r="R308" s="90"/>
+      <c r="S308" s="90"/>
+      <c r="T308" s="90"/>
+      <c r="U308" s="90"/>
+      <c r="V308" s="90"/>
+      <c r="W308" s="90"/>
+      <c r="X308" s="90"/>
+      <c r="Y308" s="90"/>
+      <c r="Z308" s="90"/>
+      <c r="AA308" s="90"/>
+      <c r="AB308" s="90"/>
+      <c r="AC308" s="90"/>
+      <c r="AD308" s="90"/>
+      <c r="AE308" s="90"/>
+      <c r="AF308" s="90"/>
+      <c r="AG308" s="90"/>
+      <c r="AH308" s="90"/>
     </row>
     <row r="511" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B511" s="95"/>
-      <c r="C511" s="95"/>
-      <c r="D511" s="95"/>
-      <c r="E511" s="95"/>
-      <c r="F511" s="95"/>
-      <c r="G511" s="95"/>
-      <c r="H511" s="95"/>
-      <c r="I511" s="95"/>
-      <c r="J511" s="95"/>
-      <c r="K511" s="95"/>
-      <c r="L511" s="95"/>
-      <c r="M511" s="95"/>
-      <c r="N511" s="95"/>
-      <c r="O511" s="95"/>
-      <c r="P511" s="95"/>
-      <c r="Q511" s="95"/>
-      <c r="R511" s="95"/>
-      <c r="S511" s="95"/>
-      <c r="T511" s="95"/>
-      <c r="U511" s="95"/>
-      <c r="V511" s="95"/>
-      <c r="W511" s="95"/>
-      <c r="X511" s="95"/>
-      <c r="Y511" s="95"/>
-      <c r="Z511" s="95"/>
-      <c r="AA511" s="95"/>
-      <c r="AB511" s="95"/>
-      <c r="AC511" s="95"/>
-      <c r="AD511" s="95"/>
-      <c r="AE511" s="95"/>
-      <c r="AF511" s="95"/>
-      <c r="AG511" s="95"/>
-      <c r="AH511" s="95"/>
+      <c r="B511" s="90"/>
+      <c r="C511" s="90"/>
+      <c r="D511" s="90"/>
+      <c r="E511" s="90"/>
+      <c r="F511" s="90"/>
+      <c r="G511" s="90"/>
+      <c r="H511" s="90"/>
+      <c r="I511" s="90"/>
+      <c r="J511" s="90"/>
+      <c r="K511" s="90"/>
+      <c r="L511" s="90"/>
+      <c r="M511" s="90"/>
+      <c r="N511" s="90"/>
+      <c r="O511" s="90"/>
+      <c r="P511" s="90"/>
+      <c r="Q511" s="90"/>
+      <c r="R511" s="90"/>
+      <c r="S511" s="90"/>
+      <c r="T511" s="90"/>
+      <c r="U511" s="90"/>
+      <c r="V511" s="90"/>
+      <c r="W511" s="90"/>
+      <c r="X511" s="90"/>
+      <c r="Y511" s="90"/>
+      <c r="Z511" s="90"/>
+      <c r="AA511" s="90"/>
+      <c r="AB511" s="90"/>
+      <c r="AC511" s="90"/>
+      <c r="AD511" s="90"/>
+      <c r="AE511" s="90"/>
+      <c r="AF511" s="90"/>
+      <c r="AG511" s="90"/>
+      <c r="AH511" s="90"/>
     </row>
     <row r="712" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B712" s="95"/>
-      <c r="C712" s="95"/>
-      <c r="D712" s="95"/>
-      <c r="E712" s="95"/>
-      <c r="F712" s="95"/>
-      <c r="G712" s="95"/>
-      <c r="H712" s="95"/>
-      <c r="I712" s="95"/>
-      <c r="J712" s="95"/>
-      <c r="K712" s="95"/>
-      <c r="L712" s="95"/>
-      <c r="M712" s="95"/>
-      <c r="N712" s="95"/>
-      <c r="O712" s="95"/>
-      <c r="P712" s="95"/>
-      <c r="Q712" s="95"/>
-      <c r="R712" s="95"/>
-      <c r="S712" s="95"/>
-      <c r="T712" s="95"/>
-      <c r="U712" s="95"/>
-      <c r="V712" s="95"/>
-      <c r="W712" s="95"/>
-      <c r="X712" s="95"/>
-      <c r="Y712" s="95"/>
-      <c r="Z712" s="95"/>
-      <c r="AA712" s="95"/>
-      <c r="AB712" s="95"/>
-      <c r="AC712" s="95"/>
-      <c r="AD712" s="95"/>
-      <c r="AE712" s="95"/>
-      <c r="AF712" s="95"/>
-      <c r="AG712" s="95"/>
-      <c r="AH712" s="95"/>
+      <c r="B712" s="90"/>
+      <c r="C712" s="90"/>
+      <c r="D712" s="90"/>
+      <c r="E712" s="90"/>
+      <c r="F712" s="90"/>
+      <c r="G712" s="90"/>
+      <c r="H712" s="90"/>
+      <c r="I712" s="90"/>
+      <c r="J712" s="90"/>
+      <c r="K712" s="90"/>
+      <c r="L712" s="90"/>
+      <c r="M712" s="90"/>
+      <c r="N712" s="90"/>
+      <c r="O712" s="90"/>
+      <c r="P712" s="90"/>
+      <c r="Q712" s="90"/>
+      <c r="R712" s="90"/>
+      <c r="S712" s="90"/>
+      <c r="T712" s="90"/>
+      <c r="U712" s="90"/>
+      <c r="V712" s="90"/>
+      <c r="W712" s="90"/>
+      <c r="X712" s="90"/>
+      <c r="Y712" s="90"/>
+      <c r="Z712" s="90"/>
+      <c r="AA712" s="90"/>
+      <c r="AB712" s="90"/>
+      <c r="AC712" s="90"/>
+      <c r="AD712" s="90"/>
+      <c r="AE712" s="90"/>
+      <c r="AF712" s="90"/>
+      <c r="AG712" s="90"/>
+      <c r="AH712" s="90"/>
     </row>
     <row r="887" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B887" s="95"/>
-      <c r="C887" s="95"/>
-      <c r="D887" s="95"/>
-      <c r="E887" s="95"/>
-      <c r="F887" s="95"/>
-      <c r="G887" s="95"/>
-      <c r="H887" s="95"/>
-      <c r="I887" s="95"/>
-      <c r="J887" s="95"/>
-      <c r="K887" s="95"/>
-      <c r="L887" s="95"/>
-      <c r="M887" s="95"/>
-      <c r="N887" s="95"/>
-      <c r="O887" s="95"/>
-      <c r="P887" s="95"/>
-      <c r="Q887" s="95"/>
-      <c r="R887" s="95"/>
-      <c r="S887" s="95"/>
-      <c r="T887" s="95"/>
-      <c r="U887" s="95"/>
-      <c r="V887" s="95"/>
-      <c r="W887" s="95"/>
-      <c r="X887" s="95"/>
-      <c r="Y887" s="95"/>
-      <c r="Z887" s="95"/>
-      <c r="AA887" s="95"/>
-      <c r="AB887" s="95"/>
-      <c r="AC887" s="95"/>
-      <c r="AD887" s="95"/>
-      <c r="AE887" s="95"/>
-      <c r="AF887" s="95"/>
-      <c r="AG887" s="95"/>
-      <c r="AH887" s="95"/>
+      <c r="B887" s="90"/>
+      <c r="C887" s="90"/>
+      <c r="D887" s="90"/>
+      <c r="E887" s="90"/>
+      <c r="F887" s="90"/>
+      <c r="G887" s="90"/>
+      <c r="H887" s="90"/>
+      <c r="I887" s="90"/>
+      <c r="J887" s="90"/>
+      <c r="K887" s="90"/>
+      <c r="L887" s="90"/>
+      <c r="M887" s="90"/>
+      <c r="N887" s="90"/>
+      <c r="O887" s="90"/>
+      <c r="P887" s="90"/>
+      <c r="Q887" s="90"/>
+      <c r="R887" s="90"/>
+      <c r="S887" s="90"/>
+      <c r="T887" s="90"/>
+      <c r="U887" s="90"/>
+      <c r="V887" s="90"/>
+      <c r="W887" s="90"/>
+      <c r="X887" s="90"/>
+      <c r="Y887" s="90"/>
+      <c r="Z887" s="90"/>
+      <c r="AA887" s="90"/>
+      <c r="AB887" s="90"/>
+      <c r="AC887" s="90"/>
+      <c r="AD887" s="90"/>
+      <c r="AE887" s="90"/>
+      <c r="AF887" s="90"/>
+      <c r="AG887" s="90"/>
+      <c r="AH887" s="90"/>
     </row>
     <row r="1100" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1100" s="95"/>
-      <c r="C1100" s="95"/>
-      <c r="D1100" s="95"/>
-      <c r="E1100" s="95"/>
-      <c r="F1100" s="95"/>
-      <c r="G1100" s="95"/>
-      <c r="H1100" s="95"/>
-      <c r="I1100" s="95"/>
-      <c r="J1100" s="95"/>
-      <c r="K1100" s="95"/>
-      <c r="L1100" s="95"/>
-      <c r="M1100" s="95"/>
-      <c r="N1100" s="95"/>
-      <c r="O1100" s="95"/>
-      <c r="P1100" s="95"/>
-      <c r="Q1100" s="95"/>
-      <c r="R1100" s="95"/>
-      <c r="S1100" s="95"/>
-      <c r="T1100" s="95"/>
-      <c r="U1100" s="95"/>
-      <c r="V1100" s="95"/>
-      <c r="W1100" s="95"/>
-      <c r="X1100" s="95"/>
-      <c r="Y1100" s="95"/>
-      <c r="Z1100" s="95"/>
-      <c r="AA1100" s="95"/>
-      <c r="AB1100" s="95"/>
-      <c r="AC1100" s="95"/>
-      <c r="AD1100" s="95"/>
-      <c r="AE1100" s="95"/>
-      <c r="AF1100" s="95"/>
-      <c r="AG1100" s="95"/>
-      <c r="AH1100" s="95"/>
+      <c r="B1100" s="90"/>
+      <c r="C1100" s="90"/>
+      <c r="D1100" s="90"/>
+      <c r="E1100" s="90"/>
+      <c r="F1100" s="90"/>
+      <c r="G1100" s="90"/>
+      <c r="H1100" s="90"/>
+      <c r="I1100" s="90"/>
+      <c r="J1100" s="90"/>
+      <c r="K1100" s="90"/>
+      <c r="L1100" s="90"/>
+      <c r="M1100" s="90"/>
+      <c r="N1100" s="90"/>
+      <c r="O1100" s="90"/>
+      <c r="P1100" s="90"/>
+      <c r="Q1100" s="90"/>
+      <c r="R1100" s="90"/>
+      <c r="S1100" s="90"/>
+      <c r="T1100" s="90"/>
+      <c r="U1100" s="90"/>
+      <c r="V1100" s="90"/>
+      <c r="W1100" s="90"/>
+      <c r="X1100" s="90"/>
+      <c r="Y1100" s="90"/>
+      <c r="Z1100" s="90"/>
+      <c r="AA1100" s="90"/>
+      <c r="AB1100" s="90"/>
+      <c r="AC1100" s="90"/>
+      <c r="AD1100" s="90"/>
+      <c r="AE1100" s="90"/>
+      <c r="AF1100" s="90"/>
+      <c r="AG1100" s="90"/>
+      <c r="AH1100" s="90"/>
     </row>
     <row r="1227" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1227" s="95"/>
-      <c r="C1227" s="95"/>
-      <c r="D1227" s="95"/>
-      <c r="E1227" s="95"/>
-      <c r="F1227" s="95"/>
-      <c r="G1227" s="95"/>
-      <c r="H1227" s="95"/>
-      <c r="I1227" s="95"/>
-      <c r="J1227" s="95"/>
-      <c r="K1227" s="95"/>
-      <c r="L1227" s="95"/>
-      <c r="M1227" s="95"/>
-      <c r="N1227" s="95"/>
-      <c r="O1227" s="95"/>
-      <c r="P1227" s="95"/>
-      <c r="Q1227" s="95"/>
-      <c r="R1227" s="95"/>
-      <c r="S1227" s="95"/>
-      <c r="T1227" s="95"/>
-      <c r="U1227" s="95"/>
-      <c r="V1227" s="95"/>
-      <c r="W1227" s="95"/>
-      <c r="X1227" s="95"/>
-      <c r="Y1227" s="95"/>
-      <c r="Z1227" s="95"/>
-      <c r="AA1227" s="95"/>
-      <c r="AB1227" s="95"/>
-      <c r="AC1227" s="95"/>
-      <c r="AD1227" s="95"/>
-      <c r="AE1227" s="95"/>
-      <c r="AF1227" s="95"/>
-      <c r="AG1227" s="95"/>
-      <c r="AH1227" s="95"/>
+      <c r="B1227" s="90"/>
+      <c r="C1227" s="90"/>
+      <c r="D1227" s="90"/>
+      <c r="E1227" s="90"/>
+      <c r="F1227" s="90"/>
+      <c r="G1227" s="90"/>
+      <c r="H1227" s="90"/>
+      <c r="I1227" s="90"/>
+      <c r="J1227" s="90"/>
+      <c r="K1227" s="90"/>
+      <c r="L1227" s="90"/>
+      <c r="M1227" s="90"/>
+      <c r="N1227" s="90"/>
+      <c r="O1227" s="90"/>
+      <c r="P1227" s="90"/>
+      <c r="Q1227" s="90"/>
+      <c r="R1227" s="90"/>
+      <c r="S1227" s="90"/>
+      <c r="T1227" s="90"/>
+      <c r="U1227" s="90"/>
+      <c r="V1227" s="90"/>
+      <c r="W1227" s="90"/>
+      <c r="X1227" s="90"/>
+      <c r="Y1227" s="90"/>
+      <c r="Z1227" s="90"/>
+      <c r="AA1227" s="90"/>
+      <c r="AB1227" s="90"/>
+      <c r="AC1227" s="90"/>
+      <c r="AD1227" s="90"/>
+      <c r="AE1227" s="90"/>
+      <c r="AF1227" s="90"/>
+      <c r="AG1227" s="90"/>
+      <c r="AH1227" s="90"/>
     </row>
     <row r="1390" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1390" s="95"/>
-      <c r="C1390" s="95"/>
-      <c r="D1390" s="95"/>
-      <c r="E1390" s="95"/>
-      <c r="F1390" s="95"/>
-      <c r="G1390" s="95"/>
-      <c r="H1390" s="95"/>
-      <c r="I1390" s="95"/>
-      <c r="J1390" s="95"/>
-      <c r="K1390" s="95"/>
-      <c r="L1390" s="95"/>
-      <c r="M1390" s="95"/>
-      <c r="N1390" s="95"/>
-      <c r="O1390" s="95"/>
-      <c r="P1390" s="95"/>
-      <c r="Q1390" s="95"/>
-      <c r="R1390" s="95"/>
-      <c r="S1390" s="95"/>
-      <c r="T1390" s="95"/>
-      <c r="U1390" s="95"/>
-      <c r="V1390" s="95"/>
-      <c r="W1390" s="95"/>
-      <c r="X1390" s="95"/>
-      <c r="Y1390" s="95"/>
-      <c r="Z1390" s="95"/>
-      <c r="AA1390" s="95"/>
-      <c r="AB1390" s="95"/>
-      <c r="AC1390" s="95"/>
-      <c r="AD1390" s="95"/>
-      <c r="AE1390" s="95"/>
-      <c r="AF1390" s="95"/>
-      <c r="AG1390" s="95"/>
-      <c r="AH1390" s="95"/>
+      <c r="B1390" s="90"/>
+      <c r="C1390" s="90"/>
+      <c r="D1390" s="90"/>
+      <c r="E1390" s="90"/>
+      <c r="F1390" s="90"/>
+      <c r="G1390" s="90"/>
+      <c r="H1390" s="90"/>
+      <c r="I1390" s="90"/>
+      <c r="J1390" s="90"/>
+      <c r="K1390" s="90"/>
+      <c r="L1390" s="90"/>
+      <c r="M1390" s="90"/>
+      <c r="N1390" s="90"/>
+      <c r="O1390" s="90"/>
+      <c r="P1390" s="90"/>
+      <c r="Q1390" s="90"/>
+      <c r="R1390" s="90"/>
+      <c r="S1390" s="90"/>
+      <c r="T1390" s="90"/>
+      <c r="U1390" s="90"/>
+      <c r="V1390" s="90"/>
+      <c r="W1390" s="90"/>
+      <c r="X1390" s="90"/>
+      <c r="Y1390" s="90"/>
+      <c r="Z1390" s="90"/>
+      <c r="AA1390" s="90"/>
+      <c r="AB1390" s="90"/>
+      <c r="AC1390" s="90"/>
+      <c r="AD1390" s="90"/>
+      <c r="AE1390" s="90"/>
+      <c r="AF1390" s="90"/>
+      <c r="AG1390" s="90"/>
+      <c r="AH1390" s="90"/>
     </row>
     <row r="1502" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1502" s="95"/>
-      <c r="C1502" s="95"/>
-      <c r="D1502" s="95"/>
-      <c r="E1502" s="95"/>
-      <c r="F1502" s="95"/>
-      <c r="G1502" s="95"/>
-      <c r="H1502" s="95"/>
-      <c r="I1502" s="95"/>
-      <c r="J1502" s="95"/>
-      <c r="K1502" s="95"/>
-      <c r="L1502" s="95"/>
-      <c r="M1502" s="95"/>
-      <c r="N1502" s="95"/>
-      <c r="O1502" s="95"/>
-      <c r="P1502" s="95"/>
-      <c r="Q1502" s="95"/>
-      <c r="R1502" s="95"/>
-      <c r="S1502" s="95"/>
-      <c r="T1502" s="95"/>
-      <c r="U1502" s="95"/>
-      <c r="V1502" s="95"/>
-      <c r="W1502" s="95"/>
-      <c r="X1502" s="95"/>
-      <c r="Y1502" s="95"/>
-      <c r="Z1502" s="95"/>
-      <c r="AA1502" s="95"/>
-      <c r="AB1502" s="95"/>
-      <c r="AC1502" s="95"/>
-      <c r="AD1502" s="95"/>
-      <c r="AE1502" s="95"/>
-      <c r="AF1502" s="95"/>
-      <c r="AG1502" s="95"/>
-      <c r="AH1502" s="95"/>
+      <c r="B1502" s="90"/>
+      <c r="C1502" s="90"/>
+      <c r="D1502" s="90"/>
+      <c r="E1502" s="90"/>
+      <c r="F1502" s="90"/>
+      <c r="G1502" s="90"/>
+      <c r="H1502" s="90"/>
+      <c r="I1502" s="90"/>
+      <c r="J1502" s="90"/>
+      <c r="K1502" s="90"/>
+      <c r="L1502" s="90"/>
+      <c r="M1502" s="90"/>
+      <c r="N1502" s="90"/>
+      <c r="O1502" s="90"/>
+      <c r="P1502" s="90"/>
+      <c r="Q1502" s="90"/>
+      <c r="R1502" s="90"/>
+      <c r="S1502" s="90"/>
+      <c r="T1502" s="90"/>
+      <c r="U1502" s="90"/>
+      <c r="V1502" s="90"/>
+      <c r="W1502" s="90"/>
+      <c r="X1502" s="90"/>
+      <c r="Y1502" s="90"/>
+      <c r="Z1502" s="90"/>
+      <c r="AA1502" s="90"/>
+      <c r="AB1502" s="90"/>
+      <c r="AC1502" s="90"/>
+      <c r="AD1502" s="90"/>
+      <c r="AE1502" s="90"/>
+      <c r="AF1502" s="90"/>
+      <c r="AG1502" s="90"/>
+      <c r="AH1502" s="90"/>
     </row>
     <row r="1604" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1604" s="95"/>
-      <c r="C1604" s="95"/>
-      <c r="D1604" s="95"/>
-      <c r="E1604" s="95"/>
-      <c r="F1604" s="95"/>
-      <c r="G1604" s="95"/>
-      <c r="H1604" s="95"/>
-      <c r="I1604" s="95"/>
-      <c r="J1604" s="95"/>
-      <c r="K1604" s="95"/>
-      <c r="L1604" s="95"/>
-      <c r="M1604" s="95"/>
-      <c r="N1604" s="95"/>
-      <c r="O1604" s="95"/>
-      <c r="P1604" s="95"/>
-      <c r="Q1604" s="95"/>
-      <c r="R1604" s="95"/>
-      <c r="S1604" s="95"/>
-      <c r="T1604" s="95"/>
-      <c r="U1604" s="95"/>
-      <c r="V1604" s="95"/>
-      <c r="W1604" s="95"/>
-      <c r="X1604" s="95"/>
-      <c r="Y1604" s="95"/>
-      <c r="Z1604" s="95"/>
-      <c r="AA1604" s="95"/>
-      <c r="AB1604" s="95"/>
-      <c r="AC1604" s="95"/>
-      <c r="AD1604" s="95"/>
-      <c r="AE1604" s="95"/>
-      <c r="AF1604" s="95"/>
-      <c r="AG1604" s="95"/>
-      <c r="AH1604" s="95"/>
+      <c r="B1604" s="90"/>
+      <c r="C1604" s="90"/>
+      <c r="D1604" s="90"/>
+      <c r="E1604" s="90"/>
+      <c r="F1604" s="90"/>
+      <c r="G1604" s="90"/>
+      <c r="H1604" s="90"/>
+      <c r="I1604" s="90"/>
+      <c r="J1604" s="90"/>
+      <c r="K1604" s="90"/>
+      <c r="L1604" s="90"/>
+      <c r="M1604" s="90"/>
+      <c r="N1604" s="90"/>
+      <c r="O1604" s="90"/>
+      <c r="P1604" s="90"/>
+      <c r="Q1604" s="90"/>
+      <c r="R1604" s="90"/>
+      <c r="S1604" s="90"/>
+      <c r="T1604" s="90"/>
+      <c r="U1604" s="90"/>
+      <c r="V1604" s="90"/>
+      <c r="W1604" s="90"/>
+      <c r="X1604" s="90"/>
+      <c r="Y1604" s="90"/>
+      <c r="Z1604" s="90"/>
+      <c r="AA1604" s="90"/>
+      <c r="AB1604" s="90"/>
+      <c r="AC1604" s="90"/>
+      <c r="AD1604" s="90"/>
+      <c r="AE1604" s="90"/>
+      <c r="AF1604" s="90"/>
+      <c r="AG1604" s="90"/>
+      <c r="AH1604" s="90"/>
     </row>
     <row r="1698" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1698" s="95"/>
-      <c r="C1698" s="95"/>
-      <c r="D1698" s="95"/>
-      <c r="E1698" s="95"/>
-      <c r="F1698" s="95"/>
-      <c r="G1698" s="95"/>
-      <c r="H1698" s="95"/>
-      <c r="I1698" s="95"/>
-      <c r="J1698" s="95"/>
-      <c r="K1698" s="95"/>
-      <c r="L1698" s="95"/>
-      <c r="M1698" s="95"/>
-      <c r="N1698" s="95"/>
-      <c r="O1698" s="95"/>
-      <c r="P1698" s="95"/>
-      <c r="Q1698" s="95"/>
-      <c r="R1698" s="95"/>
-      <c r="S1698" s="95"/>
-      <c r="T1698" s="95"/>
-      <c r="U1698" s="95"/>
-      <c r="V1698" s="95"/>
-      <c r="W1698" s="95"/>
-      <c r="X1698" s="95"/>
-      <c r="Y1698" s="95"/>
-      <c r="Z1698" s="95"/>
-      <c r="AA1698" s="95"/>
-      <c r="AB1698" s="95"/>
-      <c r="AC1698" s="95"/>
-      <c r="AD1698" s="95"/>
-      <c r="AE1698" s="95"/>
-      <c r="AF1698" s="95"/>
-      <c r="AG1698" s="95"/>
-      <c r="AH1698" s="95"/>
+      <c r="B1698" s="90"/>
+      <c r="C1698" s="90"/>
+      <c r="D1698" s="90"/>
+      <c r="E1698" s="90"/>
+      <c r="F1698" s="90"/>
+      <c r="G1698" s="90"/>
+      <c r="H1698" s="90"/>
+      <c r="I1698" s="90"/>
+      <c r="J1698" s="90"/>
+      <c r="K1698" s="90"/>
+      <c r="L1698" s="90"/>
+      <c r="M1698" s="90"/>
+      <c r="N1698" s="90"/>
+      <c r="O1698" s="90"/>
+      <c r="P1698" s="90"/>
+      <c r="Q1698" s="90"/>
+      <c r="R1698" s="90"/>
+      <c r="S1698" s="90"/>
+      <c r="T1698" s="90"/>
+      <c r="U1698" s="90"/>
+      <c r="V1698" s="90"/>
+      <c r="W1698" s="90"/>
+      <c r="X1698" s="90"/>
+      <c r="Y1698" s="90"/>
+      <c r="Z1698" s="90"/>
+      <c r="AA1698" s="90"/>
+      <c r="AB1698" s="90"/>
+      <c r="AC1698" s="90"/>
+      <c r="AD1698" s="90"/>
+      <c r="AE1698" s="90"/>
+      <c r="AF1698" s="90"/>
+      <c r="AG1698" s="90"/>
+      <c r="AH1698" s="90"/>
     </row>
     <row r="1945" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1945" s="95"/>
-      <c r="C1945" s="95"/>
-      <c r="D1945" s="95"/>
-      <c r="E1945" s="95"/>
-      <c r="F1945" s="95"/>
-      <c r="G1945" s="95"/>
-      <c r="H1945" s="95"/>
-      <c r="I1945" s="95"/>
-      <c r="J1945" s="95"/>
-      <c r="K1945" s="95"/>
-      <c r="L1945" s="95"/>
-      <c r="M1945" s="95"/>
-      <c r="N1945" s="95"/>
-      <c r="O1945" s="95"/>
-      <c r="P1945" s="95"/>
-      <c r="Q1945" s="95"/>
-      <c r="R1945" s="95"/>
-      <c r="S1945" s="95"/>
-      <c r="T1945" s="95"/>
-      <c r="U1945" s="95"/>
-      <c r="V1945" s="95"/>
-      <c r="W1945" s="95"/>
-      <c r="X1945" s="95"/>
-      <c r="Y1945" s="95"/>
-      <c r="Z1945" s="95"/>
-      <c r="AA1945" s="95"/>
-      <c r="AB1945" s="95"/>
-      <c r="AC1945" s="95"/>
-      <c r="AD1945" s="95"/>
-      <c r="AE1945" s="95"/>
-      <c r="AF1945" s="95"/>
-      <c r="AG1945" s="95"/>
-      <c r="AH1945" s="95"/>
+      <c r="B1945" s="90"/>
+      <c r="C1945" s="90"/>
+      <c r="D1945" s="90"/>
+      <c r="E1945" s="90"/>
+      <c r="F1945" s="90"/>
+      <c r="G1945" s="90"/>
+      <c r="H1945" s="90"/>
+      <c r="I1945" s="90"/>
+      <c r="J1945" s="90"/>
+      <c r="K1945" s="90"/>
+      <c r="L1945" s="90"/>
+      <c r="M1945" s="90"/>
+      <c r="N1945" s="90"/>
+      <c r="O1945" s="90"/>
+      <c r="P1945" s="90"/>
+      <c r="Q1945" s="90"/>
+      <c r="R1945" s="90"/>
+      <c r="S1945" s="90"/>
+      <c r="T1945" s="90"/>
+      <c r="U1945" s="90"/>
+      <c r="V1945" s="90"/>
+      <c r="W1945" s="90"/>
+      <c r="X1945" s="90"/>
+      <c r="Y1945" s="90"/>
+      <c r="Z1945" s="90"/>
+      <c r="AA1945" s="90"/>
+      <c r="AB1945" s="90"/>
+      <c r="AC1945" s="90"/>
+      <c r="AD1945" s="90"/>
+      <c r="AE1945" s="90"/>
+      <c r="AF1945" s="90"/>
+      <c r="AG1945" s="90"/>
+      <c r="AH1945" s="90"/>
     </row>
     <row r="2031" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2031" s="95"/>
-      <c r="C2031" s="95"/>
-      <c r="D2031" s="95"/>
-      <c r="E2031" s="95"/>
-      <c r="F2031" s="95"/>
-      <c r="G2031" s="95"/>
-      <c r="H2031" s="95"/>
-      <c r="I2031" s="95"/>
-      <c r="J2031" s="95"/>
-      <c r="K2031" s="95"/>
-      <c r="L2031" s="95"/>
-      <c r="M2031" s="95"/>
-      <c r="N2031" s="95"/>
-      <c r="O2031" s="95"/>
-      <c r="P2031" s="95"/>
-      <c r="Q2031" s="95"/>
-      <c r="R2031" s="95"/>
-      <c r="S2031" s="95"/>
-      <c r="T2031" s="95"/>
-      <c r="U2031" s="95"/>
-      <c r="V2031" s="95"/>
-      <c r="W2031" s="95"/>
-      <c r="X2031" s="95"/>
-      <c r="Y2031" s="95"/>
-      <c r="Z2031" s="95"/>
-      <c r="AA2031" s="95"/>
-      <c r="AB2031" s="95"/>
-      <c r="AC2031" s="95"/>
-      <c r="AD2031" s="95"/>
-      <c r="AE2031" s="95"/>
-      <c r="AF2031" s="95"/>
-      <c r="AG2031" s="95"/>
-      <c r="AH2031" s="95"/>
+      <c r="B2031" s="90"/>
+      <c r="C2031" s="90"/>
+      <c r="D2031" s="90"/>
+      <c r="E2031" s="90"/>
+      <c r="F2031" s="90"/>
+      <c r="G2031" s="90"/>
+      <c r="H2031" s="90"/>
+      <c r="I2031" s="90"/>
+      <c r="J2031" s="90"/>
+      <c r="K2031" s="90"/>
+      <c r="L2031" s="90"/>
+      <c r="M2031" s="90"/>
+      <c r="N2031" s="90"/>
+      <c r="O2031" s="90"/>
+      <c r="P2031" s="90"/>
+      <c r="Q2031" s="90"/>
+      <c r="R2031" s="90"/>
+      <c r="S2031" s="90"/>
+      <c r="T2031" s="90"/>
+      <c r="U2031" s="90"/>
+      <c r="V2031" s="90"/>
+      <c r="W2031" s="90"/>
+      <c r="X2031" s="90"/>
+      <c r="Y2031" s="90"/>
+      <c r="Z2031" s="90"/>
+      <c r="AA2031" s="90"/>
+      <c r="AB2031" s="90"/>
+      <c r="AC2031" s="90"/>
+      <c r="AD2031" s="90"/>
+      <c r="AE2031" s="90"/>
+      <c r="AF2031" s="90"/>
+      <c r="AG2031" s="90"/>
+      <c r="AH2031" s="90"/>
     </row>
     <row r="2153" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2153" s="95"/>
-      <c r="C2153" s="95"/>
-      <c r="D2153" s="95"/>
-      <c r="E2153" s="95"/>
-      <c r="F2153" s="95"/>
-      <c r="G2153" s="95"/>
-      <c r="H2153" s="95"/>
-      <c r="I2153" s="95"/>
-      <c r="J2153" s="95"/>
-      <c r="K2153" s="95"/>
-      <c r="L2153" s="95"/>
-      <c r="M2153" s="95"/>
-      <c r="N2153" s="95"/>
-      <c r="O2153" s="95"/>
-      <c r="P2153" s="95"/>
-      <c r="Q2153" s="95"/>
-      <c r="R2153" s="95"/>
-      <c r="S2153" s="95"/>
-      <c r="T2153" s="95"/>
-      <c r="U2153" s="95"/>
-      <c r="V2153" s="95"/>
-      <c r="W2153" s="95"/>
-      <c r="X2153" s="95"/>
-      <c r="Y2153" s="95"/>
-      <c r="Z2153" s="95"/>
-      <c r="AA2153" s="95"/>
-      <c r="AB2153" s="95"/>
-      <c r="AC2153" s="95"/>
-      <c r="AD2153" s="95"/>
-      <c r="AE2153" s="95"/>
-      <c r="AF2153" s="95"/>
-      <c r="AG2153" s="95"/>
-      <c r="AH2153" s="95"/>
+      <c r="B2153" s="90"/>
+      <c r="C2153" s="90"/>
+      <c r="D2153" s="90"/>
+      <c r="E2153" s="90"/>
+      <c r="F2153" s="90"/>
+      <c r="G2153" s="90"/>
+      <c r="H2153" s="90"/>
+      <c r="I2153" s="90"/>
+      <c r="J2153" s="90"/>
+      <c r="K2153" s="90"/>
+      <c r="L2153" s="90"/>
+      <c r="M2153" s="90"/>
+      <c r="N2153" s="90"/>
+      <c r="O2153" s="90"/>
+      <c r="P2153" s="90"/>
+      <c r="Q2153" s="90"/>
+      <c r="R2153" s="90"/>
+      <c r="S2153" s="90"/>
+      <c r="T2153" s="90"/>
+      <c r="U2153" s="90"/>
+      <c r="V2153" s="90"/>
+      <c r="W2153" s="90"/>
+      <c r="X2153" s="90"/>
+      <c r="Y2153" s="90"/>
+      <c r="Z2153" s="90"/>
+      <c r="AA2153" s="90"/>
+      <c r="AB2153" s="90"/>
+      <c r="AC2153" s="90"/>
+      <c r="AD2153" s="90"/>
+      <c r="AE2153" s="90"/>
+      <c r="AF2153" s="90"/>
+      <c r="AG2153" s="90"/>
+      <c r="AH2153" s="90"/>
     </row>
     <row r="2317" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2317" s="95"/>
-      <c r="C2317" s="95"/>
-      <c r="D2317" s="95"/>
-      <c r="E2317" s="95"/>
-      <c r="F2317" s="95"/>
-      <c r="G2317" s="95"/>
-      <c r="H2317" s="95"/>
-      <c r="I2317" s="95"/>
-      <c r="J2317" s="95"/>
-      <c r="K2317" s="95"/>
-      <c r="L2317" s="95"/>
-      <c r="M2317" s="95"/>
-      <c r="N2317" s="95"/>
-      <c r="O2317" s="95"/>
-      <c r="P2317" s="95"/>
-      <c r="Q2317" s="95"/>
-      <c r="R2317" s="95"/>
-      <c r="S2317" s="95"/>
-      <c r="T2317" s="95"/>
-      <c r="U2317" s="95"/>
-      <c r="V2317" s="95"/>
-      <c r="W2317" s="95"/>
-      <c r="X2317" s="95"/>
-      <c r="Y2317" s="95"/>
-      <c r="Z2317" s="95"/>
-      <c r="AA2317" s="95"/>
-      <c r="AB2317" s="95"/>
-      <c r="AC2317" s="95"/>
-      <c r="AD2317" s="95"/>
-      <c r="AE2317" s="95"/>
-      <c r="AF2317" s="95"/>
-      <c r="AG2317" s="95"/>
-      <c r="AH2317" s="95"/>
+      <c r="B2317" s="90"/>
+      <c r="C2317" s="90"/>
+      <c r="D2317" s="90"/>
+      <c r="E2317" s="90"/>
+      <c r="F2317" s="90"/>
+      <c r="G2317" s="90"/>
+      <c r="H2317" s="90"/>
+      <c r="I2317" s="90"/>
+      <c r="J2317" s="90"/>
+      <c r="K2317" s="90"/>
+      <c r="L2317" s="90"/>
+      <c r="M2317" s="90"/>
+      <c r="N2317" s="90"/>
+      <c r="O2317" s="90"/>
+      <c r="P2317" s="90"/>
+      <c r="Q2317" s="90"/>
+      <c r="R2317" s="90"/>
+      <c r="S2317" s="90"/>
+      <c r="T2317" s="90"/>
+      <c r="U2317" s="90"/>
+      <c r="V2317" s="90"/>
+      <c r="W2317" s="90"/>
+      <c r="X2317" s="90"/>
+      <c r="Y2317" s="90"/>
+      <c r="Z2317" s="90"/>
+      <c r="AA2317" s="90"/>
+      <c r="AB2317" s="90"/>
+      <c r="AC2317" s="90"/>
+      <c r="AD2317" s="90"/>
+      <c r="AE2317" s="90"/>
+      <c r="AF2317" s="90"/>
+      <c r="AG2317" s="90"/>
+      <c r="AH2317" s="90"/>
     </row>
     <row r="2419" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2419" s="95"/>
-      <c r="C2419" s="95"/>
-      <c r="D2419" s="95"/>
-      <c r="E2419" s="95"/>
-      <c r="F2419" s="95"/>
-      <c r="G2419" s="95"/>
-      <c r="H2419" s="95"/>
-      <c r="I2419" s="95"/>
-      <c r="J2419" s="95"/>
-      <c r="K2419" s="95"/>
-      <c r="L2419" s="95"/>
-      <c r="M2419" s="95"/>
-      <c r="N2419" s="95"/>
-      <c r="O2419" s="95"/>
-      <c r="P2419" s="95"/>
-      <c r="Q2419" s="95"/>
-      <c r="R2419" s="95"/>
-      <c r="S2419" s="95"/>
-      <c r="T2419" s="95"/>
-      <c r="U2419" s="95"/>
-      <c r="V2419" s="95"/>
-      <c r="W2419" s="95"/>
-      <c r="X2419" s="95"/>
-      <c r="Y2419" s="95"/>
-      <c r="Z2419" s="95"/>
-      <c r="AA2419" s="95"/>
-      <c r="AB2419" s="95"/>
-      <c r="AC2419" s="95"/>
-      <c r="AD2419" s="95"/>
-      <c r="AE2419" s="95"/>
-      <c r="AF2419" s="95"/>
-      <c r="AG2419" s="95"/>
-      <c r="AH2419" s="95"/>
+      <c r="B2419" s="90"/>
+      <c r="C2419" s="90"/>
+      <c r="D2419" s="90"/>
+      <c r="E2419" s="90"/>
+      <c r="F2419" s="90"/>
+      <c r="G2419" s="90"/>
+      <c r="H2419" s="90"/>
+      <c r="I2419" s="90"/>
+      <c r="J2419" s="90"/>
+      <c r="K2419" s="90"/>
+      <c r="L2419" s="90"/>
+      <c r="M2419" s="90"/>
+      <c r="N2419" s="90"/>
+      <c r="O2419" s="90"/>
+      <c r="P2419" s="90"/>
+      <c r="Q2419" s="90"/>
+      <c r="R2419" s="90"/>
+      <c r="S2419" s="90"/>
+      <c r="T2419" s="90"/>
+      <c r="U2419" s="90"/>
+      <c r="V2419" s="90"/>
+      <c r="W2419" s="90"/>
+      <c r="X2419" s="90"/>
+      <c r="Y2419" s="90"/>
+      <c r="Z2419" s="90"/>
+      <c r="AA2419" s="90"/>
+      <c r="AB2419" s="90"/>
+      <c r="AC2419" s="90"/>
+      <c r="AD2419" s="90"/>
+      <c r="AE2419" s="90"/>
+      <c r="AF2419" s="90"/>
+      <c r="AG2419" s="90"/>
+      <c r="AH2419" s="90"/>
     </row>
     <row r="2509" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2509" s="95"/>
-      <c r="C2509" s="95"/>
-      <c r="D2509" s="95"/>
-      <c r="E2509" s="95"/>
-      <c r="F2509" s="95"/>
-      <c r="G2509" s="95"/>
-      <c r="H2509" s="95"/>
-      <c r="I2509" s="95"/>
-      <c r="J2509" s="95"/>
-      <c r="K2509" s="95"/>
-      <c r="L2509" s="95"/>
-      <c r="M2509" s="95"/>
-      <c r="N2509" s="95"/>
-      <c r="O2509" s="95"/>
-      <c r="P2509" s="95"/>
-      <c r="Q2509" s="95"/>
-      <c r="R2509" s="95"/>
-      <c r="S2509" s="95"/>
-      <c r="T2509" s="95"/>
-      <c r="U2509" s="95"/>
-      <c r="V2509" s="95"/>
-      <c r="W2509" s="95"/>
-      <c r="X2509" s="95"/>
-      <c r="Y2509" s="95"/>
-      <c r="Z2509" s="95"/>
-      <c r="AA2509" s="95"/>
-      <c r="AB2509" s="95"/>
-      <c r="AC2509" s="95"/>
-      <c r="AD2509" s="95"/>
-      <c r="AE2509" s="95"/>
-      <c r="AF2509" s="95"/>
-      <c r="AG2509" s="95"/>
-      <c r="AH2509" s="95"/>
+      <c r="B2509" s="90"/>
+      <c r="C2509" s="90"/>
+      <c r="D2509" s="90"/>
+      <c r="E2509" s="90"/>
+      <c r="F2509" s="90"/>
+      <c r="G2509" s="90"/>
+      <c r="H2509" s="90"/>
+      <c r="I2509" s="90"/>
+      <c r="J2509" s="90"/>
+      <c r="K2509" s="90"/>
+      <c r="L2509" s="90"/>
+      <c r="M2509" s="90"/>
+      <c r="N2509" s="90"/>
+      <c r="O2509" s="90"/>
+      <c r="P2509" s="90"/>
+      <c r="Q2509" s="90"/>
+      <c r="R2509" s="90"/>
+      <c r="S2509" s="90"/>
+      <c r="T2509" s="90"/>
+      <c r="U2509" s="90"/>
+      <c r="V2509" s="90"/>
+      <c r="W2509" s="90"/>
+      <c r="X2509" s="90"/>
+      <c r="Y2509" s="90"/>
+      <c r="Z2509" s="90"/>
+      <c r="AA2509" s="90"/>
+      <c r="AB2509" s="90"/>
+      <c r="AC2509" s="90"/>
+      <c r="AD2509" s="90"/>
+      <c r="AE2509" s="90"/>
+      <c r="AF2509" s="90"/>
+      <c r="AG2509" s="90"/>
+      <c r="AH2509" s="90"/>
     </row>
     <row r="2598" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2598" s="95"/>
-      <c r="C2598" s="95"/>
-      <c r="D2598" s="95"/>
-      <c r="E2598" s="95"/>
-      <c r="F2598" s="95"/>
-      <c r="G2598" s="95"/>
-      <c r="H2598" s="95"/>
-      <c r="I2598" s="95"/>
-      <c r="J2598" s="95"/>
-      <c r="K2598" s="95"/>
-      <c r="L2598" s="95"/>
-      <c r="M2598" s="95"/>
-      <c r="N2598" s="95"/>
-      <c r="O2598" s="95"/>
-      <c r="P2598" s="95"/>
-      <c r="Q2598" s="95"/>
-      <c r="R2598" s="95"/>
-      <c r="S2598" s="95"/>
-      <c r="T2598" s="95"/>
-      <c r="U2598" s="95"/>
-      <c r="V2598" s="95"/>
-      <c r="W2598" s="95"/>
-      <c r="X2598" s="95"/>
-      <c r="Y2598" s="95"/>
-      <c r="Z2598" s="95"/>
-      <c r="AA2598" s="95"/>
-      <c r="AB2598" s="95"/>
-      <c r="AC2598" s="95"/>
-      <c r="AD2598" s="95"/>
-      <c r="AE2598" s="95"/>
-      <c r="AF2598" s="95"/>
-      <c r="AG2598" s="95"/>
-      <c r="AH2598" s="95"/>
+      <c r="B2598" s="90"/>
+      <c r="C2598" s="90"/>
+      <c r="D2598" s="90"/>
+      <c r="E2598" s="90"/>
+      <c r="F2598" s="90"/>
+      <c r="G2598" s="90"/>
+      <c r="H2598" s="90"/>
+      <c r="I2598" s="90"/>
+      <c r="J2598" s="90"/>
+      <c r="K2598" s="90"/>
+      <c r="L2598" s="90"/>
+      <c r="M2598" s="90"/>
+      <c r="N2598" s="90"/>
+      <c r="O2598" s="90"/>
+      <c r="P2598" s="90"/>
+      <c r="Q2598" s="90"/>
+      <c r="R2598" s="90"/>
+      <c r="S2598" s="90"/>
+      <c r="T2598" s="90"/>
+      <c r="U2598" s="90"/>
+      <c r="V2598" s="90"/>
+      <c r="W2598" s="90"/>
+      <c r="X2598" s="90"/>
+      <c r="Y2598" s="90"/>
+      <c r="Z2598" s="90"/>
+      <c r="AA2598" s="90"/>
+      <c r="AB2598" s="90"/>
+      <c r="AC2598" s="90"/>
+      <c r="AD2598" s="90"/>
+      <c r="AE2598" s="90"/>
+      <c r="AF2598" s="90"/>
+      <c r="AG2598" s="90"/>
+      <c r="AH2598" s="90"/>
     </row>
     <row r="2719" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2719" s="95"/>
-      <c r="C2719" s="95"/>
-      <c r="D2719" s="95"/>
-      <c r="E2719" s="95"/>
-      <c r="F2719" s="95"/>
-      <c r="G2719" s="95"/>
-      <c r="H2719" s="95"/>
-      <c r="I2719" s="95"/>
-      <c r="J2719" s="95"/>
-      <c r="K2719" s="95"/>
-      <c r="L2719" s="95"/>
-      <c r="M2719" s="95"/>
-      <c r="N2719" s="95"/>
-      <c r="O2719" s="95"/>
-      <c r="P2719" s="95"/>
-      <c r="Q2719" s="95"/>
-      <c r="R2719" s="95"/>
-      <c r="S2719" s="95"/>
-      <c r="T2719" s="95"/>
-      <c r="U2719" s="95"/>
-      <c r="V2719" s="95"/>
-      <c r="W2719" s="95"/>
-      <c r="X2719" s="95"/>
-      <c r="Y2719" s="95"/>
-      <c r="Z2719" s="95"/>
-      <c r="AA2719" s="95"/>
-      <c r="AB2719" s="95"/>
-      <c r="AC2719" s="95"/>
-      <c r="AD2719" s="95"/>
-      <c r="AE2719" s="95"/>
-      <c r="AF2719" s="95"/>
-      <c r="AG2719" s="95"/>
-      <c r="AH2719" s="95"/>
+      <c r="B2719" s="90"/>
+      <c r="C2719" s="90"/>
+      <c r="D2719" s="90"/>
+      <c r="E2719" s="90"/>
+      <c r="F2719" s="90"/>
+      <c r="G2719" s="90"/>
+      <c r="H2719" s="90"/>
+      <c r="I2719" s="90"/>
+      <c r="J2719" s="90"/>
+      <c r="K2719" s="90"/>
+      <c r="L2719" s="90"/>
+      <c r="M2719" s="90"/>
+      <c r="N2719" s="90"/>
+      <c r="O2719" s="90"/>
+      <c r="P2719" s="90"/>
+      <c r="Q2719" s="90"/>
+      <c r="R2719" s="90"/>
+      <c r="S2719" s="90"/>
+      <c r="T2719" s="90"/>
+      <c r="U2719" s="90"/>
+      <c r="V2719" s="90"/>
+      <c r="W2719" s="90"/>
+      <c r="X2719" s="90"/>
+      <c r="Y2719" s="90"/>
+      <c r="Z2719" s="90"/>
+      <c r="AA2719" s="90"/>
+      <c r="AB2719" s="90"/>
+      <c r="AC2719" s="90"/>
+      <c r="AD2719" s="90"/>
+      <c r="AE2719" s="90"/>
+      <c r="AF2719" s="90"/>
+      <c r="AG2719" s="90"/>
+      <c r="AH2719" s="90"/>
     </row>
     <row r="2837" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2837" s="95"/>
-      <c r="C2837" s="95"/>
-      <c r="D2837" s="95"/>
-      <c r="E2837" s="95"/>
-      <c r="F2837" s="95"/>
-      <c r="G2837" s="95"/>
-      <c r="H2837" s="95"/>
-      <c r="I2837" s="95"/>
-      <c r="J2837" s="95"/>
-      <c r="K2837" s="95"/>
-      <c r="L2837" s="95"/>
-      <c r="M2837" s="95"/>
-      <c r="N2837" s="95"/>
-      <c r="O2837" s="95"/>
-      <c r="P2837" s="95"/>
-      <c r="Q2837" s="95"/>
-      <c r="R2837" s="95"/>
-      <c r="S2837" s="95"/>
-      <c r="T2837" s="95"/>
-      <c r="U2837" s="95"/>
-      <c r="V2837" s="95"/>
-      <c r="W2837" s="95"/>
-      <c r="X2837" s="95"/>
-      <c r="Y2837" s="95"/>
-      <c r="Z2837" s="95"/>
-      <c r="AA2837" s="95"/>
-      <c r="AB2837" s="95"/>
-      <c r="AC2837" s="95"/>
-      <c r="AD2837" s="95"/>
-      <c r="AE2837" s="95"/>
-      <c r="AF2837" s="95"/>
-      <c r="AG2837" s="95"/>
-      <c r="AH2837" s="95"/>
+      <c r="B2837" s="90"/>
+      <c r="C2837" s="90"/>
+      <c r="D2837" s="90"/>
+      <c r="E2837" s="90"/>
+      <c r="F2837" s="90"/>
+      <c r="G2837" s="90"/>
+      <c r="H2837" s="90"/>
+      <c r="I2837" s="90"/>
+      <c r="J2837" s="90"/>
+      <c r="K2837" s="90"/>
+      <c r="L2837" s="90"/>
+      <c r="M2837" s="90"/>
+      <c r="N2837" s="90"/>
+      <c r="O2837" s="90"/>
+      <c r="P2837" s="90"/>
+      <c r="Q2837" s="90"/>
+      <c r="R2837" s="90"/>
+      <c r="S2837" s="90"/>
+      <c r="T2837" s="90"/>
+      <c r="U2837" s="90"/>
+      <c r="V2837" s="90"/>
+      <c r="W2837" s="90"/>
+      <c r="X2837" s="90"/>
+      <c r="Y2837" s="90"/>
+      <c r="Z2837" s="90"/>
+      <c r="AA2837" s="90"/>
+      <c r="AB2837" s="90"/>
+      <c r="AC2837" s="90"/>
+      <c r="AD2837" s="90"/>
+      <c r="AE2837" s="90"/>
+      <c r="AF2837" s="90"/>
+      <c r="AG2837" s="90"/>
+      <c r="AH2837" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B112:AH112"/>
+    <mergeCell ref="B147:AG147"/>
+    <mergeCell ref="B308:AH308"/>
+    <mergeCell ref="B511:AH511"/>
+    <mergeCell ref="B712:AH712"/>
+    <mergeCell ref="B887:AH887"/>
+    <mergeCell ref="B1100:AH1100"/>
+    <mergeCell ref="B1227:AH1227"/>
+    <mergeCell ref="B1390:AH1390"/>
+    <mergeCell ref="B1502:AH1502"/>
+    <mergeCell ref="B1604:AH1604"/>
+    <mergeCell ref="B1698:AH1698"/>
+    <mergeCell ref="B1945:AH1945"/>
+    <mergeCell ref="B2031:AH2031"/>
+    <mergeCell ref="B2719:AH2719"/>
     <mergeCell ref="B2837:AH2837"/>
     <mergeCell ref="B2153:AH2153"/>
     <mergeCell ref="B2317:AH2317"/>
     <mergeCell ref="B2419:AH2419"/>
     <mergeCell ref="B2509:AH2509"/>
     <mergeCell ref="B2598:AH2598"/>
-    <mergeCell ref="B1604:AH1604"/>
-    <mergeCell ref="B1698:AH1698"/>
-    <mergeCell ref="B1945:AH1945"/>
-    <mergeCell ref="B2031:AH2031"/>
-    <mergeCell ref="B2719:AH2719"/>
-    <mergeCell ref="B887:AH887"/>
-    <mergeCell ref="B1100:AH1100"/>
-    <mergeCell ref="B1227:AH1227"/>
-    <mergeCell ref="B1390:AH1390"/>
-    <mergeCell ref="B1502:AH1502"/>
-    <mergeCell ref="B112:AH112"/>
-    <mergeCell ref="B147:AG147"/>
-    <mergeCell ref="B308:AH308"/>
-    <mergeCell ref="B511:AH511"/>
-    <mergeCell ref="B712:AH712"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="28" priority="1"/>
@@ -43593,40 +43596,40 @@
     </row>
     <row r="121" spans="1:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="122" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="93" t="s">
+      <c r="B122" s="94" t="s">
         <v>598</v>
       </c>
-      <c r="C122" s="94"/>
-      <c r="D122" s="94"/>
-      <c r="E122" s="94"/>
-      <c r="F122" s="94"/>
-      <c r="G122" s="94"/>
-      <c r="H122" s="94"/>
-      <c r="I122" s="94"/>
-      <c r="J122" s="94"/>
-      <c r="K122" s="94"/>
-      <c r="L122" s="94"/>
-      <c r="M122" s="94"/>
-      <c r="N122" s="94"/>
-      <c r="O122" s="94"/>
-      <c r="P122" s="94"/>
-      <c r="Q122" s="94"/>
-      <c r="R122" s="94"/>
-      <c r="S122" s="94"/>
-      <c r="T122" s="94"/>
-      <c r="U122" s="94"/>
-      <c r="V122" s="94"/>
-      <c r="W122" s="94"/>
-      <c r="X122" s="94"/>
-      <c r="Y122" s="94"/>
-      <c r="Z122" s="94"/>
-      <c r="AA122" s="94"/>
-      <c r="AB122" s="94"/>
-      <c r="AC122" s="94"/>
-      <c r="AD122" s="94"/>
-      <c r="AE122" s="94"/>
-      <c r="AF122" s="94"/>
-      <c r="AG122" s="94"/>
+      <c r="C122" s="95"/>
+      <c r="D122" s="95"/>
+      <c r="E122" s="95"/>
+      <c r="F122" s="95"/>
+      <c r="G122" s="95"/>
+      <c r="H122" s="95"/>
+      <c r="I122" s="95"/>
+      <c r="J122" s="95"/>
+      <c r="K122" s="95"/>
+      <c r="L122" s="95"/>
+      <c r="M122" s="95"/>
+      <c r="N122" s="95"/>
+      <c r="O122" s="95"/>
+      <c r="P122" s="95"/>
+      <c r="Q122" s="95"/>
+      <c r="R122" s="95"/>
+      <c r="S122" s="95"/>
+      <c r="T122" s="95"/>
+      <c r="U122" s="95"/>
+      <c r="V122" s="95"/>
+      <c r="W122" s="95"/>
+      <c r="X122" s="95"/>
+      <c r="Y122" s="95"/>
+      <c r="Z122" s="95"/>
+      <c r="AA122" s="95"/>
+      <c r="AB122" s="95"/>
+      <c r="AC122" s="95"/>
+      <c r="AD122" s="95"/>
+      <c r="AE122" s="95"/>
+      <c r="AF122" s="95"/>
+      <c r="AG122" s="95"/>
       <c r="AH122" s="77"/>
     </row>
     <row r="123" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -43720,693 +43723,693 @@
       </c>
     </row>
     <row r="308" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B308" s="95"/>
-      <c r="C308" s="95"/>
-      <c r="D308" s="95"/>
-      <c r="E308" s="95"/>
-      <c r="F308" s="95"/>
-      <c r="G308" s="95"/>
-      <c r="H308" s="95"/>
-      <c r="I308" s="95"/>
-      <c r="J308" s="95"/>
-      <c r="K308" s="95"/>
-      <c r="L308" s="95"/>
-      <c r="M308" s="95"/>
-      <c r="N308" s="95"/>
-      <c r="O308" s="95"/>
-      <c r="P308" s="95"/>
-      <c r="Q308" s="95"/>
-      <c r="R308" s="95"/>
-      <c r="S308" s="95"/>
-      <c r="T308" s="95"/>
-      <c r="U308" s="95"/>
-      <c r="V308" s="95"/>
-      <c r="W308" s="95"/>
-      <c r="X308" s="95"/>
-      <c r="Y308" s="95"/>
-      <c r="Z308" s="95"/>
-      <c r="AA308" s="95"/>
-      <c r="AB308" s="95"/>
-      <c r="AC308" s="95"/>
-      <c r="AD308" s="95"/>
-      <c r="AE308" s="95"/>
-      <c r="AF308" s="95"/>
-      <c r="AG308" s="95"/>
-      <c r="AH308" s="95"/>
+      <c r="B308" s="90"/>
+      <c r="C308" s="90"/>
+      <c r="D308" s="90"/>
+      <c r="E308" s="90"/>
+      <c r="F308" s="90"/>
+      <c r="G308" s="90"/>
+      <c r="H308" s="90"/>
+      <c r="I308" s="90"/>
+      <c r="J308" s="90"/>
+      <c r="K308" s="90"/>
+      <c r="L308" s="90"/>
+      <c r="M308" s="90"/>
+      <c r="N308" s="90"/>
+      <c r="O308" s="90"/>
+      <c r="P308" s="90"/>
+      <c r="Q308" s="90"/>
+      <c r="R308" s="90"/>
+      <c r="S308" s="90"/>
+      <c r="T308" s="90"/>
+      <c r="U308" s="90"/>
+      <c r="V308" s="90"/>
+      <c r="W308" s="90"/>
+      <c r="X308" s="90"/>
+      <c r="Y308" s="90"/>
+      <c r="Z308" s="90"/>
+      <c r="AA308" s="90"/>
+      <c r="AB308" s="90"/>
+      <c r="AC308" s="90"/>
+      <c r="AD308" s="90"/>
+      <c r="AE308" s="90"/>
+      <c r="AF308" s="90"/>
+      <c r="AG308" s="90"/>
+      <c r="AH308" s="90"/>
     </row>
     <row r="511" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B511" s="95"/>
-      <c r="C511" s="95"/>
-      <c r="D511" s="95"/>
-      <c r="E511" s="95"/>
-      <c r="F511" s="95"/>
-      <c r="G511" s="95"/>
-      <c r="H511" s="95"/>
-      <c r="I511" s="95"/>
-      <c r="J511" s="95"/>
-      <c r="K511" s="95"/>
-      <c r="L511" s="95"/>
-      <c r="M511" s="95"/>
-      <c r="N511" s="95"/>
-      <c r="O511" s="95"/>
-      <c r="P511" s="95"/>
-      <c r="Q511" s="95"/>
-      <c r="R511" s="95"/>
-      <c r="S511" s="95"/>
-      <c r="T511" s="95"/>
-      <c r="U511" s="95"/>
-      <c r="V511" s="95"/>
-      <c r="W511" s="95"/>
-      <c r="X511" s="95"/>
-      <c r="Y511" s="95"/>
-      <c r="Z511" s="95"/>
-      <c r="AA511" s="95"/>
-      <c r="AB511" s="95"/>
-      <c r="AC511" s="95"/>
-      <c r="AD511" s="95"/>
-      <c r="AE511" s="95"/>
-      <c r="AF511" s="95"/>
-      <c r="AG511" s="95"/>
-      <c r="AH511" s="95"/>
+      <c r="B511" s="90"/>
+      <c r="C511" s="90"/>
+      <c r="D511" s="90"/>
+      <c r="E511" s="90"/>
+      <c r="F511" s="90"/>
+      <c r="G511" s="90"/>
+      <c r="H511" s="90"/>
+      <c r="I511" s="90"/>
+      <c r="J511" s="90"/>
+      <c r="K511" s="90"/>
+      <c r="L511" s="90"/>
+      <c r="M511" s="90"/>
+      <c r="N511" s="90"/>
+      <c r="O511" s="90"/>
+      <c r="P511" s="90"/>
+      <c r="Q511" s="90"/>
+      <c r="R511" s="90"/>
+      <c r="S511" s="90"/>
+      <c r="T511" s="90"/>
+      <c r="U511" s="90"/>
+      <c r="V511" s="90"/>
+      <c r="W511" s="90"/>
+      <c r="X511" s="90"/>
+      <c r="Y511" s="90"/>
+      <c r="Z511" s="90"/>
+      <c r="AA511" s="90"/>
+      <c r="AB511" s="90"/>
+      <c r="AC511" s="90"/>
+      <c r="AD511" s="90"/>
+      <c r="AE511" s="90"/>
+      <c r="AF511" s="90"/>
+      <c r="AG511" s="90"/>
+      <c r="AH511" s="90"/>
     </row>
     <row r="712" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B712" s="95"/>
-      <c r="C712" s="95"/>
-      <c r="D712" s="95"/>
-      <c r="E712" s="95"/>
-      <c r="F712" s="95"/>
-      <c r="G712" s="95"/>
-      <c r="H712" s="95"/>
-      <c r="I712" s="95"/>
-      <c r="J712" s="95"/>
-      <c r="K712" s="95"/>
-      <c r="L712" s="95"/>
-      <c r="M712" s="95"/>
-      <c r="N712" s="95"/>
-      <c r="O712" s="95"/>
-      <c r="P712" s="95"/>
-      <c r="Q712" s="95"/>
-      <c r="R712" s="95"/>
-      <c r="S712" s="95"/>
-      <c r="T712" s="95"/>
-      <c r="U712" s="95"/>
-      <c r="V712" s="95"/>
-      <c r="W712" s="95"/>
-      <c r="X712" s="95"/>
-      <c r="Y712" s="95"/>
-      <c r="Z712" s="95"/>
-      <c r="AA712" s="95"/>
-      <c r="AB712" s="95"/>
-      <c r="AC712" s="95"/>
-      <c r="AD712" s="95"/>
-      <c r="AE712" s="95"/>
-      <c r="AF712" s="95"/>
-      <c r="AG712" s="95"/>
-      <c r="AH712" s="95"/>
+      <c r="B712" s="90"/>
+      <c r="C712" s="90"/>
+      <c r="D712" s="90"/>
+      <c r="E712" s="90"/>
+      <c r="F712" s="90"/>
+      <c r="G712" s="90"/>
+      <c r="H712" s="90"/>
+      <c r="I712" s="90"/>
+      <c r="J712" s="90"/>
+      <c r="K712" s="90"/>
+      <c r="L712" s="90"/>
+      <c r="M712" s="90"/>
+      <c r="N712" s="90"/>
+      <c r="O712" s="90"/>
+      <c r="P712" s="90"/>
+      <c r="Q712" s="90"/>
+      <c r="R712" s="90"/>
+      <c r="S712" s="90"/>
+      <c r="T712" s="90"/>
+      <c r="U712" s="90"/>
+      <c r="V712" s="90"/>
+      <c r="W712" s="90"/>
+      <c r="X712" s="90"/>
+      <c r="Y712" s="90"/>
+      <c r="Z712" s="90"/>
+      <c r="AA712" s="90"/>
+      <c r="AB712" s="90"/>
+      <c r="AC712" s="90"/>
+      <c r="AD712" s="90"/>
+      <c r="AE712" s="90"/>
+      <c r="AF712" s="90"/>
+      <c r="AG712" s="90"/>
+      <c r="AH712" s="90"/>
     </row>
     <row r="887" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B887" s="95"/>
-      <c r="C887" s="95"/>
-      <c r="D887" s="95"/>
-      <c r="E887" s="95"/>
-      <c r="F887" s="95"/>
-      <c r="G887" s="95"/>
-      <c r="H887" s="95"/>
-      <c r="I887" s="95"/>
-      <c r="J887" s="95"/>
-      <c r="K887" s="95"/>
-      <c r="L887" s="95"/>
-      <c r="M887" s="95"/>
-      <c r="N887" s="95"/>
-      <c r="O887" s="95"/>
-      <c r="P887" s="95"/>
-      <c r="Q887" s="95"/>
-      <c r="R887" s="95"/>
-      <c r="S887" s="95"/>
-      <c r="T887" s="95"/>
-      <c r="U887" s="95"/>
-      <c r="V887" s="95"/>
-      <c r="W887" s="95"/>
-      <c r="X887" s="95"/>
-      <c r="Y887" s="95"/>
-      <c r="Z887" s="95"/>
-      <c r="AA887" s="95"/>
-      <c r="AB887" s="95"/>
-      <c r="AC887" s="95"/>
-      <c r="AD887" s="95"/>
-      <c r="AE887" s="95"/>
-      <c r="AF887" s="95"/>
-      <c r="AG887" s="95"/>
-      <c r="AH887" s="95"/>
+      <c r="B887" s="90"/>
+      <c r="C887" s="90"/>
+      <c r="D887" s="90"/>
+      <c r="E887" s="90"/>
+      <c r="F887" s="90"/>
+      <c r="G887" s="90"/>
+      <c r="H887" s="90"/>
+      <c r="I887" s="90"/>
+      <c r="J887" s="90"/>
+      <c r="K887" s="90"/>
+      <c r="L887" s="90"/>
+      <c r="M887" s="90"/>
+      <c r="N887" s="90"/>
+      <c r="O887" s="90"/>
+      <c r="P887" s="90"/>
+      <c r="Q887" s="90"/>
+      <c r="R887" s="90"/>
+      <c r="S887" s="90"/>
+      <c r="T887" s="90"/>
+      <c r="U887" s="90"/>
+      <c r="V887" s="90"/>
+      <c r="W887" s="90"/>
+      <c r="X887" s="90"/>
+      <c r="Y887" s="90"/>
+      <c r="Z887" s="90"/>
+      <c r="AA887" s="90"/>
+      <c r="AB887" s="90"/>
+      <c r="AC887" s="90"/>
+      <c r="AD887" s="90"/>
+      <c r="AE887" s="90"/>
+      <c r="AF887" s="90"/>
+      <c r="AG887" s="90"/>
+      <c r="AH887" s="90"/>
     </row>
     <row r="1100" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1100" s="95"/>
-      <c r="C1100" s="95"/>
-      <c r="D1100" s="95"/>
-      <c r="E1100" s="95"/>
-      <c r="F1100" s="95"/>
-      <c r="G1100" s="95"/>
-      <c r="H1100" s="95"/>
-      <c r="I1100" s="95"/>
-      <c r="J1100" s="95"/>
-      <c r="K1100" s="95"/>
-      <c r="L1100" s="95"/>
-      <c r="M1100" s="95"/>
-      <c r="N1100" s="95"/>
-      <c r="O1100" s="95"/>
-      <c r="P1100" s="95"/>
-      <c r="Q1100" s="95"/>
-      <c r="R1100" s="95"/>
-      <c r="S1100" s="95"/>
-      <c r="T1100" s="95"/>
-      <c r="U1100" s="95"/>
-      <c r="V1100" s="95"/>
-      <c r="W1100" s="95"/>
-      <c r="X1100" s="95"/>
-      <c r="Y1100" s="95"/>
-      <c r="Z1100" s="95"/>
-      <c r="AA1100" s="95"/>
-      <c r="AB1100" s="95"/>
-      <c r="AC1100" s="95"/>
-      <c r="AD1100" s="95"/>
-      <c r="AE1100" s="95"/>
-      <c r="AF1100" s="95"/>
-      <c r="AG1100" s="95"/>
-      <c r="AH1100" s="95"/>
+      <c r="B1100" s="90"/>
+      <c r="C1100" s="90"/>
+      <c r="D1100" s="90"/>
+      <c r="E1100" s="90"/>
+      <c r="F1100" s="90"/>
+      <c r="G1100" s="90"/>
+      <c r="H1100" s="90"/>
+      <c r="I1100" s="90"/>
+      <c r="J1100" s="90"/>
+      <c r="K1100" s="90"/>
+      <c r="L1100" s="90"/>
+      <c r="M1100" s="90"/>
+      <c r="N1100" s="90"/>
+      <c r="O1100" s="90"/>
+      <c r="P1100" s="90"/>
+      <c r="Q1100" s="90"/>
+      <c r="R1100" s="90"/>
+      <c r="S1100" s="90"/>
+      <c r="T1100" s="90"/>
+      <c r="U1100" s="90"/>
+      <c r="V1100" s="90"/>
+      <c r="W1100" s="90"/>
+      <c r="X1100" s="90"/>
+      <c r="Y1100" s="90"/>
+      <c r="Z1100" s="90"/>
+      <c r="AA1100" s="90"/>
+      <c r="AB1100" s="90"/>
+      <c r="AC1100" s="90"/>
+      <c r="AD1100" s="90"/>
+      <c r="AE1100" s="90"/>
+      <c r="AF1100" s="90"/>
+      <c r="AG1100" s="90"/>
+      <c r="AH1100" s="90"/>
     </row>
     <row r="1227" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1227" s="95"/>
-      <c r="C1227" s="95"/>
-      <c r="D1227" s="95"/>
-      <c r="E1227" s="95"/>
-      <c r="F1227" s="95"/>
-      <c r="G1227" s="95"/>
-      <c r="H1227" s="95"/>
-      <c r="I1227" s="95"/>
-      <c r="J1227" s="95"/>
-      <c r="K1227" s="95"/>
-      <c r="L1227" s="95"/>
-      <c r="M1227" s="95"/>
-      <c r="N1227" s="95"/>
-      <c r="O1227" s="95"/>
-      <c r="P1227" s="95"/>
-      <c r="Q1227" s="95"/>
-      <c r="R1227" s="95"/>
-      <c r="S1227" s="95"/>
-      <c r="T1227" s="95"/>
-      <c r="U1227" s="95"/>
-      <c r="V1227" s="95"/>
-      <c r="W1227" s="95"/>
-      <c r="X1227" s="95"/>
-      <c r="Y1227" s="95"/>
-      <c r="Z1227" s="95"/>
-      <c r="AA1227" s="95"/>
-      <c r="AB1227" s="95"/>
-      <c r="AC1227" s="95"/>
-      <c r="AD1227" s="95"/>
-      <c r="AE1227" s="95"/>
-      <c r="AF1227" s="95"/>
-      <c r="AG1227" s="95"/>
-      <c r="AH1227" s="95"/>
+      <c r="B1227" s="90"/>
+      <c r="C1227" s="90"/>
+      <c r="D1227" s="90"/>
+      <c r="E1227" s="90"/>
+      <c r="F1227" s="90"/>
+      <c r="G1227" s="90"/>
+      <c r="H1227" s="90"/>
+      <c r="I1227" s="90"/>
+      <c r="J1227" s="90"/>
+      <c r="K1227" s="90"/>
+      <c r="L1227" s="90"/>
+      <c r="M1227" s="90"/>
+      <c r="N1227" s="90"/>
+      <c r="O1227" s="90"/>
+      <c r="P1227" s="90"/>
+      <c r="Q1227" s="90"/>
+      <c r="R1227" s="90"/>
+      <c r="S1227" s="90"/>
+      <c r="T1227" s="90"/>
+      <c r="U1227" s="90"/>
+      <c r="V1227" s="90"/>
+      <c r="W1227" s="90"/>
+      <c r="X1227" s="90"/>
+      <c r="Y1227" s="90"/>
+      <c r="Z1227" s="90"/>
+      <c r="AA1227" s="90"/>
+      <c r="AB1227" s="90"/>
+      <c r="AC1227" s="90"/>
+      <c r="AD1227" s="90"/>
+      <c r="AE1227" s="90"/>
+      <c r="AF1227" s="90"/>
+      <c r="AG1227" s="90"/>
+      <c r="AH1227" s="90"/>
     </row>
     <row r="1390" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1390" s="95"/>
-      <c r="C1390" s="95"/>
-      <c r="D1390" s="95"/>
-      <c r="E1390" s="95"/>
-      <c r="F1390" s="95"/>
-      <c r="G1390" s="95"/>
-      <c r="H1390" s="95"/>
-      <c r="I1390" s="95"/>
-      <c r="J1390" s="95"/>
-      <c r="K1390" s="95"/>
-      <c r="L1390" s="95"/>
-      <c r="M1390" s="95"/>
-      <c r="N1390" s="95"/>
-      <c r="O1390" s="95"/>
-      <c r="P1390" s="95"/>
-      <c r="Q1390" s="95"/>
-      <c r="R1390" s="95"/>
-      <c r="S1390" s="95"/>
-      <c r="T1390" s="95"/>
-      <c r="U1390" s="95"/>
-      <c r="V1390" s="95"/>
-      <c r="W1390" s="95"/>
-      <c r="X1390" s="95"/>
-      <c r="Y1390" s="95"/>
-      <c r="Z1390" s="95"/>
-      <c r="AA1390" s="95"/>
-      <c r="AB1390" s="95"/>
-      <c r="AC1390" s="95"/>
-      <c r="AD1390" s="95"/>
-      <c r="AE1390" s="95"/>
-      <c r="AF1390" s="95"/>
-      <c r="AG1390" s="95"/>
-      <c r="AH1390" s="95"/>
+      <c r="B1390" s="90"/>
+      <c r="C1390" s="90"/>
+      <c r="D1390" s="90"/>
+      <c r="E1390" s="90"/>
+      <c r="F1390" s="90"/>
+      <c r="G1390" s="90"/>
+      <c r="H1390" s="90"/>
+      <c r="I1390" s="90"/>
+      <c r="J1390" s="90"/>
+      <c r="K1390" s="90"/>
+      <c r="L1390" s="90"/>
+      <c r="M1390" s="90"/>
+      <c r="N1390" s="90"/>
+      <c r="O1390" s="90"/>
+      <c r="P1390" s="90"/>
+      <c r="Q1390" s="90"/>
+      <c r="R1390" s="90"/>
+      <c r="S1390" s="90"/>
+      <c r="T1390" s="90"/>
+      <c r="U1390" s="90"/>
+      <c r="V1390" s="90"/>
+      <c r="W1390" s="90"/>
+      <c r="X1390" s="90"/>
+      <c r="Y1390" s="90"/>
+      <c r="Z1390" s="90"/>
+      <c r="AA1390" s="90"/>
+      <c r="AB1390" s="90"/>
+      <c r="AC1390" s="90"/>
+      <c r="AD1390" s="90"/>
+      <c r="AE1390" s="90"/>
+      <c r="AF1390" s="90"/>
+      <c r="AG1390" s="90"/>
+      <c r="AH1390" s="90"/>
     </row>
     <row r="1502" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1502" s="95"/>
-      <c r="C1502" s="95"/>
-      <c r="D1502" s="95"/>
-      <c r="E1502" s="95"/>
-      <c r="F1502" s="95"/>
-      <c r="G1502" s="95"/>
-      <c r="H1502" s="95"/>
-      <c r="I1502" s="95"/>
-      <c r="J1502" s="95"/>
-      <c r="K1502" s="95"/>
-      <c r="L1502" s="95"/>
-      <c r="M1502" s="95"/>
-      <c r="N1502" s="95"/>
-      <c r="O1502" s="95"/>
-      <c r="P1502" s="95"/>
-      <c r="Q1502" s="95"/>
-      <c r="R1502" s="95"/>
-      <c r="S1502" s="95"/>
-      <c r="T1502" s="95"/>
-      <c r="U1502" s="95"/>
-      <c r="V1502" s="95"/>
-      <c r="W1502" s="95"/>
-      <c r="X1502" s="95"/>
-      <c r="Y1502" s="95"/>
-      <c r="Z1502" s="95"/>
-      <c r="AA1502" s="95"/>
-      <c r="AB1502" s="95"/>
-      <c r="AC1502" s="95"/>
-      <c r="AD1502" s="95"/>
-      <c r="AE1502" s="95"/>
-      <c r="AF1502" s="95"/>
-      <c r="AG1502" s="95"/>
-      <c r="AH1502" s="95"/>
+      <c r="B1502" s="90"/>
+      <c r="C1502" s="90"/>
+      <c r="D1502" s="90"/>
+      <c r="E1502" s="90"/>
+      <c r="F1502" s="90"/>
+      <c r="G1502" s="90"/>
+      <c r="H1502" s="90"/>
+      <c r="I1502" s="90"/>
+      <c r="J1502" s="90"/>
+      <c r="K1502" s="90"/>
+      <c r="L1502" s="90"/>
+      <c r="M1502" s="90"/>
+      <c r="N1502" s="90"/>
+      <c r="O1502" s="90"/>
+      <c r="P1502" s="90"/>
+      <c r="Q1502" s="90"/>
+      <c r="R1502" s="90"/>
+      <c r="S1502" s="90"/>
+      <c r="T1502" s="90"/>
+      <c r="U1502" s="90"/>
+      <c r="V1502" s="90"/>
+      <c r="W1502" s="90"/>
+      <c r="X1502" s="90"/>
+      <c r="Y1502" s="90"/>
+      <c r="Z1502" s="90"/>
+      <c r="AA1502" s="90"/>
+      <c r="AB1502" s="90"/>
+      <c r="AC1502" s="90"/>
+      <c r="AD1502" s="90"/>
+      <c r="AE1502" s="90"/>
+      <c r="AF1502" s="90"/>
+      <c r="AG1502" s="90"/>
+      <c r="AH1502" s="90"/>
     </row>
     <row r="1604" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1604" s="95"/>
-      <c r="C1604" s="95"/>
-      <c r="D1604" s="95"/>
-      <c r="E1604" s="95"/>
-      <c r="F1604" s="95"/>
-      <c r="G1604" s="95"/>
-      <c r="H1604" s="95"/>
-      <c r="I1604" s="95"/>
-      <c r="J1604" s="95"/>
-      <c r="K1604" s="95"/>
-      <c r="L1604" s="95"/>
-      <c r="M1604" s="95"/>
-      <c r="N1604" s="95"/>
-      <c r="O1604" s="95"/>
-      <c r="P1604" s="95"/>
-      <c r="Q1604" s="95"/>
-      <c r="R1604" s="95"/>
-      <c r="S1604" s="95"/>
-      <c r="T1604" s="95"/>
-      <c r="U1604" s="95"/>
-      <c r="V1604" s="95"/>
-      <c r="W1604" s="95"/>
-      <c r="X1604" s="95"/>
-      <c r="Y1604" s="95"/>
-      <c r="Z1604" s="95"/>
-      <c r="AA1604" s="95"/>
-      <c r="AB1604" s="95"/>
-      <c r="AC1604" s="95"/>
-      <c r="AD1604" s="95"/>
-      <c r="AE1604" s="95"/>
-      <c r="AF1604" s="95"/>
-      <c r="AG1604" s="95"/>
-      <c r="AH1604" s="95"/>
+      <c r="B1604" s="90"/>
+      <c r="C1604" s="90"/>
+      <c r="D1604" s="90"/>
+      <c r="E1604" s="90"/>
+      <c r="F1604" s="90"/>
+      <c r="G1604" s="90"/>
+      <c r="H1604" s="90"/>
+      <c r="I1604" s="90"/>
+      <c r="J1604" s="90"/>
+      <c r="K1604" s="90"/>
+      <c r="L1604" s="90"/>
+      <c r="M1604" s="90"/>
+      <c r="N1604" s="90"/>
+      <c r="O1604" s="90"/>
+      <c r="P1604" s="90"/>
+      <c r="Q1604" s="90"/>
+      <c r="R1604" s="90"/>
+      <c r="S1604" s="90"/>
+      <c r="T1604" s="90"/>
+      <c r="U1604" s="90"/>
+      <c r="V1604" s="90"/>
+      <c r="W1604" s="90"/>
+      <c r="X1604" s="90"/>
+      <c r="Y1604" s="90"/>
+      <c r="Z1604" s="90"/>
+      <c r="AA1604" s="90"/>
+      <c r="AB1604" s="90"/>
+      <c r="AC1604" s="90"/>
+      <c r="AD1604" s="90"/>
+      <c r="AE1604" s="90"/>
+      <c r="AF1604" s="90"/>
+      <c r="AG1604" s="90"/>
+      <c r="AH1604" s="90"/>
     </row>
     <row r="1698" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1698" s="95"/>
-      <c r="C1698" s="95"/>
-      <c r="D1698" s="95"/>
-      <c r="E1698" s="95"/>
-      <c r="F1698" s="95"/>
-      <c r="G1698" s="95"/>
-      <c r="H1698" s="95"/>
-      <c r="I1698" s="95"/>
-      <c r="J1698" s="95"/>
-      <c r="K1698" s="95"/>
-      <c r="L1698" s="95"/>
-      <c r="M1698" s="95"/>
-      <c r="N1698" s="95"/>
-      <c r="O1698" s="95"/>
-      <c r="P1698" s="95"/>
-      <c r="Q1698" s="95"/>
-      <c r="R1698" s="95"/>
-      <c r="S1698" s="95"/>
-      <c r="T1698" s="95"/>
-      <c r="U1698" s="95"/>
-      <c r="V1698" s="95"/>
-      <c r="W1698" s="95"/>
-      <c r="X1698" s="95"/>
-      <c r="Y1698" s="95"/>
-      <c r="Z1698" s="95"/>
-      <c r="AA1698" s="95"/>
-      <c r="AB1698" s="95"/>
-      <c r="AC1698" s="95"/>
-      <c r="AD1698" s="95"/>
-      <c r="AE1698" s="95"/>
-      <c r="AF1698" s="95"/>
-      <c r="AG1698" s="95"/>
-      <c r="AH1698" s="95"/>
+      <c r="B1698" s="90"/>
+      <c r="C1698" s="90"/>
+      <c r="D1698" s="90"/>
+      <c r="E1698" s="90"/>
+      <c r="F1698" s="90"/>
+      <c r="G1698" s="90"/>
+      <c r="H1698" s="90"/>
+      <c r="I1698" s="90"/>
+      <c r="J1698" s="90"/>
+      <c r="K1698" s="90"/>
+      <c r="L1698" s="90"/>
+      <c r="M1698" s="90"/>
+      <c r="N1698" s="90"/>
+      <c r="O1698" s="90"/>
+      <c r="P1698" s="90"/>
+      <c r="Q1698" s="90"/>
+      <c r="R1698" s="90"/>
+      <c r="S1698" s="90"/>
+      <c r="T1698" s="90"/>
+      <c r="U1698" s="90"/>
+      <c r="V1698" s="90"/>
+      <c r="W1698" s="90"/>
+      <c r="X1698" s="90"/>
+      <c r="Y1698" s="90"/>
+      <c r="Z1698" s="90"/>
+      <c r="AA1698" s="90"/>
+      <c r="AB1698" s="90"/>
+      <c r="AC1698" s="90"/>
+      <c r="AD1698" s="90"/>
+      <c r="AE1698" s="90"/>
+      <c r="AF1698" s="90"/>
+      <c r="AG1698" s="90"/>
+      <c r="AH1698" s="90"/>
     </row>
     <row r="1945" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1945" s="95"/>
-      <c r="C1945" s="95"/>
-      <c r="D1945" s="95"/>
-      <c r="E1945" s="95"/>
-      <c r="F1945" s="95"/>
-      <c r="G1945" s="95"/>
-      <c r="H1945" s="95"/>
-      <c r="I1945" s="95"/>
-      <c r="J1945" s="95"/>
-      <c r="K1945" s="95"/>
-      <c r="L1945" s="95"/>
-      <c r="M1945" s="95"/>
-      <c r="N1945" s="95"/>
-      <c r="O1945" s="95"/>
-      <c r="P1945" s="95"/>
-      <c r="Q1945" s="95"/>
-      <c r="R1945" s="95"/>
-      <c r="S1945" s="95"/>
-      <c r="T1945" s="95"/>
-      <c r="U1945" s="95"/>
-      <c r="V1945" s="95"/>
-      <c r="W1945" s="95"/>
-      <c r="X1945" s="95"/>
-      <c r="Y1945" s="95"/>
-      <c r="Z1945" s="95"/>
-      <c r="AA1945" s="95"/>
-      <c r="AB1945" s="95"/>
-      <c r="AC1945" s="95"/>
-      <c r="AD1945" s="95"/>
-      <c r="AE1945" s="95"/>
-      <c r="AF1945" s="95"/>
-      <c r="AG1945" s="95"/>
-      <c r="AH1945" s="95"/>
+      <c r="B1945" s="90"/>
+      <c r="C1945" s="90"/>
+      <c r="D1945" s="90"/>
+      <c r="E1945" s="90"/>
+      <c r="F1945" s="90"/>
+      <c r="G1945" s="90"/>
+      <c r="H1945" s="90"/>
+      <c r="I1945" s="90"/>
+      <c r="J1945" s="90"/>
+      <c r="K1945" s="90"/>
+      <c r="L1945" s="90"/>
+      <c r="M1945" s="90"/>
+      <c r="N1945" s="90"/>
+      <c r="O1945" s="90"/>
+      <c r="P1945" s="90"/>
+      <c r="Q1945" s="90"/>
+      <c r="R1945" s="90"/>
+      <c r="S1945" s="90"/>
+      <c r="T1945" s="90"/>
+      <c r="U1945" s="90"/>
+      <c r="V1945" s="90"/>
+      <c r="W1945" s="90"/>
+      <c r="X1945" s="90"/>
+      <c r="Y1945" s="90"/>
+      <c r="Z1945" s="90"/>
+      <c r="AA1945" s="90"/>
+      <c r="AB1945" s="90"/>
+      <c r="AC1945" s="90"/>
+      <c r="AD1945" s="90"/>
+      <c r="AE1945" s="90"/>
+      <c r="AF1945" s="90"/>
+      <c r="AG1945" s="90"/>
+      <c r="AH1945" s="90"/>
     </row>
     <row r="2031" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2031" s="95"/>
-      <c r="C2031" s="95"/>
-      <c r="D2031" s="95"/>
-      <c r="E2031" s="95"/>
-      <c r="F2031" s="95"/>
-      <c r="G2031" s="95"/>
-      <c r="H2031" s="95"/>
-      <c r="I2031" s="95"/>
-      <c r="J2031" s="95"/>
-      <c r="K2031" s="95"/>
-      <c r="L2031" s="95"/>
-      <c r="M2031" s="95"/>
-      <c r="N2031" s="95"/>
-      <c r="O2031" s="95"/>
-      <c r="P2031" s="95"/>
-      <c r="Q2031" s="95"/>
-      <c r="R2031" s="95"/>
-      <c r="S2031" s="95"/>
-      <c r="T2031" s="95"/>
-      <c r="U2031" s="95"/>
-      <c r="V2031" s="95"/>
-      <c r="W2031" s="95"/>
-      <c r="X2031" s="95"/>
-      <c r="Y2031" s="95"/>
-      <c r="Z2031" s="95"/>
-      <c r="AA2031" s="95"/>
-      <c r="AB2031" s="95"/>
-      <c r="AC2031" s="95"/>
-      <c r="AD2031" s="95"/>
-      <c r="AE2031" s="95"/>
-      <c r="AF2031" s="95"/>
-      <c r="AG2031" s="95"/>
-      <c r="AH2031" s="95"/>
+      <c r="B2031" s="90"/>
+      <c r="C2031" s="90"/>
+      <c r="D2031" s="90"/>
+      <c r="E2031" s="90"/>
+      <c r="F2031" s="90"/>
+      <c r="G2031" s="90"/>
+      <c r="H2031" s="90"/>
+      <c r="I2031" s="90"/>
+      <c r="J2031" s="90"/>
+      <c r="K2031" s="90"/>
+      <c r="L2031" s="90"/>
+      <c r="M2031" s="90"/>
+      <c r="N2031" s="90"/>
+      <c r="O2031" s="90"/>
+      <c r="P2031" s="90"/>
+      <c r="Q2031" s="90"/>
+      <c r="R2031" s="90"/>
+      <c r="S2031" s="90"/>
+      <c r="T2031" s="90"/>
+      <c r="U2031" s="90"/>
+      <c r="V2031" s="90"/>
+      <c r="W2031" s="90"/>
+      <c r="X2031" s="90"/>
+      <c r="Y2031" s="90"/>
+      <c r="Z2031" s="90"/>
+      <c r="AA2031" s="90"/>
+      <c r="AB2031" s="90"/>
+      <c r="AC2031" s="90"/>
+      <c r="AD2031" s="90"/>
+      <c r="AE2031" s="90"/>
+      <c r="AF2031" s="90"/>
+      <c r="AG2031" s="90"/>
+      <c r="AH2031" s="90"/>
     </row>
     <row r="2153" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2153" s="95"/>
-      <c r="C2153" s="95"/>
-      <c r="D2153" s="95"/>
-      <c r="E2153" s="95"/>
-      <c r="F2153" s="95"/>
-      <c r="G2153" s="95"/>
-      <c r="H2153" s="95"/>
-      <c r="I2153" s="95"/>
-      <c r="J2153" s="95"/>
-      <c r="K2153" s="95"/>
-      <c r="L2153" s="95"/>
-      <c r="M2153" s="95"/>
-      <c r="N2153" s="95"/>
-      <c r="O2153" s="95"/>
-      <c r="P2153" s="95"/>
-      <c r="Q2153" s="95"/>
-      <c r="R2153" s="95"/>
-      <c r="S2153" s="95"/>
-      <c r="T2153" s="95"/>
-      <c r="U2153" s="95"/>
-      <c r="V2153" s="95"/>
-      <c r="W2153" s="95"/>
-      <c r="X2153" s="95"/>
-      <c r="Y2153" s="95"/>
-      <c r="Z2153" s="95"/>
-      <c r="AA2153" s="95"/>
-      <c r="AB2153" s="95"/>
-      <c r="AC2153" s="95"/>
-      <c r="AD2153" s="95"/>
-      <c r="AE2153" s="95"/>
-      <c r="AF2153" s="95"/>
-      <c r="AG2153" s="95"/>
-      <c r="AH2153" s="95"/>
+      <c r="B2153" s="90"/>
+      <c r="C2153" s="90"/>
+      <c r="D2153" s="90"/>
+      <c r="E2153" s="90"/>
+      <c r="F2153" s="90"/>
+      <c r="G2153" s="90"/>
+      <c r="H2153" s="90"/>
+      <c r="I2153" s="90"/>
+      <c r="J2153" s="90"/>
+      <c r="K2153" s="90"/>
+      <c r="L2153" s="90"/>
+      <c r="M2153" s="90"/>
+      <c r="N2153" s="90"/>
+      <c r="O2153" s="90"/>
+      <c r="P2153" s="90"/>
+      <c r="Q2153" s="90"/>
+      <c r="R2153" s="90"/>
+      <c r="S2153" s="90"/>
+      <c r="T2153" s="90"/>
+      <c r="U2153" s="90"/>
+      <c r="V2153" s="90"/>
+      <c r="W2153" s="90"/>
+      <c r="X2153" s="90"/>
+      <c r="Y2153" s="90"/>
+      <c r="Z2153" s="90"/>
+      <c r="AA2153" s="90"/>
+      <c r="AB2153" s="90"/>
+      <c r="AC2153" s="90"/>
+      <c r="AD2153" s="90"/>
+      <c r="AE2153" s="90"/>
+      <c r="AF2153" s="90"/>
+      <c r="AG2153" s="90"/>
+      <c r="AH2153" s="90"/>
     </row>
     <row r="2317" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2317" s="95"/>
-      <c r="C2317" s="95"/>
-      <c r="D2317" s="95"/>
-      <c r="E2317" s="95"/>
-      <c r="F2317" s="95"/>
-      <c r="G2317" s="95"/>
-      <c r="H2317" s="95"/>
-      <c r="I2317" s="95"/>
-      <c r="J2317" s="95"/>
-      <c r="K2317" s="95"/>
-      <c r="L2317" s="95"/>
-      <c r="M2317" s="95"/>
-      <c r="N2317" s="95"/>
-      <c r="O2317" s="95"/>
-      <c r="P2317" s="95"/>
-      <c r="Q2317" s="95"/>
-      <c r="R2317" s="95"/>
-      <c r="S2317" s="95"/>
-      <c r="T2317" s="95"/>
-      <c r="U2317" s="95"/>
-      <c r="V2317" s="95"/>
-      <c r="W2317" s="95"/>
-      <c r="X2317" s="95"/>
-      <c r="Y2317" s="95"/>
-      <c r="Z2317" s="95"/>
-      <c r="AA2317" s="95"/>
-      <c r="AB2317" s="95"/>
-      <c r="AC2317" s="95"/>
-      <c r="AD2317" s="95"/>
-      <c r="AE2317" s="95"/>
-      <c r="AF2317" s="95"/>
-      <c r="AG2317" s="95"/>
-      <c r="AH2317" s="95"/>
+      <c r="B2317" s="90"/>
+      <c r="C2317" s="90"/>
+      <c r="D2317" s="90"/>
+      <c r="E2317" s="90"/>
+      <c r="F2317" s="90"/>
+      <c r="G2317" s="90"/>
+      <c r="H2317" s="90"/>
+      <c r="I2317" s="90"/>
+      <c r="J2317" s="90"/>
+      <c r="K2317" s="90"/>
+      <c r="L2317" s="90"/>
+      <c r="M2317" s="90"/>
+      <c r="N2317" s="90"/>
+      <c r="O2317" s="90"/>
+      <c r="P2317" s="90"/>
+      <c r="Q2317" s="90"/>
+      <c r="R2317" s="90"/>
+      <c r="S2317" s="90"/>
+      <c r="T2317" s="90"/>
+      <c r="U2317" s="90"/>
+      <c r="V2317" s="90"/>
+      <c r="W2317" s="90"/>
+      <c r="X2317" s="90"/>
+      <c r="Y2317" s="90"/>
+      <c r="Z2317" s="90"/>
+      <c r="AA2317" s="90"/>
+      <c r="AB2317" s="90"/>
+      <c r="AC2317" s="90"/>
+      <c r="AD2317" s="90"/>
+      <c r="AE2317" s="90"/>
+      <c r="AF2317" s="90"/>
+      <c r="AG2317" s="90"/>
+      <c r="AH2317" s="90"/>
     </row>
     <row r="2419" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2419" s="95"/>
-      <c r="C2419" s="95"/>
-      <c r="D2419" s="95"/>
-      <c r="E2419" s="95"/>
-      <c r="F2419" s="95"/>
-      <c r="G2419" s="95"/>
-      <c r="H2419" s="95"/>
-      <c r="I2419" s="95"/>
-      <c r="J2419" s="95"/>
-      <c r="K2419" s="95"/>
-      <c r="L2419" s="95"/>
-      <c r="M2419" s="95"/>
-      <c r="N2419" s="95"/>
-      <c r="O2419" s="95"/>
-      <c r="P2419" s="95"/>
-      <c r="Q2419" s="95"/>
-      <c r="R2419" s="95"/>
-      <c r="S2419" s="95"/>
-      <c r="T2419" s="95"/>
-      <c r="U2419" s="95"/>
-      <c r="V2419" s="95"/>
-      <c r="W2419" s="95"/>
-      <c r="X2419" s="95"/>
-      <c r="Y2419" s="95"/>
-      <c r="Z2419" s="95"/>
-      <c r="AA2419" s="95"/>
-      <c r="AB2419" s="95"/>
-      <c r="AC2419" s="95"/>
-      <c r="AD2419" s="95"/>
-      <c r="AE2419" s="95"/>
-      <c r="AF2419" s="95"/>
-      <c r="AG2419" s="95"/>
-      <c r="AH2419" s="95"/>
+      <c r="B2419" s="90"/>
+      <c r="C2419" s="90"/>
+      <c r="D2419" s="90"/>
+      <c r="E2419" s="90"/>
+      <c r="F2419" s="90"/>
+      <c r="G2419" s="90"/>
+      <c r="H2419" s="90"/>
+      <c r="I2419" s="90"/>
+      <c r="J2419" s="90"/>
+      <c r="K2419" s="90"/>
+      <c r="L2419" s="90"/>
+      <c r="M2419" s="90"/>
+      <c r="N2419" s="90"/>
+      <c r="O2419" s="90"/>
+      <c r="P2419" s="90"/>
+      <c r="Q2419" s="90"/>
+      <c r="R2419" s="90"/>
+      <c r="S2419" s="90"/>
+      <c r="T2419" s="90"/>
+      <c r="U2419" s="90"/>
+      <c r="V2419" s="90"/>
+      <c r="W2419" s="90"/>
+      <c r="X2419" s="90"/>
+      <c r="Y2419" s="90"/>
+      <c r="Z2419" s="90"/>
+      <c r="AA2419" s="90"/>
+      <c r="AB2419" s="90"/>
+      <c r="AC2419" s="90"/>
+      <c r="AD2419" s="90"/>
+      <c r="AE2419" s="90"/>
+      <c r="AF2419" s="90"/>
+      <c r="AG2419" s="90"/>
+      <c r="AH2419" s="90"/>
     </row>
     <row r="2509" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2509" s="95"/>
-      <c r="C2509" s="95"/>
-      <c r="D2509" s="95"/>
-      <c r="E2509" s="95"/>
-      <c r="F2509" s="95"/>
-      <c r="G2509" s="95"/>
-      <c r="H2509" s="95"/>
-      <c r="I2509" s="95"/>
-      <c r="J2509" s="95"/>
-      <c r="K2509" s="95"/>
-      <c r="L2509" s="95"/>
-      <c r="M2509" s="95"/>
-      <c r="N2509" s="95"/>
-      <c r="O2509" s="95"/>
-      <c r="P2509" s="95"/>
-      <c r="Q2509" s="95"/>
-      <c r="R2509" s="95"/>
-      <c r="S2509" s="95"/>
-      <c r="T2509" s="95"/>
-      <c r="U2509" s="95"/>
-      <c r="V2509" s="95"/>
-      <c r="W2509" s="95"/>
-      <c r="X2509" s="95"/>
-      <c r="Y2509" s="95"/>
-      <c r="Z2509" s="95"/>
-      <c r="AA2509" s="95"/>
-      <c r="AB2509" s="95"/>
-      <c r="AC2509" s="95"/>
-      <c r="AD2509" s="95"/>
-      <c r="AE2509" s="95"/>
-      <c r="AF2509" s="95"/>
-      <c r="AG2509" s="95"/>
-      <c r="AH2509" s="95"/>
+      <c r="B2509" s="90"/>
+      <c r="C2509" s="90"/>
+      <c r="D2509" s="90"/>
+      <c r="E2509" s="90"/>
+      <c r="F2509" s="90"/>
+      <c r="G2509" s="90"/>
+      <c r="H2509" s="90"/>
+      <c r="I2509" s="90"/>
+      <c r="J2509" s="90"/>
+      <c r="K2509" s="90"/>
+      <c r="L2509" s="90"/>
+      <c r="M2509" s="90"/>
+      <c r="N2509" s="90"/>
+      <c r="O2509" s="90"/>
+      <c r="P2509" s="90"/>
+      <c r="Q2509" s="90"/>
+      <c r="R2509" s="90"/>
+      <c r="S2509" s="90"/>
+      <c r="T2509" s="90"/>
+      <c r="U2509" s="90"/>
+      <c r="V2509" s="90"/>
+      <c r="W2509" s="90"/>
+      <c r="X2509" s="90"/>
+      <c r="Y2509" s="90"/>
+      <c r="Z2509" s="90"/>
+      <c r="AA2509" s="90"/>
+      <c r="AB2509" s="90"/>
+      <c r="AC2509" s="90"/>
+      <c r="AD2509" s="90"/>
+      <c r="AE2509" s="90"/>
+      <c r="AF2509" s="90"/>
+      <c r="AG2509" s="90"/>
+      <c r="AH2509" s="90"/>
     </row>
     <row r="2598" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2598" s="95"/>
-      <c r="C2598" s="95"/>
-      <c r="D2598" s="95"/>
-      <c r="E2598" s="95"/>
-      <c r="F2598" s="95"/>
-      <c r="G2598" s="95"/>
-      <c r="H2598" s="95"/>
-      <c r="I2598" s="95"/>
-      <c r="J2598" s="95"/>
-      <c r="K2598" s="95"/>
-      <c r="L2598" s="95"/>
-      <c r="M2598" s="95"/>
-      <c r="N2598" s="95"/>
-      <c r="O2598" s="95"/>
-      <c r="P2598" s="95"/>
-      <c r="Q2598" s="95"/>
-      <c r="R2598" s="95"/>
-      <c r="S2598" s="95"/>
-      <c r="T2598" s="95"/>
-      <c r="U2598" s="95"/>
-      <c r="V2598" s="95"/>
-      <c r="W2598" s="95"/>
-      <c r="X2598" s="95"/>
-      <c r="Y2598" s="95"/>
-      <c r="Z2598" s="95"/>
-      <c r="AA2598" s="95"/>
-      <c r="AB2598" s="95"/>
-      <c r="AC2598" s="95"/>
-      <c r="AD2598" s="95"/>
-      <c r="AE2598" s="95"/>
-      <c r="AF2598" s="95"/>
-      <c r="AG2598" s="95"/>
-      <c r="AH2598" s="95"/>
+      <c r="B2598" s="90"/>
+      <c r="C2598" s="90"/>
+      <c r="D2598" s="90"/>
+      <c r="E2598" s="90"/>
+      <c r="F2598" s="90"/>
+      <c r="G2598" s="90"/>
+      <c r="H2598" s="90"/>
+      <c r="I2598" s="90"/>
+      <c r="J2598" s="90"/>
+      <c r="K2598" s="90"/>
+      <c r="L2598" s="90"/>
+      <c r="M2598" s="90"/>
+      <c r="N2598" s="90"/>
+      <c r="O2598" s="90"/>
+      <c r="P2598" s="90"/>
+      <c r="Q2598" s="90"/>
+      <c r="R2598" s="90"/>
+      <c r="S2598" s="90"/>
+      <c r="T2598" s="90"/>
+      <c r="U2598" s="90"/>
+      <c r="V2598" s="90"/>
+      <c r="W2598" s="90"/>
+      <c r="X2598" s="90"/>
+      <c r="Y2598" s="90"/>
+      <c r="Z2598" s="90"/>
+      <c r="AA2598" s="90"/>
+      <c r="AB2598" s="90"/>
+      <c r="AC2598" s="90"/>
+      <c r="AD2598" s="90"/>
+      <c r="AE2598" s="90"/>
+      <c r="AF2598" s="90"/>
+      <c r="AG2598" s="90"/>
+      <c r="AH2598" s="90"/>
     </row>
     <row r="2719" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2719" s="95"/>
-      <c r="C2719" s="95"/>
-      <c r="D2719" s="95"/>
-      <c r="E2719" s="95"/>
-      <c r="F2719" s="95"/>
-      <c r="G2719" s="95"/>
-      <c r="H2719" s="95"/>
-      <c r="I2719" s="95"/>
-      <c r="J2719" s="95"/>
-      <c r="K2719" s="95"/>
-      <c r="L2719" s="95"/>
-      <c r="M2719" s="95"/>
-      <c r="N2719" s="95"/>
-      <c r="O2719" s="95"/>
-      <c r="P2719" s="95"/>
-      <c r="Q2719" s="95"/>
-      <c r="R2719" s="95"/>
-      <c r="S2719" s="95"/>
-      <c r="T2719" s="95"/>
-      <c r="U2719" s="95"/>
-      <c r="V2719" s="95"/>
-      <c r="W2719" s="95"/>
-      <c r="X2719" s="95"/>
-      <c r="Y2719" s="95"/>
-      <c r="Z2719" s="95"/>
-      <c r="AA2719" s="95"/>
-      <c r="AB2719" s="95"/>
-      <c r="AC2719" s="95"/>
-      <c r="AD2719" s="95"/>
-      <c r="AE2719" s="95"/>
-      <c r="AF2719" s="95"/>
-      <c r="AG2719" s="95"/>
-      <c r="AH2719" s="95"/>
+      <c r="B2719" s="90"/>
+      <c r="C2719" s="90"/>
+      <c r="D2719" s="90"/>
+      <c r="E2719" s="90"/>
+      <c r="F2719" s="90"/>
+      <c r="G2719" s="90"/>
+      <c r="H2719" s="90"/>
+      <c r="I2719" s="90"/>
+      <c r="J2719" s="90"/>
+      <c r="K2719" s="90"/>
+      <c r="L2719" s="90"/>
+      <c r="M2719" s="90"/>
+      <c r="N2719" s="90"/>
+      <c r="O2719" s="90"/>
+      <c r="P2719" s="90"/>
+      <c r="Q2719" s="90"/>
+      <c r="R2719" s="90"/>
+      <c r="S2719" s="90"/>
+      <c r="T2719" s="90"/>
+      <c r="U2719" s="90"/>
+      <c r="V2719" s="90"/>
+      <c r="W2719" s="90"/>
+      <c r="X2719" s="90"/>
+      <c r="Y2719" s="90"/>
+      <c r="Z2719" s="90"/>
+      <c r="AA2719" s="90"/>
+      <c r="AB2719" s="90"/>
+      <c r="AC2719" s="90"/>
+      <c r="AD2719" s="90"/>
+      <c r="AE2719" s="90"/>
+      <c r="AF2719" s="90"/>
+      <c r="AG2719" s="90"/>
+      <c r="AH2719" s="90"/>
     </row>
     <row r="2837" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2837" s="95"/>
-      <c r="C2837" s="95"/>
-      <c r="D2837" s="95"/>
-      <c r="E2837" s="95"/>
-      <c r="F2837" s="95"/>
-      <c r="G2837" s="95"/>
-      <c r="H2837" s="95"/>
-      <c r="I2837" s="95"/>
-      <c r="J2837" s="95"/>
-      <c r="K2837" s="95"/>
-      <c r="L2837" s="95"/>
-      <c r="M2837" s="95"/>
-      <c r="N2837" s="95"/>
-      <c r="O2837" s="95"/>
-      <c r="P2837" s="95"/>
-      <c r="Q2837" s="95"/>
-      <c r="R2837" s="95"/>
-      <c r="S2837" s="95"/>
-      <c r="T2837" s="95"/>
-      <c r="U2837" s="95"/>
-      <c r="V2837" s="95"/>
-      <c r="W2837" s="95"/>
-      <c r="X2837" s="95"/>
-      <c r="Y2837" s="95"/>
-      <c r="Z2837" s="95"/>
-      <c r="AA2837" s="95"/>
-      <c r="AB2837" s="95"/>
-      <c r="AC2837" s="95"/>
-      <c r="AD2837" s="95"/>
-      <c r="AE2837" s="95"/>
-      <c r="AF2837" s="95"/>
-      <c r="AG2837" s="95"/>
-      <c r="AH2837" s="95"/>
+      <c r="B2837" s="90"/>
+      <c r="C2837" s="90"/>
+      <c r="D2837" s="90"/>
+      <c r="E2837" s="90"/>
+      <c r="F2837" s="90"/>
+      <c r="G2837" s="90"/>
+      <c r="H2837" s="90"/>
+      <c r="I2837" s="90"/>
+      <c r="J2837" s="90"/>
+      <c r="K2837" s="90"/>
+      <c r="L2837" s="90"/>
+      <c r="M2837" s="90"/>
+      <c r="N2837" s="90"/>
+      <c r="O2837" s="90"/>
+      <c r="P2837" s="90"/>
+      <c r="Q2837" s="90"/>
+      <c r="R2837" s="90"/>
+      <c r="S2837" s="90"/>
+      <c r="T2837" s="90"/>
+      <c r="U2837" s="90"/>
+      <c r="V2837" s="90"/>
+      <c r="W2837" s="90"/>
+      <c r="X2837" s="90"/>
+      <c r="Y2837" s="90"/>
+      <c r="Z2837" s="90"/>
+      <c r="AA2837" s="90"/>
+      <c r="AB2837" s="90"/>
+      <c r="AC2837" s="90"/>
+      <c r="AD2837" s="90"/>
+      <c r="AE2837" s="90"/>
+      <c r="AF2837" s="90"/>
+      <c r="AG2837" s="90"/>
+      <c r="AH2837" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B112:AH112"/>
-    <mergeCell ref="B122:AG122"/>
-    <mergeCell ref="B308:AH308"/>
-    <mergeCell ref="B511:AH511"/>
-    <mergeCell ref="B712:AH712"/>
-    <mergeCell ref="B887:AH887"/>
-    <mergeCell ref="B1100:AH1100"/>
-    <mergeCell ref="B1227:AH1227"/>
-    <mergeCell ref="B1390:AH1390"/>
-    <mergeCell ref="B1502:AH1502"/>
-    <mergeCell ref="B1604:AH1604"/>
-    <mergeCell ref="B1698:AH1698"/>
-    <mergeCell ref="B1945:AH1945"/>
-    <mergeCell ref="B2031:AH2031"/>
-    <mergeCell ref="B2719:AH2719"/>
     <mergeCell ref="B2837:AH2837"/>
     <mergeCell ref="B2153:AH2153"/>
     <mergeCell ref="B2317:AH2317"/>
     <mergeCell ref="B2419:AH2419"/>
     <mergeCell ref="B2509:AH2509"/>
     <mergeCell ref="B2598:AH2598"/>
+    <mergeCell ref="B1604:AH1604"/>
+    <mergeCell ref="B1698:AH1698"/>
+    <mergeCell ref="B1945:AH1945"/>
+    <mergeCell ref="B2031:AH2031"/>
+    <mergeCell ref="B2719:AH2719"/>
+    <mergeCell ref="B887:AH887"/>
+    <mergeCell ref="B1100:AH1100"/>
+    <mergeCell ref="B1227:AH1227"/>
+    <mergeCell ref="B1390:AH1390"/>
+    <mergeCell ref="B1502:AH1502"/>
+    <mergeCell ref="B112:AH112"/>
+    <mergeCell ref="B122:AG122"/>
+    <mergeCell ref="B308:AH308"/>
+    <mergeCell ref="B511:AH511"/>
+    <mergeCell ref="B712:AH712"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
@@ -44415,10 +44418,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AI9"/>
+  <dimension ref="A1:AJ9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AI9" sqref="AI9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44429,10 +44432,11 @@
     <col min="4" max="28" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="30" max="31" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="35" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="34" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>92</v>
       </c>
@@ -44443,7 +44447,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>94</v>
       </c>
@@ -44454,7 +44458,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -44466,17 +44470,17 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>2017</v>
       </c>
@@ -44580,7 +44584,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>97</v>
       </c>
@@ -44591,133 +44595,133 @@
         <v>0</v>
       </c>
       <c r="D9" s="9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9">
         <f>$B$3*('AEO Table 5'!C61/'AEO Table 5'!$C61)</f>
         <v>336352809191520</v>
       </c>
-      <c r="E9" s="9">
+      <c r="F9" s="9">
         <f>$B$3*('AEO Table 5'!D61/'AEO Table 5'!$C61)</f>
         <v>348233022820383.44</v>
       </c>
-      <c r="F9" s="9">
+      <c r="G9" s="9">
         <f>$B$3*('AEO Table 5'!E61/'AEO Table 5'!$C61)</f>
         <v>347221008177414</v>
       </c>
-      <c r="G9" s="9">
+      <c r="H9" s="9">
         <f>$B$3*('AEO Table 5'!F61/'AEO Table 5'!$C61)</f>
         <v>347869235071709.25</v>
       </c>
-      <c r="H9" s="9">
+      <c r="I9" s="9">
         <f>$B$3*('AEO Table 5'!G61/'AEO Table 5'!$C61)</f>
         <v>350786576050082.56</v>
       </c>
-      <c r="I9" s="9">
+      <c r="J9" s="9">
         <f>$B$3*('AEO Table 5'!H61/'AEO Table 5'!$C61)</f>
         <v>352843560602611.69</v>
       </c>
-      <c r="J9" s="9">
+      <c r="K9" s="9">
         <f>$B$3*('AEO Table 5'!I61/'AEO Table 5'!$C61)</f>
         <v>353347488222806.69</v>
       </c>
-      <c r="K9" s="9">
+      <c r="L9" s="9">
         <f>$B$3*('AEO Table 5'!J61/'AEO Table 5'!$C61)</f>
         <v>352608394379854</v>
       </c>
-      <c r="L9" s="9">
+      <c r="M9" s="9">
         <f>$B$3*('AEO Table 5'!K61/'AEO Table 5'!$C61)</f>
         <v>351575582723987.81</v>
       </c>
-      <c r="M9" s="9">
+      <c r="N9" s="9">
         <f>$B$3*('AEO Table 5'!L61/'AEO Table 5'!$C61)</f>
         <v>349976132455191.19</v>
       </c>
-      <c r="N9" s="9">
+      <c r="O9" s="9">
         <f>$B$3*('AEO Table 5'!M61/'AEO Table 5'!$C61)</f>
         <v>347839159391519.88</v>
       </c>
-      <c r="O9" s="9">
+      <c r="P9" s="9">
         <f>$B$3*('AEO Table 5'!N61/'AEO Table 5'!$C61)</f>
         <v>346373289936330.5</v>
       </c>
-      <c r="P9" s="9">
+      <c r="Q9" s="9">
         <f>$B$3*('AEO Table 5'!O61/'AEO Table 5'!$C61)</f>
         <v>345300484024893.13</v>
       </c>
-      <c r="Q9" s="9">
+      <c r="R9" s="9">
         <f>$B$3*('AEO Table 5'!P61/'AEO Table 5'!$C61)</f>
         <v>344274711358007.38</v>
       </c>
-      <c r="R9" s="9">
+      <c r="S9" s="9">
         <f>$B$3*('AEO Table 5'!Q61/'AEO Table 5'!$C61)</f>
         <v>343328607248219.06</v>
       </c>
-      <c r="S9" s="9">
+      <c r="T9" s="9">
         <f>$B$3*('AEO Table 5'!R61/'AEO Table 5'!$C61)</f>
         <v>342625668212302.69</v>
       </c>
-      <c r="T9" s="9">
+      <c r="U9" s="9">
         <f>$B$3*('AEO Table 5'!S61/'AEO Table 5'!$C61)</f>
         <v>341985280192099.31</v>
       </c>
-      <c r="U9" s="9">
+      <c r="V9" s="9">
         <f>$B$3*('AEO Table 5'!T61/'AEO Table 5'!$C61)</f>
         <v>341153399676221.88</v>
       </c>
-      <c r="V9" s="9">
+      <c r="W9" s="9">
         <f>$B$3*('AEO Table 5'!U61/'AEO Table 5'!$C61)</f>
         <v>340303281779804</v>
       </c>
-      <c r="W9" s="9">
+      <c r="X9" s="9">
         <f>$B$3*('AEO Table 5'!V61/'AEO Table 5'!$C61)</f>
         <v>339511715473542.25</v>
       </c>
-      <c r="X9" s="9">
+      <c r="Y9" s="9">
         <f>$B$3*('AEO Table 5'!W61/'AEO Table 5'!$C61)</f>
         <v>338614084401506</v>
       </c>
-      <c r="Y9" s="9">
+      <c r="Z9" s="9">
         <f>$B$3*('AEO Table 5'!X61/'AEO Table 5'!$C61)</f>
         <v>337634545094060.38</v>
       </c>
-      <c r="Z9" s="9">
+      <c r="AA9" s="9">
         <f>$B$3*('AEO Table 5'!Y61/'AEO Table 5'!$C61)</f>
         <v>336460633704539.5</v>
       </c>
-      <c r="AA9" s="9">
+      <c r="AB9" s="9">
         <f>$B$3*('AEO Table 5'!Z61/'AEO Table 5'!$C61)</f>
         <v>335200334722985.19</v>
       </c>
-      <c r="AB9" s="9">
+      <c r="AC9" s="9">
         <f>$B$3*('AEO Table 5'!AA61/'AEO Table 5'!$C61)</f>
         <v>333844849413171.81</v>
       </c>
-      <c r="AC9" s="9">
+      <c r="AD9" s="9">
         <f>$B$3*('AEO Table 5'!AB61/'AEO Table 5'!$C61)</f>
         <v>332403136488347.38</v>
       </c>
-      <c r="AD9" s="9">
+      <c r="AE9" s="9">
         <f>$B$3*('AEO Table 5'!AC61/'AEO Table 5'!$C61)</f>
         <v>331004937313584.13</v>
       </c>
-      <c r="AE9" s="9">
+      <c r="AF9" s="9">
         <f>$B$3*('AEO Table 5'!AD61/'AEO Table 5'!$C61)</f>
         <v>329646412440347.31</v>
       </c>
-      <c r="AF9" s="9">
+      <c r="AG9" s="9">
         <f>$B$3*('AEO Table 5'!AE61/'AEO Table 5'!$C61)</f>
         <v>328457943141798.63</v>
       </c>
-      <c r="AG9" s="9">
+      <c r="AH9" s="9">
         <f>$B$3*('AEO Table 5'!AF61/'AEO Table 5'!$C61)</f>
         <v>327133493374308.38</v>
       </c>
-      <c r="AH9" s="9">
+      <c r="AI9" s="9">
         <f>$B$3*('AEO Table 5'!AG61/'AEO Table 5'!$C61)</f>
         <v>325590674971400.31</v>
       </c>
-      <c r="AI9" s="9">
-        <f>$B$3*('AEO Table 5'!AH61/'AEO Table 5'!$C61)</f>
-        <v>-173255115133.70282</v>
-      </c>
+      <c r="AJ9" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -51568,8 +51572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AO195"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="P188" sqref="P188"/>
+    <sheetView topLeftCell="I127" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K138" sqref="K138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63825,11 +63829,11 @@
       </c>
       <c r="J134" s="55"/>
       <c r="K134" s="55">
-        <f t="shared" ref="K134:AO134" si="36">INDEX(Table5,MATCH($H134,Table5_A,0),MATCH(K$133,Table5_1,0))*quadrillion</f>
+        <f>INDEX(Table5,MATCH($H134,Table5_A,0),MATCH(K$133,Table5_1,0))*quadrillion</f>
         <v>113108000000000</v>
       </c>
       <c r="L134" s="55">
-        <f t="shared" si="36"/>
+        <f t="shared" ref="K134:AO134" si="36">INDEX(Table5,MATCH($H134,Table5_A,0),MATCH(L$133,Table5_1,0))*quadrillion</f>
         <v>115901000000000</v>
       </c>
       <c r="M134" s="55">
@@ -64321,127 +64325,127 @@
       <c r="J138" s="56"/>
       <c r="K138" s="56">
         <f>'District Heat'!E9</f>
-        <v>348233022820383.44</v>
+        <v>336352809191520</v>
       </c>
       <c r="L138" s="56">
         <f>'District Heat'!F9</f>
-        <v>347221008177414</v>
+        <v>348233022820383.44</v>
       </c>
       <c r="M138" s="56">
         <f>'District Heat'!G9</f>
-        <v>347869235071709.25</v>
+        <v>347221008177414</v>
       </c>
       <c r="N138" s="56">
         <f>'District Heat'!H9</f>
-        <v>350786576050082.56</v>
+        <v>347869235071709.25</v>
       </c>
       <c r="O138" s="56">
         <f>'District Heat'!I9</f>
-        <v>352843560602611.69</v>
+        <v>350786576050082.56</v>
       </c>
       <c r="P138" s="56">
         <f>'District Heat'!J9</f>
-        <v>353347488222806.69</v>
+        <v>352843560602611.69</v>
       </c>
       <c r="Q138" s="56">
         <f>'District Heat'!K9</f>
-        <v>352608394379854</v>
+        <v>353347488222806.69</v>
       </c>
       <c r="R138" s="56">
         <f>'District Heat'!L9</f>
-        <v>351575582723987.81</v>
+        <v>352608394379854</v>
       </c>
       <c r="S138" s="56">
         <f>'District Heat'!M9</f>
-        <v>349976132455191.19</v>
+        <v>351575582723987.81</v>
       </c>
       <c r="T138" s="56">
         <f>'District Heat'!N9</f>
-        <v>347839159391519.88</v>
+        <v>349976132455191.19</v>
       </c>
       <c r="U138" s="56">
         <f>'District Heat'!O9</f>
-        <v>346373289936330.5</v>
+        <v>347839159391519.88</v>
       </c>
       <c r="V138" s="56">
         <f>'District Heat'!P9</f>
-        <v>345300484024893.13</v>
+        <v>346373289936330.5</v>
       </c>
       <c r="W138" s="56">
         <f>'District Heat'!Q9</f>
-        <v>344274711358007.38</v>
+        <v>345300484024893.13</v>
       </c>
       <c r="X138" s="56">
         <f>'District Heat'!R9</f>
-        <v>343328607248219.06</v>
+        <v>344274711358007.38</v>
       </c>
       <c r="Y138" s="56">
         <f>'District Heat'!S9</f>
-        <v>342625668212302.69</v>
+        <v>343328607248219.06</v>
       </c>
       <c r="Z138" s="56">
         <f>'District Heat'!T9</f>
-        <v>341985280192099.31</v>
+        <v>342625668212302.69</v>
       </c>
       <c r="AA138" s="56">
         <f>'District Heat'!U9</f>
-        <v>341153399676221.88</v>
+        <v>341985280192099.31</v>
       </c>
       <c r="AB138" s="56">
         <f>'District Heat'!V9</f>
-        <v>340303281779804</v>
+        <v>341153399676221.88</v>
       </c>
       <c r="AC138" s="56">
         <f>'District Heat'!W9</f>
-        <v>339511715473542.25</v>
+        <v>340303281779804</v>
       </c>
       <c r="AD138" s="56">
         <f>'District Heat'!X9</f>
-        <v>338614084401506</v>
+        <v>339511715473542.25</v>
       </c>
       <c r="AE138" s="56">
         <f>'District Heat'!Y9</f>
-        <v>337634545094060.38</v>
+        <v>338614084401506</v>
       </c>
       <c r="AF138" s="56">
         <f>'District Heat'!Z9</f>
-        <v>336460633704539.5</v>
+        <v>337634545094060.38</v>
       </c>
       <c r="AG138" s="56">
         <f>'District Heat'!AA9</f>
-        <v>335200334722985.19</v>
+        <v>336460633704539.5</v>
       </c>
       <c r="AH138" s="56">
         <f>'District Heat'!AB9</f>
-        <v>333844849413171.81</v>
+        <v>335200334722985.19</v>
       </c>
       <c r="AI138" s="56">
         <f>'District Heat'!AC9</f>
-        <v>332403136488347.38</v>
+        <v>333844849413171.81</v>
       </c>
       <c r="AJ138" s="56">
         <f>'District Heat'!AD9</f>
-        <v>331004937313584.13</v>
+        <v>332403136488347.38</v>
       </c>
       <c r="AK138" s="56">
         <f>'District Heat'!AE9</f>
-        <v>329646412440347.31</v>
+        <v>331004937313584.13</v>
       </c>
       <c r="AL138" s="56">
         <f>'District Heat'!AF9</f>
-        <v>328457943141798.63</v>
+        <v>329646412440347.31</v>
       </c>
       <c r="AM138" s="56">
         <f>'District Heat'!AG9</f>
-        <v>327133493374308.38</v>
+        <v>328457943141798.63</v>
       </c>
       <c r="AN138" s="56">
         <f>'District Heat'!AH9</f>
-        <v>325590674971400.31</v>
+        <v>327133493374308.38</v>
       </c>
       <c r="AO138" s="56">
         <f>'District Heat'!AI9</f>
-        <v>-173255115133.70282</v>
+        <v>325590674971400.31</v>
       </c>
     </row>
     <row r="139" spans="1:41" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update bceu, adjust for water and wastewater
</commit_message>
<xml_diff>
--- a/InputData/bldgs/BCEU/BAU Components Energy Use.xlsx
+++ b/InputData/bldgs/BCEU/BAU Components Energy Use.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\US-EPS\InputData\bldgs\BCEU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\US-eps\InputData\bldgs\BCEU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CFE285-42E5-4D1D-ABB5-32CA823875EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBFA21F-DD65-4EF2-925F-D157A572F55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7320" yWindow="1005" windowWidth="19710" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="AEO Table 5" sheetId="29" r:id="rId3"/>
     <sheet name="District Heat" sheetId="19" r:id="rId4"/>
     <sheet name="RECS HC2.1" sheetId="22" r:id="rId5"/>
-    <sheet name="Water and Waste" sheetId="32" r:id="rId6"/>
+    <sheet name="Water and Waste" sheetId="33" r:id="rId6"/>
     <sheet name="Calculations" sheetId="30" r:id="rId7"/>
     <sheet name="BCEU-urban-residential-heating" sheetId="18" r:id="rId8"/>
     <sheet name="BCEU-urban-residential-cooling" sheetId="20" r:id="rId9"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1841" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="659">
   <si>
     <t>Sources:</t>
   </si>
@@ -2157,12 +2157,6 @@
     <t>U.S. Population</t>
   </si>
   <si>
-    <t>U.S. Population (2010)</t>
-  </si>
-  <si>
-    <t>2010 Primary Energy (assumed to be elec.)</t>
-  </si>
-  <si>
     <t>Primary Energy Use (assumed to be elec.)</t>
   </si>
   <si>
@@ -2171,18 +2165,31 @@
   <si>
     <t>Commercial electricity consumption includes electricity used for water and waste facilities. In the EPS model, these are included in the industrial fuel use. To avoid double counting, we removed water and waste electricity consumption from commercial-other.</t>
   </si>
+  <si>
+    <t>btu per kwh</t>
+  </si>
+  <si>
+    <t>U.S. Population (2000)</t>
+  </si>
+  <si>
+    <t>2000 Primary Energy (assumed to be elec.) kwh</t>
+  </si>
+  <si>
+    <t>2001 Primary Energy (assumed to be elec.) btu</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.000E+00"/>
     <numFmt numFmtId="167" formatCode="@*."/>
     <numFmt numFmtId="168" formatCode="#,##0.0"/>
+    <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28" x14ac:knownFonts="1">
     <font>
@@ -2378,7 +2385,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2423,7 +2430,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2593,7 +2606,7 @@
     </xf>
     <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2806,7 +2819,8 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="5">
       <alignment wrapText="1"/>
     </xf>
@@ -2820,7 +2834,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="4" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2848,6 +2861,13 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="16" fillId="0" borderId="0" xfId="17" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="11" fontId="16" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -5869,6 +5889,55 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>589734</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>18306</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9ACE5179-3382-4D6A-AA95-DF9D4AB09C50}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="247650" y="3590925"/>
+          <a:ext cx="6523809" cy="5952381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
@@ -6298,8 +6367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6647,12 +6716,12 @@
     </row>
     <row r="75" spans="1:1" s="90" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="76" spans="1:1" s="90" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="90" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="77" spans="1:1" s="90" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -29708,103 +29777,103 @@
       <c r="A112" s="14" t="s">
         <v>446</v>
       </c>
-      <c r="B112" s="98" t="s">
+      <c r="B112" s="99" t="s">
         <v>591</v>
       </c>
-      <c r="C112" s="99">
+      <c r="C112" s="100">
         <v>21.012035000000001</v>
       </c>
-      <c r="D112" s="99">
+      <c r="D112" s="100">
         <v>21.043247000000001</v>
       </c>
-      <c r="E112" s="99">
+      <c r="E112" s="100">
         <v>21.216681999999999</v>
       </c>
-      <c r="F112" s="99">
+      <c r="F112" s="100">
         <v>21.018280000000001</v>
       </c>
-      <c r="G112" s="99">
+      <c r="G112" s="100">
         <v>20.85379</v>
       </c>
-      <c r="H112" s="99">
+      <c r="H112" s="100">
         <v>20.627789</v>
       </c>
-      <c r="I112" s="99">
+      <c r="I112" s="100">
         <v>20.385228999999999</v>
       </c>
-      <c r="J112" s="99">
+      <c r="J112" s="100">
         <v>20.220219</v>
       </c>
-      <c r="K112" s="99">
+      <c r="K112" s="100">
         <v>20.168883999999998</v>
       </c>
-      <c r="L112" s="99">
+      <c r="L112" s="100">
         <v>20.144856999999998</v>
       </c>
-      <c r="M112" s="99">
+      <c r="M112" s="100">
         <v>20.183903000000001</v>
       </c>
-      <c r="N112" s="99">
+      <c r="N112" s="100">
         <v>20.200790000000001</v>
       </c>
-      <c r="O112" s="99">
+      <c r="O112" s="100">
         <v>20.210455</v>
       </c>
-      <c r="P112" s="99">
+      <c r="P112" s="100">
         <v>20.251712999999999</v>
       </c>
-      <c r="Q112" s="99">
+      <c r="Q112" s="100">
         <v>20.298100000000002</v>
       </c>
-      <c r="R112" s="99">
+      <c r="R112" s="100">
         <v>20.374268000000001</v>
       </c>
-      <c r="S112" s="99">
+      <c r="S112" s="100">
         <v>20.453151999999999</v>
       </c>
-      <c r="T112" s="99">
+      <c r="T112" s="100">
         <v>20.522358000000001</v>
       </c>
-      <c r="U112" s="99">
+      <c r="U112" s="100">
         <v>20.597715000000001</v>
       </c>
-      <c r="V112" s="99">
+      <c r="V112" s="100">
         <v>20.691054999999999</v>
       </c>
-      <c r="W112" s="99">
+      <c r="W112" s="100">
         <v>20.79027</v>
       </c>
-      <c r="X112" s="99">
+      <c r="X112" s="100">
         <v>20.887352</v>
       </c>
-      <c r="Y112" s="99">
+      <c r="Y112" s="100">
         <v>20.988150000000001</v>
       </c>
-      <c r="Z112" s="99">
+      <c r="Z112" s="100">
         <v>21.068726000000002</v>
       </c>
-      <c r="AA112" s="99">
+      <c r="AA112" s="100">
         <v>21.118212</v>
       </c>
-      <c r="AB112" s="99">
+      <c r="AB112" s="100">
         <v>21.216028000000001</v>
       </c>
-      <c r="AC112" s="99">
+      <c r="AC112" s="100">
         <v>21.321000999999999</v>
       </c>
-      <c r="AD112" s="99">
+      <c r="AD112" s="100">
         <v>21.423819999999999</v>
       </c>
-      <c r="AE112" s="99">
+      <c r="AE112" s="100">
         <v>21.530754000000002</v>
       </c>
-      <c r="AF112" s="99">
+      <c r="AF112" s="100">
         <v>21.665205</v>
       </c>
-      <c r="AG112" s="99">
+      <c r="AG112" s="100">
         <v>21.802175999999999</v>
       </c>
-      <c r="AH112" s="100">
+      <c r="AH112" s="101">
         <v>1.2310000000000001E-3</v>
       </c>
     </row>
@@ -32633,40 +32702,40 @@
     </row>
     <row r="146" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="147" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B147" s="101" t="s">
+      <c r="B147" s="102" t="s">
         <v>597</v>
       </c>
-      <c r="C147" s="102"/>
-      <c r="D147" s="102"/>
-      <c r="E147" s="102"/>
-      <c r="F147" s="102"/>
-      <c r="G147" s="102"/>
-      <c r="H147" s="102"/>
-      <c r="I147" s="102"/>
-      <c r="J147" s="102"/>
-      <c r="K147" s="102"/>
-      <c r="L147" s="102"/>
-      <c r="M147" s="102"/>
-      <c r="N147" s="102"/>
-      <c r="O147" s="102"/>
-      <c r="P147" s="102"/>
-      <c r="Q147" s="102"/>
-      <c r="R147" s="102"/>
-      <c r="S147" s="102"/>
-      <c r="T147" s="102"/>
-      <c r="U147" s="102"/>
-      <c r="V147" s="102"/>
-      <c r="W147" s="102"/>
-      <c r="X147" s="102"/>
-      <c r="Y147" s="102"/>
-      <c r="Z147" s="102"/>
-      <c r="AA147" s="102"/>
-      <c r="AB147" s="102"/>
-      <c r="AC147" s="102"/>
-      <c r="AD147" s="102"/>
-      <c r="AE147" s="102"/>
-      <c r="AF147" s="102"/>
-      <c r="AG147" s="102"/>
+      <c r="C147" s="103"/>
+      <c r="D147" s="103"/>
+      <c r="E147" s="103"/>
+      <c r="F147" s="103"/>
+      <c r="G147" s="103"/>
+      <c r="H147" s="103"/>
+      <c r="I147" s="103"/>
+      <c r="J147" s="103"/>
+      <c r="K147" s="103"/>
+      <c r="L147" s="103"/>
+      <c r="M147" s="103"/>
+      <c r="N147" s="103"/>
+      <c r="O147" s="103"/>
+      <c r="P147" s="103"/>
+      <c r="Q147" s="103"/>
+      <c r="R147" s="103"/>
+      <c r="S147" s="103"/>
+      <c r="T147" s="103"/>
+      <c r="U147" s="103"/>
+      <c r="V147" s="103"/>
+      <c r="W147" s="103"/>
+      <c r="X147" s="103"/>
+      <c r="Y147" s="103"/>
+      <c r="Z147" s="103"/>
+      <c r="AA147" s="103"/>
+      <c r="AB147" s="103"/>
+      <c r="AC147" s="103"/>
+      <c r="AD147" s="103"/>
+      <c r="AE147" s="103"/>
+      <c r="AF147" s="103"/>
+      <c r="AG147" s="103"/>
       <c r="AH147" s="77"/>
     </row>
     <row r="148" spans="1:34" x14ac:dyDescent="0.25">
@@ -32770,693 +32839,693 @@
       </c>
     </row>
     <row r="308" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B308" s="103"/>
-      <c r="C308" s="103"/>
-      <c r="D308" s="103"/>
-      <c r="E308" s="103"/>
-      <c r="F308" s="103"/>
-      <c r="G308" s="103"/>
-      <c r="H308" s="103"/>
-      <c r="I308" s="103"/>
-      <c r="J308" s="103"/>
-      <c r="K308" s="103"/>
-      <c r="L308" s="103"/>
-      <c r="M308" s="103"/>
-      <c r="N308" s="103"/>
-      <c r="O308" s="103"/>
-      <c r="P308" s="103"/>
-      <c r="Q308" s="103"/>
-      <c r="R308" s="103"/>
-      <c r="S308" s="103"/>
-      <c r="T308" s="103"/>
-      <c r="U308" s="103"/>
-      <c r="V308" s="103"/>
-      <c r="W308" s="103"/>
-      <c r="X308" s="103"/>
-      <c r="Y308" s="103"/>
-      <c r="Z308" s="103"/>
-      <c r="AA308" s="103"/>
-      <c r="AB308" s="103"/>
-      <c r="AC308" s="103"/>
-      <c r="AD308" s="103"/>
-      <c r="AE308" s="103"/>
-      <c r="AF308" s="103"/>
-      <c r="AG308" s="103"/>
-      <c r="AH308" s="103"/>
+      <c r="B308" s="98"/>
+      <c r="C308" s="98"/>
+      <c r="D308" s="98"/>
+      <c r="E308" s="98"/>
+      <c r="F308" s="98"/>
+      <c r="G308" s="98"/>
+      <c r="H308" s="98"/>
+      <c r="I308" s="98"/>
+      <c r="J308" s="98"/>
+      <c r="K308" s="98"/>
+      <c r="L308" s="98"/>
+      <c r="M308" s="98"/>
+      <c r="N308" s="98"/>
+      <c r="O308" s="98"/>
+      <c r="P308" s="98"/>
+      <c r="Q308" s="98"/>
+      <c r="R308" s="98"/>
+      <c r="S308" s="98"/>
+      <c r="T308" s="98"/>
+      <c r="U308" s="98"/>
+      <c r="V308" s="98"/>
+      <c r="W308" s="98"/>
+      <c r="X308" s="98"/>
+      <c r="Y308" s="98"/>
+      <c r="Z308" s="98"/>
+      <c r="AA308" s="98"/>
+      <c r="AB308" s="98"/>
+      <c r="AC308" s="98"/>
+      <c r="AD308" s="98"/>
+      <c r="AE308" s="98"/>
+      <c r="AF308" s="98"/>
+      <c r="AG308" s="98"/>
+      <c r="AH308" s="98"/>
     </row>
     <row r="511" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B511" s="103"/>
-      <c r="C511" s="103"/>
-      <c r="D511" s="103"/>
-      <c r="E511" s="103"/>
-      <c r="F511" s="103"/>
-      <c r="G511" s="103"/>
-      <c r="H511" s="103"/>
-      <c r="I511" s="103"/>
-      <c r="J511" s="103"/>
-      <c r="K511" s="103"/>
-      <c r="L511" s="103"/>
-      <c r="M511" s="103"/>
-      <c r="N511" s="103"/>
-      <c r="O511" s="103"/>
-      <c r="P511" s="103"/>
-      <c r="Q511" s="103"/>
-      <c r="R511" s="103"/>
-      <c r="S511" s="103"/>
-      <c r="T511" s="103"/>
-      <c r="U511" s="103"/>
-      <c r="V511" s="103"/>
-      <c r="W511" s="103"/>
-      <c r="X511" s="103"/>
-      <c r="Y511" s="103"/>
-      <c r="Z511" s="103"/>
-      <c r="AA511" s="103"/>
-      <c r="AB511" s="103"/>
-      <c r="AC511" s="103"/>
-      <c r="AD511" s="103"/>
-      <c r="AE511" s="103"/>
-      <c r="AF511" s="103"/>
-      <c r="AG511" s="103"/>
-      <c r="AH511" s="103"/>
+      <c r="B511" s="98"/>
+      <c r="C511" s="98"/>
+      <c r="D511" s="98"/>
+      <c r="E511" s="98"/>
+      <c r="F511" s="98"/>
+      <c r="G511" s="98"/>
+      <c r="H511" s="98"/>
+      <c r="I511" s="98"/>
+      <c r="J511" s="98"/>
+      <c r="K511" s="98"/>
+      <c r="L511" s="98"/>
+      <c r="M511" s="98"/>
+      <c r="N511" s="98"/>
+      <c r="O511" s="98"/>
+      <c r="P511" s="98"/>
+      <c r="Q511" s="98"/>
+      <c r="R511" s="98"/>
+      <c r="S511" s="98"/>
+      <c r="T511" s="98"/>
+      <c r="U511" s="98"/>
+      <c r="V511" s="98"/>
+      <c r="W511" s="98"/>
+      <c r="X511" s="98"/>
+      <c r="Y511" s="98"/>
+      <c r="Z511" s="98"/>
+      <c r="AA511" s="98"/>
+      <c r="AB511" s="98"/>
+      <c r="AC511" s="98"/>
+      <c r="AD511" s="98"/>
+      <c r="AE511" s="98"/>
+      <c r="AF511" s="98"/>
+      <c r="AG511" s="98"/>
+      <c r="AH511" s="98"/>
     </row>
     <row r="712" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B712" s="103"/>
-      <c r="C712" s="103"/>
-      <c r="D712" s="103"/>
-      <c r="E712" s="103"/>
-      <c r="F712" s="103"/>
-      <c r="G712" s="103"/>
-      <c r="H712" s="103"/>
-      <c r="I712" s="103"/>
-      <c r="J712" s="103"/>
-      <c r="K712" s="103"/>
-      <c r="L712" s="103"/>
-      <c r="M712" s="103"/>
-      <c r="N712" s="103"/>
-      <c r="O712" s="103"/>
-      <c r="P712" s="103"/>
-      <c r="Q712" s="103"/>
-      <c r="R712" s="103"/>
-      <c r="S712" s="103"/>
-      <c r="T712" s="103"/>
-      <c r="U712" s="103"/>
-      <c r="V712" s="103"/>
-      <c r="W712" s="103"/>
-      <c r="X712" s="103"/>
-      <c r="Y712" s="103"/>
-      <c r="Z712" s="103"/>
-      <c r="AA712" s="103"/>
-      <c r="AB712" s="103"/>
-      <c r="AC712" s="103"/>
-      <c r="AD712" s="103"/>
-      <c r="AE712" s="103"/>
-      <c r="AF712" s="103"/>
-      <c r="AG712" s="103"/>
-      <c r="AH712" s="103"/>
+      <c r="B712" s="98"/>
+      <c r="C712" s="98"/>
+      <c r="D712" s="98"/>
+      <c r="E712" s="98"/>
+      <c r="F712" s="98"/>
+      <c r="G712" s="98"/>
+      <c r="H712" s="98"/>
+      <c r="I712" s="98"/>
+      <c r="J712" s="98"/>
+      <c r="K712" s="98"/>
+      <c r="L712" s="98"/>
+      <c r="M712" s="98"/>
+      <c r="N712" s="98"/>
+      <c r="O712" s="98"/>
+      <c r="P712" s="98"/>
+      <c r="Q712" s="98"/>
+      <c r="R712" s="98"/>
+      <c r="S712" s="98"/>
+      <c r="T712" s="98"/>
+      <c r="U712" s="98"/>
+      <c r="V712" s="98"/>
+      <c r="W712" s="98"/>
+      <c r="X712" s="98"/>
+      <c r="Y712" s="98"/>
+      <c r="Z712" s="98"/>
+      <c r="AA712" s="98"/>
+      <c r="AB712" s="98"/>
+      <c r="AC712" s="98"/>
+      <c r="AD712" s="98"/>
+      <c r="AE712" s="98"/>
+      <c r="AF712" s="98"/>
+      <c r="AG712" s="98"/>
+      <c r="AH712" s="98"/>
     </row>
     <row r="887" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B887" s="103"/>
-      <c r="C887" s="103"/>
-      <c r="D887" s="103"/>
-      <c r="E887" s="103"/>
-      <c r="F887" s="103"/>
-      <c r="G887" s="103"/>
-      <c r="H887" s="103"/>
-      <c r="I887" s="103"/>
-      <c r="J887" s="103"/>
-      <c r="K887" s="103"/>
-      <c r="L887" s="103"/>
-      <c r="M887" s="103"/>
-      <c r="N887" s="103"/>
-      <c r="O887" s="103"/>
-      <c r="P887" s="103"/>
-      <c r="Q887" s="103"/>
-      <c r="R887" s="103"/>
-      <c r="S887" s="103"/>
-      <c r="T887" s="103"/>
-      <c r="U887" s="103"/>
-      <c r="V887" s="103"/>
-      <c r="W887" s="103"/>
-      <c r="X887" s="103"/>
-      <c r="Y887" s="103"/>
-      <c r="Z887" s="103"/>
-      <c r="AA887" s="103"/>
-      <c r="AB887" s="103"/>
-      <c r="AC887" s="103"/>
-      <c r="AD887" s="103"/>
-      <c r="AE887" s="103"/>
-      <c r="AF887" s="103"/>
-      <c r="AG887" s="103"/>
-      <c r="AH887" s="103"/>
+      <c r="B887" s="98"/>
+      <c r="C887" s="98"/>
+      <c r="D887" s="98"/>
+      <c r="E887" s="98"/>
+      <c r="F887" s="98"/>
+      <c r="G887" s="98"/>
+      <c r="H887" s="98"/>
+      <c r="I887" s="98"/>
+      <c r="J887" s="98"/>
+      <c r="K887" s="98"/>
+      <c r="L887" s="98"/>
+      <c r="M887" s="98"/>
+      <c r="N887" s="98"/>
+      <c r="O887" s="98"/>
+      <c r="P887" s="98"/>
+      <c r="Q887" s="98"/>
+      <c r="R887" s="98"/>
+      <c r="S887" s="98"/>
+      <c r="T887" s="98"/>
+      <c r="U887" s="98"/>
+      <c r="V887" s="98"/>
+      <c r="W887" s="98"/>
+      <c r="X887" s="98"/>
+      <c r="Y887" s="98"/>
+      <c r="Z887" s="98"/>
+      <c r="AA887" s="98"/>
+      <c r="AB887" s="98"/>
+      <c r="AC887" s="98"/>
+      <c r="AD887" s="98"/>
+      <c r="AE887" s="98"/>
+      <c r="AF887" s="98"/>
+      <c r="AG887" s="98"/>
+      <c r="AH887" s="98"/>
     </row>
     <row r="1100" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1100" s="103"/>
-      <c r="C1100" s="103"/>
-      <c r="D1100" s="103"/>
-      <c r="E1100" s="103"/>
-      <c r="F1100" s="103"/>
-      <c r="G1100" s="103"/>
-      <c r="H1100" s="103"/>
-      <c r="I1100" s="103"/>
-      <c r="J1100" s="103"/>
-      <c r="K1100" s="103"/>
-      <c r="L1100" s="103"/>
-      <c r="M1100" s="103"/>
-      <c r="N1100" s="103"/>
-      <c r="O1100" s="103"/>
-      <c r="P1100" s="103"/>
-      <c r="Q1100" s="103"/>
-      <c r="R1100" s="103"/>
-      <c r="S1100" s="103"/>
-      <c r="T1100" s="103"/>
-      <c r="U1100" s="103"/>
-      <c r="V1100" s="103"/>
-      <c r="W1100" s="103"/>
-      <c r="X1100" s="103"/>
-      <c r="Y1100" s="103"/>
-      <c r="Z1100" s="103"/>
-      <c r="AA1100" s="103"/>
-      <c r="AB1100" s="103"/>
-      <c r="AC1100" s="103"/>
-      <c r="AD1100" s="103"/>
-      <c r="AE1100" s="103"/>
-      <c r="AF1100" s="103"/>
-      <c r="AG1100" s="103"/>
-      <c r="AH1100" s="103"/>
+      <c r="B1100" s="98"/>
+      <c r="C1100" s="98"/>
+      <c r="D1100" s="98"/>
+      <c r="E1100" s="98"/>
+      <c r="F1100" s="98"/>
+      <c r="G1100" s="98"/>
+      <c r="H1100" s="98"/>
+      <c r="I1100" s="98"/>
+      <c r="J1100" s="98"/>
+      <c r="K1100" s="98"/>
+      <c r="L1100" s="98"/>
+      <c r="M1100" s="98"/>
+      <c r="N1100" s="98"/>
+      <c r="O1100" s="98"/>
+      <c r="P1100" s="98"/>
+      <c r="Q1100" s="98"/>
+      <c r="R1100" s="98"/>
+      <c r="S1100" s="98"/>
+      <c r="T1100" s="98"/>
+      <c r="U1100" s="98"/>
+      <c r="V1100" s="98"/>
+      <c r="W1100" s="98"/>
+      <c r="X1100" s="98"/>
+      <c r="Y1100" s="98"/>
+      <c r="Z1100" s="98"/>
+      <c r="AA1100" s="98"/>
+      <c r="AB1100" s="98"/>
+      <c r="AC1100" s="98"/>
+      <c r="AD1100" s="98"/>
+      <c r="AE1100" s="98"/>
+      <c r="AF1100" s="98"/>
+      <c r="AG1100" s="98"/>
+      <c r="AH1100" s="98"/>
     </row>
     <row r="1227" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1227" s="103"/>
-      <c r="C1227" s="103"/>
-      <c r="D1227" s="103"/>
-      <c r="E1227" s="103"/>
-      <c r="F1227" s="103"/>
-      <c r="G1227" s="103"/>
-      <c r="H1227" s="103"/>
-      <c r="I1227" s="103"/>
-      <c r="J1227" s="103"/>
-      <c r="K1227" s="103"/>
-      <c r="L1227" s="103"/>
-      <c r="M1227" s="103"/>
-      <c r="N1227" s="103"/>
-      <c r="O1227" s="103"/>
-      <c r="P1227" s="103"/>
-      <c r="Q1227" s="103"/>
-      <c r="R1227" s="103"/>
-      <c r="S1227" s="103"/>
-      <c r="T1227" s="103"/>
-      <c r="U1227" s="103"/>
-      <c r="V1227" s="103"/>
-      <c r="W1227" s="103"/>
-      <c r="X1227" s="103"/>
-      <c r="Y1227" s="103"/>
-      <c r="Z1227" s="103"/>
-      <c r="AA1227" s="103"/>
-      <c r="AB1227" s="103"/>
-      <c r="AC1227" s="103"/>
-      <c r="AD1227" s="103"/>
-      <c r="AE1227" s="103"/>
-      <c r="AF1227" s="103"/>
-      <c r="AG1227" s="103"/>
-      <c r="AH1227" s="103"/>
+      <c r="B1227" s="98"/>
+      <c r="C1227" s="98"/>
+      <c r="D1227" s="98"/>
+      <c r="E1227" s="98"/>
+      <c r="F1227" s="98"/>
+      <c r="G1227" s="98"/>
+      <c r="H1227" s="98"/>
+      <c r="I1227" s="98"/>
+      <c r="J1227" s="98"/>
+      <c r="K1227" s="98"/>
+      <c r="L1227" s="98"/>
+      <c r="M1227" s="98"/>
+      <c r="N1227" s="98"/>
+      <c r="O1227" s="98"/>
+      <c r="P1227" s="98"/>
+      <c r="Q1227" s="98"/>
+      <c r="R1227" s="98"/>
+      <c r="S1227" s="98"/>
+      <c r="T1227" s="98"/>
+      <c r="U1227" s="98"/>
+      <c r="V1227" s="98"/>
+      <c r="W1227" s="98"/>
+      <c r="X1227" s="98"/>
+      <c r="Y1227" s="98"/>
+      <c r="Z1227" s="98"/>
+      <c r="AA1227" s="98"/>
+      <c r="AB1227" s="98"/>
+      <c r="AC1227" s="98"/>
+      <c r="AD1227" s="98"/>
+      <c r="AE1227" s="98"/>
+      <c r="AF1227" s="98"/>
+      <c r="AG1227" s="98"/>
+      <c r="AH1227" s="98"/>
     </row>
     <row r="1390" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1390" s="103"/>
-      <c r="C1390" s="103"/>
-      <c r="D1390" s="103"/>
-      <c r="E1390" s="103"/>
-      <c r="F1390" s="103"/>
-      <c r="G1390" s="103"/>
-      <c r="H1390" s="103"/>
-      <c r="I1390" s="103"/>
-      <c r="J1390" s="103"/>
-      <c r="K1390" s="103"/>
-      <c r="L1390" s="103"/>
-      <c r="M1390" s="103"/>
-      <c r="N1390" s="103"/>
-      <c r="O1390" s="103"/>
-      <c r="P1390" s="103"/>
-      <c r="Q1390" s="103"/>
-      <c r="R1390" s="103"/>
-      <c r="S1390" s="103"/>
-      <c r="T1390" s="103"/>
-      <c r="U1390" s="103"/>
-      <c r="V1390" s="103"/>
-      <c r="W1390" s="103"/>
-      <c r="X1390" s="103"/>
-      <c r="Y1390" s="103"/>
-      <c r="Z1390" s="103"/>
-      <c r="AA1390" s="103"/>
-      <c r="AB1390" s="103"/>
-      <c r="AC1390" s="103"/>
-      <c r="AD1390" s="103"/>
-      <c r="AE1390" s="103"/>
-      <c r="AF1390" s="103"/>
-      <c r="AG1390" s="103"/>
-      <c r="AH1390" s="103"/>
+      <c r="B1390" s="98"/>
+      <c r="C1390" s="98"/>
+      <c r="D1390" s="98"/>
+      <c r="E1390" s="98"/>
+      <c r="F1390" s="98"/>
+      <c r="G1390" s="98"/>
+      <c r="H1390" s="98"/>
+      <c r="I1390" s="98"/>
+      <c r="J1390" s="98"/>
+      <c r="K1390" s="98"/>
+      <c r="L1390" s="98"/>
+      <c r="M1390" s="98"/>
+      <c r="N1390" s="98"/>
+      <c r="O1390" s="98"/>
+      <c r="P1390" s="98"/>
+      <c r="Q1390" s="98"/>
+      <c r="R1390" s="98"/>
+      <c r="S1390" s="98"/>
+      <c r="T1390" s="98"/>
+      <c r="U1390" s="98"/>
+      <c r="V1390" s="98"/>
+      <c r="W1390" s="98"/>
+      <c r="X1390" s="98"/>
+      <c r="Y1390" s="98"/>
+      <c r="Z1390" s="98"/>
+      <c r="AA1390" s="98"/>
+      <c r="AB1390" s="98"/>
+      <c r="AC1390" s="98"/>
+      <c r="AD1390" s="98"/>
+      <c r="AE1390" s="98"/>
+      <c r="AF1390" s="98"/>
+      <c r="AG1390" s="98"/>
+      <c r="AH1390" s="98"/>
     </row>
     <row r="1502" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1502" s="103"/>
-      <c r="C1502" s="103"/>
-      <c r="D1502" s="103"/>
-      <c r="E1502" s="103"/>
-      <c r="F1502" s="103"/>
-      <c r="G1502" s="103"/>
-      <c r="H1502" s="103"/>
-      <c r="I1502" s="103"/>
-      <c r="J1502" s="103"/>
-      <c r="K1502" s="103"/>
-      <c r="L1502" s="103"/>
-      <c r="M1502" s="103"/>
-      <c r="N1502" s="103"/>
-      <c r="O1502" s="103"/>
-      <c r="P1502" s="103"/>
-      <c r="Q1502" s="103"/>
-      <c r="R1502" s="103"/>
-      <c r="S1502" s="103"/>
-      <c r="T1502" s="103"/>
-      <c r="U1502" s="103"/>
-      <c r="V1502" s="103"/>
-      <c r="W1502" s="103"/>
-      <c r="X1502" s="103"/>
-      <c r="Y1502" s="103"/>
-      <c r="Z1502" s="103"/>
-      <c r="AA1502" s="103"/>
-      <c r="AB1502" s="103"/>
-      <c r="AC1502" s="103"/>
-      <c r="AD1502" s="103"/>
-      <c r="AE1502" s="103"/>
-      <c r="AF1502" s="103"/>
-      <c r="AG1502" s="103"/>
-      <c r="AH1502" s="103"/>
+      <c r="B1502" s="98"/>
+      <c r="C1502" s="98"/>
+      <c r="D1502" s="98"/>
+      <c r="E1502" s="98"/>
+      <c r="F1502" s="98"/>
+      <c r="G1502" s="98"/>
+      <c r="H1502" s="98"/>
+      <c r="I1502" s="98"/>
+      <c r="J1502" s="98"/>
+      <c r="K1502" s="98"/>
+      <c r="L1502" s="98"/>
+      <c r="M1502" s="98"/>
+      <c r="N1502" s="98"/>
+      <c r="O1502" s="98"/>
+      <c r="P1502" s="98"/>
+      <c r="Q1502" s="98"/>
+      <c r="R1502" s="98"/>
+      <c r="S1502" s="98"/>
+      <c r="T1502" s="98"/>
+      <c r="U1502" s="98"/>
+      <c r="V1502" s="98"/>
+      <c r="W1502" s="98"/>
+      <c r="X1502" s="98"/>
+      <c r="Y1502" s="98"/>
+      <c r="Z1502" s="98"/>
+      <c r="AA1502" s="98"/>
+      <c r="AB1502" s="98"/>
+      <c r="AC1502" s="98"/>
+      <c r="AD1502" s="98"/>
+      <c r="AE1502" s="98"/>
+      <c r="AF1502" s="98"/>
+      <c r="AG1502" s="98"/>
+      <c r="AH1502" s="98"/>
     </row>
     <row r="1604" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1604" s="103"/>
-      <c r="C1604" s="103"/>
-      <c r="D1604" s="103"/>
-      <c r="E1604" s="103"/>
-      <c r="F1604" s="103"/>
-      <c r="G1604" s="103"/>
-      <c r="H1604" s="103"/>
-      <c r="I1604" s="103"/>
-      <c r="J1604" s="103"/>
-      <c r="K1604" s="103"/>
-      <c r="L1604" s="103"/>
-      <c r="M1604" s="103"/>
-      <c r="N1604" s="103"/>
-      <c r="O1604" s="103"/>
-      <c r="P1604" s="103"/>
-      <c r="Q1604" s="103"/>
-      <c r="R1604" s="103"/>
-      <c r="S1604" s="103"/>
-      <c r="T1604" s="103"/>
-      <c r="U1604" s="103"/>
-      <c r="V1604" s="103"/>
-      <c r="W1604" s="103"/>
-      <c r="X1604" s="103"/>
-      <c r="Y1604" s="103"/>
-      <c r="Z1604" s="103"/>
-      <c r="AA1604" s="103"/>
-      <c r="AB1604" s="103"/>
-      <c r="AC1604" s="103"/>
-      <c r="AD1604" s="103"/>
-      <c r="AE1604" s="103"/>
-      <c r="AF1604" s="103"/>
-      <c r="AG1604" s="103"/>
-      <c r="AH1604" s="103"/>
+      <c r="B1604" s="98"/>
+      <c r="C1604" s="98"/>
+      <c r="D1604" s="98"/>
+      <c r="E1604" s="98"/>
+      <c r="F1604" s="98"/>
+      <c r="G1604" s="98"/>
+      <c r="H1604" s="98"/>
+      <c r="I1604" s="98"/>
+      <c r="J1604" s="98"/>
+      <c r="K1604" s="98"/>
+      <c r="L1604" s="98"/>
+      <c r="M1604" s="98"/>
+      <c r="N1604" s="98"/>
+      <c r="O1604" s="98"/>
+      <c r="P1604" s="98"/>
+      <c r="Q1604" s="98"/>
+      <c r="R1604" s="98"/>
+      <c r="S1604" s="98"/>
+      <c r="T1604" s="98"/>
+      <c r="U1604" s="98"/>
+      <c r="V1604" s="98"/>
+      <c r="W1604" s="98"/>
+      <c r="X1604" s="98"/>
+      <c r="Y1604" s="98"/>
+      <c r="Z1604" s="98"/>
+      <c r="AA1604" s="98"/>
+      <c r="AB1604" s="98"/>
+      <c r="AC1604" s="98"/>
+      <c r="AD1604" s="98"/>
+      <c r="AE1604" s="98"/>
+      <c r="AF1604" s="98"/>
+      <c r="AG1604" s="98"/>
+      <c r="AH1604" s="98"/>
     </row>
     <row r="1698" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1698" s="103"/>
-      <c r="C1698" s="103"/>
-      <c r="D1698" s="103"/>
-      <c r="E1698" s="103"/>
-      <c r="F1698" s="103"/>
-      <c r="G1698" s="103"/>
-      <c r="H1698" s="103"/>
-      <c r="I1698" s="103"/>
-      <c r="J1698" s="103"/>
-      <c r="K1698" s="103"/>
-      <c r="L1698" s="103"/>
-      <c r="M1698" s="103"/>
-      <c r="N1698" s="103"/>
-      <c r="O1698" s="103"/>
-      <c r="P1698" s="103"/>
-      <c r="Q1698" s="103"/>
-      <c r="R1698" s="103"/>
-      <c r="S1698" s="103"/>
-      <c r="T1698" s="103"/>
-      <c r="U1698" s="103"/>
-      <c r="V1698" s="103"/>
-      <c r="W1698" s="103"/>
-      <c r="X1698" s="103"/>
-      <c r="Y1698" s="103"/>
-      <c r="Z1698" s="103"/>
-      <c r="AA1698" s="103"/>
-      <c r="AB1698" s="103"/>
-      <c r="AC1698" s="103"/>
-      <c r="AD1698" s="103"/>
-      <c r="AE1698" s="103"/>
-      <c r="AF1698" s="103"/>
-      <c r="AG1698" s="103"/>
-      <c r="AH1698" s="103"/>
+      <c r="B1698" s="98"/>
+      <c r="C1698" s="98"/>
+      <c r="D1698" s="98"/>
+      <c r="E1698" s="98"/>
+      <c r="F1698" s="98"/>
+      <c r="G1698" s="98"/>
+      <c r="H1698" s="98"/>
+      <c r="I1698" s="98"/>
+      <c r="J1698" s="98"/>
+      <c r="K1698" s="98"/>
+      <c r="L1698" s="98"/>
+      <c r="M1698" s="98"/>
+      <c r="N1698" s="98"/>
+      <c r="O1698" s="98"/>
+      <c r="P1698" s="98"/>
+      <c r="Q1698" s="98"/>
+      <c r="R1698" s="98"/>
+      <c r="S1698" s="98"/>
+      <c r="T1698" s="98"/>
+      <c r="U1698" s="98"/>
+      <c r="V1698" s="98"/>
+      <c r="W1698" s="98"/>
+      <c r="X1698" s="98"/>
+      <c r="Y1698" s="98"/>
+      <c r="Z1698" s="98"/>
+      <c r="AA1698" s="98"/>
+      <c r="AB1698" s="98"/>
+      <c r="AC1698" s="98"/>
+      <c r="AD1698" s="98"/>
+      <c r="AE1698" s="98"/>
+      <c r="AF1698" s="98"/>
+      <c r="AG1698" s="98"/>
+      <c r="AH1698" s="98"/>
     </row>
     <row r="1945" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1945" s="103"/>
-      <c r="C1945" s="103"/>
-      <c r="D1945" s="103"/>
-      <c r="E1945" s="103"/>
-      <c r="F1945" s="103"/>
-      <c r="G1945" s="103"/>
-      <c r="H1945" s="103"/>
-      <c r="I1945" s="103"/>
-      <c r="J1945" s="103"/>
-      <c r="K1945" s="103"/>
-      <c r="L1945" s="103"/>
-      <c r="M1945" s="103"/>
-      <c r="N1945" s="103"/>
-      <c r="O1945" s="103"/>
-      <c r="P1945" s="103"/>
-      <c r="Q1945" s="103"/>
-      <c r="R1945" s="103"/>
-      <c r="S1945" s="103"/>
-      <c r="T1945" s="103"/>
-      <c r="U1945" s="103"/>
-      <c r="V1945" s="103"/>
-      <c r="W1945" s="103"/>
-      <c r="X1945" s="103"/>
-      <c r="Y1945" s="103"/>
-      <c r="Z1945" s="103"/>
-      <c r="AA1945" s="103"/>
-      <c r="AB1945" s="103"/>
-      <c r="AC1945" s="103"/>
-      <c r="AD1945" s="103"/>
-      <c r="AE1945" s="103"/>
-      <c r="AF1945" s="103"/>
-      <c r="AG1945" s="103"/>
-      <c r="AH1945" s="103"/>
+      <c r="B1945" s="98"/>
+      <c r="C1945" s="98"/>
+      <c r="D1945" s="98"/>
+      <c r="E1945" s="98"/>
+      <c r="F1945" s="98"/>
+      <c r="G1945" s="98"/>
+      <c r="H1945" s="98"/>
+      <c r="I1945" s="98"/>
+      <c r="J1945" s="98"/>
+      <c r="K1945" s="98"/>
+      <c r="L1945" s="98"/>
+      <c r="M1945" s="98"/>
+      <c r="N1945" s="98"/>
+      <c r="O1945" s="98"/>
+      <c r="P1945" s="98"/>
+      <c r="Q1945" s="98"/>
+      <c r="R1945" s="98"/>
+      <c r="S1945" s="98"/>
+      <c r="T1945" s="98"/>
+      <c r="U1945" s="98"/>
+      <c r="V1945" s="98"/>
+      <c r="W1945" s="98"/>
+      <c r="X1945" s="98"/>
+      <c r="Y1945" s="98"/>
+      <c r="Z1945" s="98"/>
+      <c r="AA1945" s="98"/>
+      <c r="AB1945" s="98"/>
+      <c r="AC1945" s="98"/>
+      <c r="AD1945" s="98"/>
+      <c r="AE1945" s="98"/>
+      <c r="AF1945" s="98"/>
+      <c r="AG1945" s="98"/>
+      <c r="AH1945" s="98"/>
     </row>
     <row r="2031" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2031" s="103"/>
-      <c r="C2031" s="103"/>
-      <c r="D2031" s="103"/>
-      <c r="E2031" s="103"/>
-      <c r="F2031" s="103"/>
-      <c r="G2031" s="103"/>
-      <c r="H2031" s="103"/>
-      <c r="I2031" s="103"/>
-      <c r="J2031" s="103"/>
-      <c r="K2031" s="103"/>
-      <c r="L2031" s="103"/>
-      <c r="M2031" s="103"/>
-      <c r="N2031" s="103"/>
-      <c r="O2031" s="103"/>
-      <c r="P2031" s="103"/>
-      <c r="Q2031" s="103"/>
-      <c r="R2031" s="103"/>
-      <c r="S2031" s="103"/>
-      <c r="T2031" s="103"/>
-      <c r="U2031" s="103"/>
-      <c r="V2031" s="103"/>
-      <c r="W2031" s="103"/>
-      <c r="X2031" s="103"/>
-      <c r="Y2031" s="103"/>
-      <c r="Z2031" s="103"/>
-      <c r="AA2031" s="103"/>
-      <c r="AB2031" s="103"/>
-      <c r="AC2031" s="103"/>
-      <c r="AD2031" s="103"/>
-      <c r="AE2031" s="103"/>
-      <c r="AF2031" s="103"/>
-      <c r="AG2031" s="103"/>
-      <c r="AH2031" s="103"/>
+      <c r="B2031" s="98"/>
+      <c r="C2031" s="98"/>
+      <c r="D2031" s="98"/>
+      <c r="E2031" s="98"/>
+      <c r="F2031" s="98"/>
+      <c r="G2031" s="98"/>
+      <c r="H2031" s="98"/>
+      <c r="I2031" s="98"/>
+      <c r="J2031" s="98"/>
+      <c r="K2031" s="98"/>
+      <c r="L2031" s="98"/>
+      <c r="M2031" s="98"/>
+      <c r="N2031" s="98"/>
+      <c r="O2031" s="98"/>
+      <c r="P2031" s="98"/>
+      <c r="Q2031" s="98"/>
+      <c r="R2031" s="98"/>
+      <c r="S2031" s="98"/>
+      <c r="T2031" s="98"/>
+      <c r="U2031" s="98"/>
+      <c r="V2031" s="98"/>
+      <c r="W2031" s="98"/>
+      <c r="X2031" s="98"/>
+      <c r="Y2031" s="98"/>
+      <c r="Z2031" s="98"/>
+      <c r="AA2031" s="98"/>
+      <c r="AB2031" s="98"/>
+      <c r="AC2031" s="98"/>
+      <c r="AD2031" s="98"/>
+      <c r="AE2031" s="98"/>
+      <c r="AF2031" s="98"/>
+      <c r="AG2031" s="98"/>
+      <c r="AH2031" s="98"/>
     </row>
     <row r="2153" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2153" s="103"/>
-      <c r="C2153" s="103"/>
-      <c r="D2153" s="103"/>
-      <c r="E2153" s="103"/>
-      <c r="F2153" s="103"/>
-      <c r="G2153" s="103"/>
-      <c r="H2153" s="103"/>
-      <c r="I2153" s="103"/>
-      <c r="J2153" s="103"/>
-      <c r="K2153" s="103"/>
-      <c r="L2153" s="103"/>
-      <c r="M2153" s="103"/>
-      <c r="N2153" s="103"/>
-      <c r="O2153" s="103"/>
-      <c r="P2153" s="103"/>
-      <c r="Q2153" s="103"/>
-      <c r="R2153" s="103"/>
-      <c r="S2153" s="103"/>
-      <c r="T2153" s="103"/>
-      <c r="U2153" s="103"/>
-      <c r="V2153" s="103"/>
-      <c r="W2153" s="103"/>
-      <c r="X2153" s="103"/>
-      <c r="Y2153" s="103"/>
-      <c r="Z2153" s="103"/>
-      <c r="AA2153" s="103"/>
-      <c r="AB2153" s="103"/>
-      <c r="AC2153" s="103"/>
-      <c r="AD2153" s="103"/>
-      <c r="AE2153" s="103"/>
-      <c r="AF2153" s="103"/>
-      <c r="AG2153" s="103"/>
-      <c r="AH2153" s="103"/>
+      <c r="B2153" s="98"/>
+      <c r="C2153" s="98"/>
+      <c r="D2153" s="98"/>
+      <c r="E2153" s="98"/>
+      <c r="F2153" s="98"/>
+      <c r="G2153" s="98"/>
+      <c r="H2153" s="98"/>
+      <c r="I2153" s="98"/>
+      <c r="J2153" s="98"/>
+      <c r="K2153" s="98"/>
+      <c r="L2153" s="98"/>
+      <c r="M2153" s="98"/>
+      <c r="N2153" s="98"/>
+      <c r="O2153" s="98"/>
+      <c r="P2153" s="98"/>
+      <c r="Q2153" s="98"/>
+      <c r="R2153" s="98"/>
+      <c r="S2153" s="98"/>
+      <c r="T2153" s="98"/>
+      <c r="U2153" s="98"/>
+      <c r="V2153" s="98"/>
+      <c r="W2153" s="98"/>
+      <c r="X2153" s="98"/>
+      <c r="Y2153" s="98"/>
+      <c r="Z2153" s="98"/>
+      <c r="AA2153" s="98"/>
+      <c r="AB2153" s="98"/>
+      <c r="AC2153" s="98"/>
+      <c r="AD2153" s="98"/>
+      <c r="AE2153" s="98"/>
+      <c r="AF2153" s="98"/>
+      <c r="AG2153" s="98"/>
+      <c r="AH2153" s="98"/>
     </row>
     <row r="2317" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2317" s="103"/>
-      <c r="C2317" s="103"/>
-      <c r="D2317" s="103"/>
-      <c r="E2317" s="103"/>
-      <c r="F2317" s="103"/>
-      <c r="G2317" s="103"/>
-      <c r="H2317" s="103"/>
-      <c r="I2317" s="103"/>
-      <c r="J2317" s="103"/>
-      <c r="K2317" s="103"/>
-      <c r="L2317" s="103"/>
-      <c r="M2317" s="103"/>
-      <c r="N2317" s="103"/>
-      <c r="O2317" s="103"/>
-      <c r="P2317" s="103"/>
-      <c r="Q2317" s="103"/>
-      <c r="R2317" s="103"/>
-      <c r="S2317" s="103"/>
-      <c r="T2317" s="103"/>
-      <c r="U2317" s="103"/>
-      <c r="V2317" s="103"/>
-      <c r="W2317" s="103"/>
-      <c r="X2317" s="103"/>
-      <c r="Y2317" s="103"/>
-      <c r="Z2317" s="103"/>
-      <c r="AA2317" s="103"/>
-      <c r="AB2317" s="103"/>
-      <c r="AC2317" s="103"/>
-      <c r="AD2317" s="103"/>
-      <c r="AE2317" s="103"/>
-      <c r="AF2317" s="103"/>
-      <c r="AG2317" s="103"/>
-      <c r="AH2317" s="103"/>
+      <c r="B2317" s="98"/>
+      <c r="C2317" s="98"/>
+      <c r="D2317" s="98"/>
+      <c r="E2317" s="98"/>
+      <c r="F2317" s="98"/>
+      <c r="G2317" s="98"/>
+      <c r="H2317" s="98"/>
+      <c r="I2317" s="98"/>
+      <c r="J2317" s="98"/>
+      <c r="K2317" s="98"/>
+      <c r="L2317" s="98"/>
+      <c r="M2317" s="98"/>
+      <c r="N2317" s="98"/>
+      <c r="O2317" s="98"/>
+      <c r="P2317" s="98"/>
+      <c r="Q2317" s="98"/>
+      <c r="R2317" s="98"/>
+      <c r="S2317" s="98"/>
+      <c r="T2317" s="98"/>
+      <c r="U2317" s="98"/>
+      <c r="V2317" s="98"/>
+      <c r="W2317" s="98"/>
+      <c r="X2317" s="98"/>
+      <c r="Y2317" s="98"/>
+      <c r="Z2317" s="98"/>
+      <c r="AA2317" s="98"/>
+      <c r="AB2317" s="98"/>
+      <c r="AC2317" s="98"/>
+      <c r="AD2317" s="98"/>
+      <c r="AE2317" s="98"/>
+      <c r="AF2317" s="98"/>
+      <c r="AG2317" s="98"/>
+      <c r="AH2317" s="98"/>
     </row>
     <row r="2419" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2419" s="103"/>
-      <c r="C2419" s="103"/>
-      <c r="D2419" s="103"/>
-      <c r="E2419" s="103"/>
-      <c r="F2419" s="103"/>
-      <c r="G2419" s="103"/>
-      <c r="H2419" s="103"/>
-      <c r="I2419" s="103"/>
-      <c r="J2419" s="103"/>
-      <c r="K2419" s="103"/>
-      <c r="L2419" s="103"/>
-      <c r="M2419" s="103"/>
-      <c r="N2419" s="103"/>
-      <c r="O2419" s="103"/>
-      <c r="P2419" s="103"/>
-      <c r="Q2419" s="103"/>
-      <c r="R2419" s="103"/>
-      <c r="S2419" s="103"/>
-      <c r="T2419" s="103"/>
-      <c r="U2419" s="103"/>
-      <c r="V2419" s="103"/>
-      <c r="W2419" s="103"/>
-      <c r="X2419" s="103"/>
-      <c r="Y2419" s="103"/>
-      <c r="Z2419" s="103"/>
-      <c r="AA2419" s="103"/>
-      <c r="AB2419" s="103"/>
-      <c r="AC2419" s="103"/>
-      <c r="AD2419" s="103"/>
-      <c r="AE2419" s="103"/>
-      <c r="AF2419" s="103"/>
-      <c r="AG2419" s="103"/>
-      <c r="AH2419" s="103"/>
+      <c r="B2419" s="98"/>
+      <c r="C2419" s="98"/>
+      <c r="D2419" s="98"/>
+      <c r="E2419" s="98"/>
+      <c r="F2419" s="98"/>
+      <c r="G2419" s="98"/>
+      <c r="H2419" s="98"/>
+      <c r="I2419" s="98"/>
+      <c r="J2419" s="98"/>
+      <c r="K2419" s="98"/>
+      <c r="L2419" s="98"/>
+      <c r="M2419" s="98"/>
+      <c r="N2419" s="98"/>
+      <c r="O2419" s="98"/>
+      <c r="P2419" s="98"/>
+      <c r="Q2419" s="98"/>
+      <c r="R2419" s="98"/>
+      <c r="S2419" s="98"/>
+      <c r="T2419" s="98"/>
+      <c r="U2419" s="98"/>
+      <c r="V2419" s="98"/>
+      <c r="W2419" s="98"/>
+      <c r="X2419" s="98"/>
+      <c r="Y2419" s="98"/>
+      <c r="Z2419" s="98"/>
+      <c r="AA2419" s="98"/>
+      <c r="AB2419" s="98"/>
+      <c r="AC2419" s="98"/>
+      <c r="AD2419" s="98"/>
+      <c r="AE2419" s="98"/>
+      <c r="AF2419" s="98"/>
+      <c r="AG2419" s="98"/>
+      <c r="AH2419" s="98"/>
     </row>
     <row r="2509" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2509" s="103"/>
-      <c r="C2509" s="103"/>
-      <c r="D2509" s="103"/>
-      <c r="E2509" s="103"/>
-      <c r="F2509" s="103"/>
-      <c r="G2509" s="103"/>
-      <c r="H2509" s="103"/>
-      <c r="I2509" s="103"/>
-      <c r="J2509" s="103"/>
-      <c r="K2509" s="103"/>
-      <c r="L2509" s="103"/>
-      <c r="M2509" s="103"/>
-      <c r="N2509" s="103"/>
-      <c r="O2509" s="103"/>
-      <c r="P2509" s="103"/>
-      <c r="Q2509" s="103"/>
-      <c r="R2509" s="103"/>
-      <c r="S2509" s="103"/>
-      <c r="T2509" s="103"/>
-      <c r="U2509" s="103"/>
-      <c r="V2509" s="103"/>
-      <c r="W2509" s="103"/>
-      <c r="X2509" s="103"/>
-      <c r="Y2509" s="103"/>
-      <c r="Z2509" s="103"/>
-      <c r="AA2509" s="103"/>
-      <c r="AB2509" s="103"/>
-      <c r="AC2509" s="103"/>
-      <c r="AD2509" s="103"/>
-      <c r="AE2509" s="103"/>
-      <c r="AF2509" s="103"/>
-      <c r="AG2509" s="103"/>
-      <c r="AH2509" s="103"/>
+      <c r="B2509" s="98"/>
+      <c r="C2509" s="98"/>
+      <c r="D2509" s="98"/>
+      <c r="E2509" s="98"/>
+      <c r="F2509" s="98"/>
+      <c r="G2509" s="98"/>
+      <c r="H2509" s="98"/>
+      <c r="I2509" s="98"/>
+      <c r="J2509" s="98"/>
+      <c r="K2509" s="98"/>
+      <c r="L2509" s="98"/>
+      <c r="M2509" s="98"/>
+      <c r="N2509" s="98"/>
+      <c r="O2509" s="98"/>
+      <c r="P2509" s="98"/>
+      <c r="Q2509" s="98"/>
+      <c r="R2509" s="98"/>
+      <c r="S2509" s="98"/>
+      <c r="T2509" s="98"/>
+      <c r="U2509" s="98"/>
+      <c r="V2509" s="98"/>
+      <c r="W2509" s="98"/>
+      <c r="X2509" s="98"/>
+      <c r="Y2509" s="98"/>
+      <c r="Z2509" s="98"/>
+      <c r="AA2509" s="98"/>
+      <c r="AB2509" s="98"/>
+      <c r="AC2509" s="98"/>
+      <c r="AD2509" s="98"/>
+      <c r="AE2509" s="98"/>
+      <c r="AF2509" s="98"/>
+      <c r="AG2509" s="98"/>
+      <c r="AH2509" s="98"/>
     </row>
     <row r="2598" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2598" s="103"/>
-      <c r="C2598" s="103"/>
-      <c r="D2598" s="103"/>
-      <c r="E2598" s="103"/>
-      <c r="F2598" s="103"/>
-      <c r="G2598" s="103"/>
-      <c r="H2598" s="103"/>
-      <c r="I2598" s="103"/>
-      <c r="J2598" s="103"/>
-      <c r="K2598" s="103"/>
-      <c r="L2598" s="103"/>
-      <c r="M2598" s="103"/>
-      <c r="N2598" s="103"/>
-      <c r="O2598" s="103"/>
-      <c r="P2598" s="103"/>
-      <c r="Q2598" s="103"/>
-      <c r="R2598" s="103"/>
-      <c r="S2598" s="103"/>
-      <c r="T2598" s="103"/>
-      <c r="U2598" s="103"/>
-      <c r="V2598" s="103"/>
-      <c r="W2598" s="103"/>
-      <c r="X2598" s="103"/>
-      <c r="Y2598" s="103"/>
-      <c r="Z2598" s="103"/>
-      <c r="AA2598" s="103"/>
-      <c r="AB2598" s="103"/>
-      <c r="AC2598" s="103"/>
-      <c r="AD2598" s="103"/>
-      <c r="AE2598" s="103"/>
-      <c r="AF2598" s="103"/>
-      <c r="AG2598" s="103"/>
-      <c r="AH2598" s="103"/>
+      <c r="B2598" s="98"/>
+      <c r="C2598" s="98"/>
+      <c r="D2598" s="98"/>
+      <c r="E2598" s="98"/>
+      <c r="F2598" s="98"/>
+      <c r="G2598" s="98"/>
+      <c r="H2598" s="98"/>
+      <c r="I2598" s="98"/>
+      <c r="J2598" s="98"/>
+      <c r="K2598" s="98"/>
+      <c r="L2598" s="98"/>
+      <c r="M2598" s="98"/>
+      <c r="N2598" s="98"/>
+      <c r="O2598" s="98"/>
+      <c r="P2598" s="98"/>
+      <c r="Q2598" s="98"/>
+      <c r="R2598" s="98"/>
+      <c r="S2598" s="98"/>
+      <c r="T2598" s="98"/>
+      <c r="U2598" s="98"/>
+      <c r="V2598" s="98"/>
+      <c r="W2598" s="98"/>
+      <c r="X2598" s="98"/>
+      <c r="Y2598" s="98"/>
+      <c r="Z2598" s="98"/>
+      <c r="AA2598" s="98"/>
+      <c r="AB2598" s="98"/>
+      <c r="AC2598" s="98"/>
+      <c r="AD2598" s="98"/>
+      <c r="AE2598" s="98"/>
+      <c r="AF2598" s="98"/>
+      <c r="AG2598" s="98"/>
+      <c r="AH2598" s="98"/>
     </row>
     <row r="2719" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2719" s="103"/>
-      <c r="C2719" s="103"/>
-      <c r="D2719" s="103"/>
-      <c r="E2719" s="103"/>
-      <c r="F2719" s="103"/>
-      <c r="G2719" s="103"/>
-      <c r="H2719" s="103"/>
-      <c r="I2719" s="103"/>
-      <c r="J2719" s="103"/>
-      <c r="K2719" s="103"/>
-      <c r="L2719" s="103"/>
-      <c r="M2719" s="103"/>
-      <c r="N2719" s="103"/>
-      <c r="O2719" s="103"/>
-      <c r="P2719" s="103"/>
-      <c r="Q2719" s="103"/>
-      <c r="R2719" s="103"/>
-      <c r="S2719" s="103"/>
-      <c r="T2719" s="103"/>
-      <c r="U2719" s="103"/>
-      <c r="V2719" s="103"/>
-      <c r="W2719" s="103"/>
-      <c r="X2719" s="103"/>
-      <c r="Y2719" s="103"/>
-      <c r="Z2719" s="103"/>
-      <c r="AA2719" s="103"/>
-      <c r="AB2719" s="103"/>
-      <c r="AC2719" s="103"/>
-      <c r="AD2719" s="103"/>
-      <c r="AE2719" s="103"/>
-      <c r="AF2719" s="103"/>
-      <c r="AG2719" s="103"/>
-      <c r="AH2719" s="103"/>
+      <c r="B2719" s="98"/>
+      <c r="C2719" s="98"/>
+      <c r="D2719" s="98"/>
+      <c r="E2719" s="98"/>
+      <c r="F2719" s="98"/>
+      <c r="G2719" s="98"/>
+      <c r="H2719" s="98"/>
+      <c r="I2719" s="98"/>
+      <c r="J2719" s="98"/>
+      <c r="K2719" s="98"/>
+      <c r="L2719" s="98"/>
+      <c r="M2719" s="98"/>
+      <c r="N2719" s="98"/>
+      <c r="O2719" s="98"/>
+      <c r="P2719" s="98"/>
+      <c r="Q2719" s="98"/>
+      <c r="R2719" s="98"/>
+      <c r="S2719" s="98"/>
+      <c r="T2719" s="98"/>
+      <c r="U2719" s="98"/>
+      <c r="V2719" s="98"/>
+      <c r="W2719" s="98"/>
+      <c r="X2719" s="98"/>
+      <c r="Y2719" s="98"/>
+      <c r="Z2719" s="98"/>
+      <c r="AA2719" s="98"/>
+      <c r="AB2719" s="98"/>
+      <c r="AC2719" s="98"/>
+      <c r="AD2719" s="98"/>
+      <c r="AE2719" s="98"/>
+      <c r="AF2719" s="98"/>
+      <c r="AG2719" s="98"/>
+      <c r="AH2719" s="98"/>
     </row>
     <row r="2837" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2837" s="103"/>
-      <c r="C2837" s="103"/>
-      <c r="D2837" s="103"/>
-      <c r="E2837" s="103"/>
-      <c r="F2837" s="103"/>
-      <c r="G2837" s="103"/>
-      <c r="H2837" s="103"/>
-      <c r="I2837" s="103"/>
-      <c r="J2837" s="103"/>
-      <c r="K2837" s="103"/>
-      <c r="L2837" s="103"/>
-      <c r="M2837" s="103"/>
-      <c r="N2837" s="103"/>
-      <c r="O2837" s="103"/>
-      <c r="P2837" s="103"/>
-      <c r="Q2837" s="103"/>
-      <c r="R2837" s="103"/>
-      <c r="S2837" s="103"/>
-      <c r="T2837" s="103"/>
-      <c r="U2837" s="103"/>
-      <c r="V2837" s="103"/>
-      <c r="W2837" s="103"/>
-      <c r="X2837" s="103"/>
-      <c r="Y2837" s="103"/>
-      <c r="Z2837" s="103"/>
-      <c r="AA2837" s="103"/>
-      <c r="AB2837" s="103"/>
-      <c r="AC2837" s="103"/>
-      <c r="AD2837" s="103"/>
-      <c r="AE2837" s="103"/>
-      <c r="AF2837" s="103"/>
-      <c r="AG2837" s="103"/>
-      <c r="AH2837" s="103"/>
+      <c r="B2837" s="98"/>
+      <c r="C2837" s="98"/>
+      <c r="D2837" s="98"/>
+      <c r="E2837" s="98"/>
+      <c r="F2837" s="98"/>
+      <c r="G2837" s="98"/>
+      <c r="H2837" s="98"/>
+      <c r="I2837" s="98"/>
+      <c r="J2837" s="98"/>
+      <c r="K2837" s="98"/>
+      <c r="L2837" s="98"/>
+      <c r="M2837" s="98"/>
+      <c r="N2837" s="98"/>
+      <c r="O2837" s="98"/>
+      <c r="P2837" s="98"/>
+      <c r="Q2837" s="98"/>
+      <c r="R2837" s="98"/>
+      <c r="S2837" s="98"/>
+      <c r="T2837" s="98"/>
+      <c r="U2837" s="98"/>
+      <c r="V2837" s="98"/>
+      <c r="W2837" s="98"/>
+      <c r="X2837" s="98"/>
+      <c r="Y2837" s="98"/>
+      <c r="Z2837" s="98"/>
+      <c r="AA2837" s="98"/>
+      <c r="AB2837" s="98"/>
+      <c r="AC2837" s="98"/>
+      <c r="AD2837" s="98"/>
+      <c r="AE2837" s="98"/>
+      <c r="AF2837" s="98"/>
+      <c r="AG2837" s="98"/>
+      <c r="AH2837" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B112:AH112"/>
+    <mergeCell ref="B147:AG147"/>
+    <mergeCell ref="B308:AH308"/>
+    <mergeCell ref="B511:AH511"/>
+    <mergeCell ref="B712:AH712"/>
+    <mergeCell ref="B887:AH887"/>
+    <mergeCell ref="B1100:AH1100"/>
+    <mergeCell ref="B1227:AH1227"/>
+    <mergeCell ref="B1390:AH1390"/>
+    <mergeCell ref="B1502:AH1502"/>
+    <mergeCell ref="B1604:AH1604"/>
+    <mergeCell ref="B1698:AH1698"/>
+    <mergeCell ref="B1945:AH1945"/>
+    <mergeCell ref="B2031:AH2031"/>
+    <mergeCell ref="B2719:AH2719"/>
     <mergeCell ref="B2837:AH2837"/>
     <mergeCell ref="B2153:AH2153"/>
     <mergeCell ref="B2317:AH2317"/>
     <mergeCell ref="B2419:AH2419"/>
     <mergeCell ref="B2509:AH2509"/>
     <mergeCell ref="B2598:AH2598"/>
-    <mergeCell ref="B1604:AH1604"/>
-    <mergeCell ref="B1698:AH1698"/>
-    <mergeCell ref="B1945:AH1945"/>
-    <mergeCell ref="B2031:AH2031"/>
-    <mergeCell ref="B2719:AH2719"/>
-    <mergeCell ref="B887:AH887"/>
-    <mergeCell ref="B1100:AH1100"/>
-    <mergeCell ref="B1227:AH1227"/>
-    <mergeCell ref="B1390:AH1390"/>
-    <mergeCell ref="B1502:AH1502"/>
-    <mergeCell ref="B112:AH112"/>
-    <mergeCell ref="B147:AG147"/>
-    <mergeCell ref="B308:AH308"/>
-    <mergeCell ref="B511:AH511"/>
-    <mergeCell ref="B712:AH712"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="28" priority="1"/>
@@ -36386,7 +36455,7 @@
   <dimension ref="A1:AI11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36506,129 +36575,129 @@
         <f>Calculations!J186</f>
         <v>0</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="113">
         <f>Calculations!K186-'Water and Waste'!C14</f>
-        <v>1753075107369824.5</v>
-      </c>
-      <c r="D2" s="9">
+        <v>1484313638179564</v>
+      </c>
+      <c r="D2" s="113">
         <f>Calculations!L186-'Water and Waste'!D14</f>
-        <v>1878070126794797.8</v>
-      </c>
-      <c r="E2" s="9">
+        <v>1607380033719217</v>
+      </c>
+      <c r="E2" s="113">
         <f>Calculations!M186-'Water and Waste'!E14</f>
-        <v>1963288614062102.5</v>
-      </c>
-      <c r="F2" s="9">
+        <v>1690678848520078.3</v>
+      </c>
+      <c r="F2" s="113">
         <f>Calculations!N186-'Water and Waste'!F14</f>
-        <v>2048660284750767.8</v>
-      </c>
-      <c r="G2" s="9">
+        <v>1774143053222586.8</v>
+      </c>
+      <c r="G2" s="113">
         <f>Calculations!O186-'Water and Waste'!G14</f>
-        <v>2136586212229338.5</v>
-      </c>
-      <c r="H2" s="9">
+        <v>1860178603787402.5</v>
+      </c>
+      <c r="H2" s="113">
         <f>Calculations!P186-'Water and Waste'!H14</f>
-        <v>2224578112076844.3</v>
-      </c>
-      <c r="I2" s="9">
+        <v>1946300470854964.5</v>
+      </c>
+      <c r="I2" s="113">
         <f>Calculations!Q186-'Water and Waste'!I14</f>
-        <v>2255714342082799.5</v>
-      </c>
-      <c r="J2" s="9">
+        <v>1975588639745492.5</v>
+      </c>
+      <c r="J2" s="113">
         <f>Calculations!R186-'Water and Waste'!J14</f>
-        <v>2287728865562932.5</v>
-      </c>
-      <c r="K2" s="9">
+        <v>2005774632478657</v>
+      </c>
+      <c r="K2" s="113">
         <f>Calculations!S186-'Water and Waste'!K14</f>
-        <v>2319840792570059.5</v>
-      </c>
-      <c r="L2" s="9">
+        <v>2036084882995446.5</v>
+      </c>
+      <c r="L2" s="113">
         <f>Calculations!T186-'Water and Waste'!L14</f>
-        <v>2351849838683210</v>
-      </c>
-      <c r="M2" s="9">
+        <v>2066322361936300.5</v>
+      </c>
+      <c r="M2" s="113">
         <f>Calculations!U186-'Water and Waste'!M14</f>
-        <v>2383531719481413.5</v>
-      </c>
-      <c r="N2" s="9">
+        <v>2096266039941658.5</v>
+      </c>
+      <c r="N2" s="113">
         <f>Calculations!V186-'Water and Waste'!N14</f>
-        <v>2416076792754185.5</v>
-      </c>
-      <c r="O2" s="9">
+        <v>2127107902331740</v>
+      </c>
+      <c r="O2" s="113">
         <f>Calculations!W186-'Water and Waste'!O14</f>
-        <v>2450652774080554.5</v>
-      </c>
-      <c r="P2" s="9">
+        <v>2160018919746984.5</v>
+      </c>
+      <c r="P2" s="113">
         <f>Calculations!X186-'Water and Waste'!P14</f>
-        <v>2485559984565764.5</v>
-      </c>
-      <c r="Q2" s="9">
+        <v>2193298599527282.5</v>
+      </c>
+      <c r="Q2" s="113">
         <f>Calculations!Y186-'Water and Waste'!Q14</f>
-        <v>2521566781999328.5</v>
-      </c>
-      <c r="R2" s="9">
+        <v>2227716926992852.5</v>
+      </c>
+      <c r="R2" s="113">
         <f>Calculations!Z186-'Water and Waste'!R14</f>
-        <v>2558977166381248</v>
-      </c>
-      <c r="S2" s="9">
+        <v>2263577902143696</v>
+      </c>
+      <c r="S2" s="113">
         <f>Calculations!AA186-'Water and Waste'!S14</f>
-        <v>2597311101027250</v>
-      </c>
-      <c r="T2" s="9">
+        <v>2300399046999482.5</v>
+      </c>
+      <c r="T2" s="113">
         <f>Calculations!AB186-'Water and Waste'!T14</f>
-        <v>2636267585937335</v>
-      </c>
-      <c r="U2" s="9">
+        <v>2337879361560212.5</v>
+      </c>
+      <c r="U2" s="113">
         <f>Calculations!AC186-'Water and Waste'!U14</f>
-        <v>2676315584427231.5</v>
-      </c>
-      <c r="V2" s="9">
+        <v>2376485367845557</v>
+      </c>
+      <c r="V2" s="113">
         <f>Calculations!AD186-'Water and Waste'!V14</f>
-        <v>2717339417602179</v>
-      </c>
-      <c r="W2" s="9">
+        <v>2416100573195403.5</v>
+      </c>
+      <c r="W2" s="113">
         <f>Calculations!AE186-'Water and Waste'!W14</f>
-        <v>2760842727672667</v>
-      </c>
-      <c r="X2" s="9">
+        <v>2458226992289536</v>
+      </c>
+      <c r="X2" s="113">
         <f>Calculations!AF186-'Water and Waste'!X14</f>
-        <v>2806574799059663</v>
-      </c>
-      <c r="Y2" s="9">
+        <v>2502610654487512.5</v>
+      </c>
+      <c r="Y2" s="113">
         <f>Calculations!AG186-'Water and Waste'!Y14</f>
-        <v>2853534273973652.5</v>
-      </c>
-      <c r="Z2" s="9">
+        <v>2548248574469113.5</v>
+      </c>
+      <c r="Z2" s="113">
         <f>Calculations!AH186-'Water and Waste'!Z14</f>
-        <v>2903522115730365</v>
-      </c>
-      <c r="AA2" s="9">
+        <v>2596939274254011.5</v>
+      </c>
+      <c r="AA2" s="113">
         <f>Calculations!AI186-'Water and Waste'!AA14</f>
-        <v>2954814608750768.5</v>
-      </c>
-      <c r="AB2" s="9">
+        <v>2646955783201764</v>
+      </c>
+      <c r="AB2" s="113">
         <f>Calculations!AJ186-'Water and Waste'!AB14</f>
-        <v>3008777358561079</v>
-      </c>
-      <c r="AC2" s="9">
+        <v>2699659638011825.5</v>
+      </c>
+      <c r="AC2" s="113">
         <f>Calculations!AK186-'Water and Waste'!AC14</f>
-        <v>3065299328477021.5</v>
-      </c>
-      <c r="AD2" s="9">
+        <v>2754937360703862.5</v>
+      </c>
+      <c r="AD2" s="113">
         <f>Calculations!AL186-'Water and Waste'!AD14</f>
-        <v>3124923445130053</v>
-      </c>
-      <c r="AE2" s="9">
+        <v>2813326995317219</v>
+      </c>
+      <c r="AE2" s="113">
         <f>Calculations!AM186-'Water and Waste'!AE14</f>
-        <v>3186796671835901</v>
-      </c>
-      <c r="AF2" s="9">
+        <v>2873973063871563</v>
+      </c>
+      <c r="AF2" s="113">
         <f>Calculations!AN186-'Water and Waste'!AF14</f>
-        <v>3252025293015535.5</v>
-      </c>
-      <c r="AG2" s="9">
+        <v>2937978595726456.5</v>
+      </c>
+      <c r="AG2" s="113">
         <f>Calculations!AO186-'Water and Waste'!AG14</f>
-        <v>3320115271984685.5</v>
+        <v>3004847112901570</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
@@ -36639,7 +36708,7 @@
         <f>Calculations!J187</f>
         <v>0</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="116">
         <f>Calculations!K187</f>
         <v>20544799999999.996</v>
       </c>
@@ -36772,7 +36841,7 @@
         <f>Calculations!J188</f>
         <v>0</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="116">
         <f>Calculations!K188</f>
         <v>555670000000000</v>
       </c>
@@ -36905,7 +36974,7 @@
         <f>Calculations!J189</f>
         <v>0</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="116">
         <f>Calculations!K189</f>
         <v>86303000000000</v>
       </c>
@@ -37038,7 +37107,7 @@
         <f>Calculations!J190</f>
         <v>0</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="116">
         <f>Calculations!K190</f>
         <v>0</v>
       </c>
@@ -37171,7 +37240,7 @@
         <f>Calculations!J191</f>
         <v>0</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="116">
         <f>Calculations!K191</f>
         <v>0</v>
       </c>
@@ -37304,7 +37373,7 @@
         <f>Calculations!J192</f>
         <v>0</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="116">
         <f>Calculations!K192</f>
         <v>0</v>
       </c>
@@ -37437,7 +37506,7 @@
         <f>Calculations!J193</f>
         <v>0</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="116">
         <f>Calculations!K193</f>
         <v>0</v>
       </c>
@@ -37570,7 +37639,7 @@
         <f>Calculations!J194</f>
         <v>0</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="116">
         <f>Calculations!K194</f>
         <v>137550082379028.25</v>
       </c>
@@ -37703,7 +37772,7 @@
         <f>Calculations!J195</f>
         <v>0</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="116">
         <f>Calculations!K195</f>
         <v>0</v>
       </c>
@@ -47960,40 +48029,40 @@
     </row>
     <row r="121" spans="1:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="122" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="101" t="s">
+      <c r="B122" s="102" t="s">
         <v>597</v>
       </c>
-      <c r="C122" s="102"/>
-      <c r="D122" s="102"/>
-      <c r="E122" s="102"/>
-      <c r="F122" s="102"/>
-      <c r="G122" s="102"/>
-      <c r="H122" s="102"/>
-      <c r="I122" s="102"/>
-      <c r="J122" s="102"/>
-      <c r="K122" s="102"/>
-      <c r="L122" s="102"/>
-      <c r="M122" s="102"/>
-      <c r="N122" s="102"/>
-      <c r="O122" s="102"/>
-      <c r="P122" s="102"/>
-      <c r="Q122" s="102"/>
-      <c r="R122" s="102"/>
-      <c r="S122" s="102"/>
-      <c r="T122" s="102"/>
-      <c r="U122" s="102"/>
-      <c r="V122" s="102"/>
-      <c r="W122" s="102"/>
-      <c r="X122" s="102"/>
-      <c r="Y122" s="102"/>
-      <c r="Z122" s="102"/>
-      <c r="AA122" s="102"/>
-      <c r="AB122" s="102"/>
-      <c r="AC122" s="102"/>
-      <c r="AD122" s="102"/>
-      <c r="AE122" s="102"/>
-      <c r="AF122" s="102"/>
-      <c r="AG122" s="102"/>
+      <c r="C122" s="103"/>
+      <c r="D122" s="103"/>
+      <c r="E122" s="103"/>
+      <c r="F122" s="103"/>
+      <c r="G122" s="103"/>
+      <c r="H122" s="103"/>
+      <c r="I122" s="103"/>
+      <c r="J122" s="103"/>
+      <c r="K122" s="103"/>
+      <c r="L122" s="103"/>
+      <c r="M122" s="103"/>
+      <c r="N122" s="103"/>
+      <c r="O122" s="103"/>
+      <c r="P122" s="103"/>
+      <c r="Q122" s="103"/>
+      <c r="R122" s="103"/>
+      <c r="S122" s="103"/>
+      <c r="T122" s="103"/>
+      <c r="U122" s="103"/>
+      <c r="V122" s="103"/>
+      <c r="W122" s="103"/>
+      <c r="X122" s="103"/>
+      <c r="Y122" s="103"/>
+      <c r="Z122" s="103"/>
+      <c r="AA122" s="103"/>
+      <c r="AB122" s="103"/>
+      <c r="AC122" s="103"/>
+      <c r="AD122" s="103"/>
+      <c r="AE122" s="103"/>
+      <c r="AF122" s="103"/>
+      <c r="AG122" s="103"/>
       <c r="AH122" s="77"/>
     </row>
     <row r="123" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -48087,693 +48156,693 @@
       </c>
     </row>
     <row r="308" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B308" s="103"/>
-      <c r="C308" s="103"/>
-      <c r="D308" s="103"/>
-      <c r="E308" s="103"/>
-      <c r="F308" s="103"/>
-      <c r="G308" s="103"/>
-      <c r="H308" s="103"/>
-      <c r="I308" s="103"/>
-      <c r="J308" s="103"/>
-      <c r="K308" s="103"/>
-      <c r="L308" s="103"/>
-      <c r="M308" s="103"/>
-      <c r="N308" s="103"/>
-      <c r="O308" s="103"/>
-      <c r="P308" s="103"/>
-      <c r="Q308" s="103"/>
-      <c r="R308" s="103"/>
-      <c r="S308" s="103"/>
-      <c r="T308" s="103"/>
-      <c r="U308" s="103"/>
-      <c r="V308" s="103"/>
-      <c r="W308" s="103"/>
-      <c r="X308" s="103"/>
-      <c r="Y308" s="103"/>
-      <c r="Z308" s="103"/>
-      <c r="AA308" s="103"/>
-      <c r="AB308" s="103"/>
-      <c r="AC308" s="103"/>
-      <c r="AD308" s="103"/>
-      <c r="AE308" s="103"/>
-      <c r="AF308" s="103"/>
-      <c r="AG308" s="103"/>
-      <c r="AH308" s="103"/>
+      <c r="B308" s="98"/>
+      <c r="C308" s="98"/>
+      <c r="D308" s="98"/>
+      <c r="E308" s="98"/>
+      <c r="F308" s="98"/>
+      <c r="G308" s="98"/>
+      <c r="H308" s="98"/>
+      <c r="I308" s="98"/>
+      <c r="J308" s="98"/>
+      <c r="K308" s="98"/>
+      <c r="L308" s="98"/>
+      <c r="M308" s="98"/>
+      <c r="N308" s="98"/>
+      <c r="O308" s="98"/>
+      <c r="P308" s="98"/>
+      <c r="Q308" s="98"/>
+      <c r="R308" s="98"/>
+      <c r="S308" s="98"/>
+      <c r="T308" s="98"/>
+      <c r="U308" s="98"/>
+      <c r="V308" s="98"/>
+      <c r="W308" s="98"/>
+      <c r="X308" s="98"/>
+      <c r="Y308" s="98"/>
+      <c r="Z308" s="98"/>
+      <c r="AA308" s="98"/>
+      <c r="AB308" s="98"/>
+      <c r="AC308" s="98"/>
+      <c r="AD308" s="98"/>
+      <c r="AE308" s="98"/>
+      <c r="AF308" s="98"/>
+      <c r="AG308" s="98"/>
+      <c r="AH308" s="98"/>
     </row>
     <row r="511" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B511" s="103"/>
-      <c r="C511" s="103"/>
-      <c r="D511" s="103"/>
-      <c r="E511" s="103"/>
-      <c r="F511" s="103"/>
-      <c r="G511" s="103"/>
-      <c r="H511" s="103"/>
-      <c r="I511" s="103"/>
-      <c r="J511" s="103"/>
-      <c r="K511" s="103"/>
-      <c r="L511" s="103"/>
-      <c r="M511" s="103"/>
-      <c r="N511" s="103"/>
-      <c r="O511" s="103"/>
-      <c r="P511" s="103"/>
-      <c r="Q511" s="103"/>
-      <c r="R511" s="103"/>
-      <c r="S511" s="103"/>
-      <c r="T511" s="103"/>
-      <c r="U511" s="103"/>
-      <c r="V511" s="103"/>
-      <c r="W511" s="103"/>
-      <c r="X511" s="103"/>
-      <c r="Y511" s="103"/>
-      <c r="Z511" s="103"/>
-      <c r="AA511" s="103"/>
-      <c r="AB511" s="103"/>
-      <c r="AC511" s="103"/>
-      <c r="AD511" s="103"/>
-      <c r="AE511" s="103"/>
-      <c r="AF511" s="103"/>
-      <c r="AG511" s="103"/>
-      <c r="AH511" s="103"/>
+      <c r="B511" s="98"/>
+      <c r="C511" s="98"/>
+      <c r="D511" s="98"/>
+      <c r="E511" s="98"/>
+      <c r="F511" s="98"/>
+      <c r="G511" s="98"/>
+      <c r="H511" s="98"/>
+      <c r="I511" s="98"/>
+      <c r="J511" s="98"/>
+      <c r="K511" s="98"/>
+      <c r="L511" s="98"/>
+      <c r="M511" s="98"/>
+      <c r="N511" s="98"/>
+      <c r="O511" s="98"/>
+      <c r="P511" s="98"/>
+      <c r="Q511" s="98"/>
+      <c r="R511" s="98"/>
+      <c r="S511" s="98"/>
+      <c r="T511" s="98"/>
+      <c r="U511" s="98"/>
+      <c r="V511" s="98"/>
+      <c r="W511" s="98"/>
+      <c r="X511" s="98"/>
+      <c r="Y511" s="98"/>
+      <c r="Z511" s="98"/>
+      <c r="AA511" s="98"/>
+      <c r="AB511" s="98"/>
+      <c r="AC511" s="98"/>
+      <c r="AD511" s="98"/>
+      <c r="AE511" s="98"/>
+      <c r="AF511" s="98"/>
+      <c r="AG511" s="98"/>
+      <c r="AH511" s="98"/>
     </row>
     <row r="712" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B712" s="103"/>
-      <c r="C712" s="103"/>
-      <c r="D712" s="103"/>
-      <c r="E712" s="103"/>
-      <c r="F712" s="103"/>
-      <c r="G712" s="103"/>
-      <c r="H712" s="103"/>
-      <c r="I712" s="103"/>
-      <c r="J712" s="103"/>
-      <c r="K712" s="103"/>
-      <c r="L712" s="103"/>
-      <c r="M712" s="103"/>
-      <c r="N712" s="103"/>
-      <c r="O712" s="103"/>
-      <c r="P712" s="103"/>
-      <c r="Q712" s="103"/>
-      <c r="R712" s="103"/>
-      <c r="S712" s="103"/>
-      <c r="T712" s="103"/>
-      <c r="U712" s="103"/>
-      <c r="V712" s="103"/>
-      <c r="W712" s="103"/>
-      <c r="X712" s="103"/>
-      <c r="Y712" s="103"/>
-      <c r="Z712" s="103"/>
-      <c r="AA712" s="103"/>
-      <c r="AB712" s="103"/>
-      <c r="AC712" s="103"/>
-      <c r="AD712" s="103"/>
-      <c r="AE712" s="103"/>
-      <c r="AF712" s="103"/>
-      <c r="AG712" s="103"/>
-      <c r="AH712" s="103"/>
+      <c r="B712" s="98"/>
+      <c r="C712" s="98"/>
+      <c r="D712" s="98"/>
+      <c r="E712" s="98"/>
+      <c r="F712" s="98"/>
+      <c r="G712" s="98"/>
+      <c r="H712" s="98"/>
+      <c r="I712" s="98"/>
+      <c r="J712" s="98"/>
+      <c r="K712" s="98"/>
+      <c r="L712" s="98"/>
+      <c r="M712" s="98"/>
+      <c r="N712" s="98"/>
+      <c r="O712" s="98"/>
+      <c r="P712" s="98"/>
+      <c r="Q712" s="98"/>
+      <c r="R712" s="98"/>
+      <c r="S712" s="98"/>
+      <c r="T712" s="98"/>
+      <c r="U712" s="98"/>
+      <c r="V712" s="98"/>
+      <c r="W712" s="98"/>
+      <c r="X712" s="98"/>
+      <c r="Y712" s="98"/>
+      <c r="Z712" s="98"/>
+      <c r="AA712" s="98"/>
+      <c r="AB712" s="98"/>
+      <c r="AC712" s="98"/>
+      <c r="AD712" s="98"/>
+      <c r="AE712" s="98"/>
+      <c r="AF712" s="98"/>
+      <c r="AG712" s="98"/>
+      <c r="AH712" s="98"/>
     </row>
     <row r="887" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B887" s="103"/>
-      <c r="C887" s="103"/>
-      <c r="D887" s="103"/>
-      <c r="E887" s="103"/>
-      <c r="F887" s="103"/>
-      <c r="G887" s="103"/>
-      <c r="H887" s="103"/>
-      <c r="I887" s="103"/>
-      <c r="J887" s="103"/>
-      <c r="K887" s="103"/>
-      <c r="L887" s="103"/>
-      <c r="M887" s="103"/>
-      <c r="N887" s="103"/>
-      <c r="O887" s="103"/>
-      <c r="P887" s="103"/>
-      <c r="Q887" s="103"/>
-      <c r="R887" s="103"/>
-      <c r="S887" s="103"/>
-      <c r="T887" s="103"/>
-      <c r="U887" s="103"/>
-      <c r="V887" s="103"/>
-      <c r="W887" s="103"/>
-      <c r="X887" s="103"/>
-      <c r="Y887" s="103"/>
-      <c r="Z887" s="103"/>
-      <c r="AA887" s="103"/>
-      <c r="AB887" s="103"/>
-      <c r="AC887" s="103"/>
-      <c r="AD887" s="103"/>
-      <c r="AE887" s="103"/>
-      <c r="AF887" s="103"/>
-      <c r="AG887" s="103"/>
-      <c r="AH887" s="103"/>
+      <c r="B887" s="98"/>
+      <c r="C887" s="98"/>
+      <c r="D887" s="98"/>
+      <c r="E887" s="98"/>
+      <c r="F887" s="98"/>
+      <c r="G887" s="98"/>
+      <c r="H887" s="98"/>
+      <c r="I887" s="98"/>
+      <c r="J887" s="98"/>
+      <c r="K887" s="98"/>
+      <c r="L887" s="98"/>
+      <c r="M887" s="98"/>
+      <c r="N887" s="98"/>
+      <c r="O887" s="98"/>
+      <c r="P887" s="98"/>
+      <c r="Q887" s="98"/>
+      <c r="R887" s="98"/>
+      <c r="S887" s="98"/>
+      <c r="T887" s="98"/>
+      <c r="U887" s="98"/>
+      <c r="V887" s="98"/>
+      <c r="W887" s="98"/>
+      <c r="X887" s="98"/>
+      <c r="Y887" s="98"/>
+      <c r="Z887" s="98"/>
+      <c r="AA887" s="98"/>
+      <c r="AB887" s="98"/>
+      <c r="AC887" s="98"/>
+      <c r="AD887" s="98"/>
+      <c r="AE887" s="98"/>
+      <c r="AF887" s="98"/>
+      <c r="AG887" s="98"/>
+      <c r="AH887" s="98"/>
     </row>
     <row r="1100" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1100" s="103"/>
-      <c r="C1100" s="103"/>
-      <c r="D1100" s="103"/>
-      <c r="E1100" s="103"/>
-      <c r="F1100" s="103"/>
-      <c r="G1100" s="103"/>
-      <c r="H1100" s="103"/>
-      <c r="I1100" s="103"/>
-      <c r="J1100" s="103"/>
-      <c r="K1100" s="103"/>
-      <c r="L1100" s="103"/>
-      <c r="M1100" s="103"/>
-      <c r="N1100" s="103"/>
-      <c r="O1100" s="103"/>
-      <c r="P1100" s="103"/>
-      <c r="Q1100" s="103"/>
-      <c r="R1100" s="103"/>
-      <c r="S1100" s="103"/>
-      <c r="T1100" s="103"/>
-      <c r="U1100" s="103"/>
-      <c r="V1100" s="103"/>
-      <c r="W1100" s="103"/>
-      <c r="X1100" s="103"/>
-      <c r="Y1100" s="103"/>
-      <c r="Z1100" s="103"/>
-      <c r="AA1100" s="103"/>
-      <c r="AB1100" s="103"/>
-      <c r="AC1100" s="103"/>
-      <c r="AD1100" s="103"/>
-      <c r="AE1100" s="103"/>
-      <c r="AF1100" s="103"/>
-      <c r="AG1100" s="103"/>
-      <c r="AH1100" s="103"/>
+      <c r="B1100" s="98"/>
+      <c r="C1100" s="98"/>
+      <c r="D1100" s="98"/>
+      <c r="E1100" s="98"/>
+      <c r="F1100" s="98"/>
+      <c r="G1100" s="98"/>
+      <c r="H1100" s="98"/>
+      <c r="I1100" s="98"/>
+      <c r="J1100" s="98"/>
+      <c r="K1100" s="98"/>
+      <c r="L1100" s="98"/>
+      <c r="M1100" s="98"/>
+      <c r="N1100" s="98"/>
+      <c r="O1100" s="98"/>
+      <c r="P1100" s="98"/>
+      <c r="Q1100" s="98"/>
+      <c r="R1100" s="98"/>
+      <c r="S1100" s="98"/>
+      <c r="T1100" s="98"/>
+      <c r="U1100" s="98"/>
+      <c r="V1100" s="98"/>
+      <c r="W1100" s="98"/>
+      <c r="X1100" s="98"/>
+      <c r="Y1100" s="98"/>
+      <c r="Z1100" s="98"/>
+      <c r="AA1100" s="98"/>
+      <c r="AB1100" s="98"/>
+      <c r="AC1100" s="98"/>
+      <c r="AD1100" s="98"/>
+      <c r="AE1100" s="98"/>
+      <c r="AF1100" s="98"/>
+      <c r="AG1100" s="98"/>
+      <c r="AH1100" s="98"/>
     </row>
     <row r="1227" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1227" s="103"/>
-      <c r="C1227" s="103"/>
-      <c r="D1227" s="103"/>
-      <c r="E1227" s="103"/>
-      <c r="F1227" s="103"/>
-      <c r="G1227" s="103"/>
-      <c r="H1227" s="103"/>
-      <c r="I1227" s="103"/>
-      <c r="J1227" s="103"/>
-      <c r="K1227" s="103"/>
-      <c r="L1227" s="103"/>
-      <c r="M1227" s="103"/>
-      <c r="N1227" s="103"/>
-      <c r="O1227" s="103"/>
-      <c r="P1227" s="103"/>
-      <c r="Q1227" s="103"/>
-      <c r="R1227" s="103"/>
-      <c r="S1227" s="103"/>
-      <c r="T1227" s="103"/>
-      <c r="U1227" s="103"/>
-      <c r="V1227" s="103"/>
-      <c r="W1227" s="103"/>
-      <c r="X1227" s="103"/>
-      <c r="Y1227" s="103"/>
-      <c r="Z1227" s="103"/>
-      <c r="AA1227" s="103"/>
-      <c r="AB1227" s="103"/>
-      <c r="AC1227" s="103"/>
-      <c r="AD1227" s="103"/>
-      <c r="AE1227" s="103"/>
-      <c r="AF1227" s="103"/>
-      <c r="AG1227" s="103"/>
-      <c r="AH1227" s="103"/>
+      <c r="B1227" s="98"/>
+      <c r="C1227" s="98"/>
+      <c r="D1227" s="98"/>
+      <c r="E1227" s="98"/>
+      <c r="F1227" s="98"/>
+      <c r="G1227" s="98"/>
+      <c r="H1227" s="98"/>
+      <c r="I1227" s="98"/>
+      <c r="J1227" s="98"/>
+      <c r="K1227" s="98"/>
+      <c r="L1227" s="98"/>
+      <c r="M1227" s="98"/>
+      <c r="N1227" s="98"/>
+      <c r="O1227" s="98"/>
+      <c r="P1227" s="98"/>
+      <c r="Q1227" s="98"/>
+      <c r="R1227" s="98"/>
+      <c r="S1227" s="98"/>
+      <c r="T1227" s="98"/>
+      <c r="U1227" s="98"/>
+      <c r="V1227" s="98"/>
+      <c r="W1227" s="98"/>
+      <c r="X1227" s="98"/>
+      <c r="Y1227" s="98"/>
+      <c r="Z1227" s="98"/>
+      <c r="AA1227" s="98"/>
+      <c r="AB1227" s="98"/>
+      <c r="AC1227" s="98"/>
+      <c r="AD1227" s="98"/>
+      <c r="AE1227" s="98"/>
+      <c r="AF1227" s="98"/>
+      <c r="AG1227" s="98"/>
+      <c r="AH1227" s="98"/>
     </row>
     <row r="1390" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1390" s="103"/>
-      <c r="C1390" s="103"/>
-      <c r="D1390" s="103"/>
-      <c r="E1390" s="103"/>
-      <c r="F1390" s="103"/>
-      <c r="G1390" s="103"/>
-      <c r="H1390" s="103"/>
-      <c r="I1390" s="103"/>
-      <c r="J1390" s="103"/>
-      <c r="K1390" s="103"/>
-      <c r="L1390" s="103"/>
-      <c r="M1390" s="103"/>
-      <c r="N1390" s="103"/>
-      <c r="O1390" s="103"/>
-      <c r="P1390" s="103"/>
-      <c r="Q1390" s="103"/>
-      <c r="R1390" s="103"/>
-      <c r="S1390" s="103"/>
-      <c r="T1390" s="103"/>
-      <c r="U1390" s="103"/>
-      <c r="V1390" s="103"/>
-      <c r="W1390" s="103"/>
-      <c r="X1390" s="103"/>
-      <c r="Y1390" s="103"/>
-      <c r="Z1390" s="103"/>
-      <c r="AA1390" s="103"/>
-      <c r="AB1390" s="103"/>
-      <c r="AC1390" s="103"/>
-      <c r="AD1390" s="103"/>
-      <c r="AE1390" s="103"/>
-      <c r="AF1390" s="103"/>
-      <c r="AG1390" s="103"/>
-      <c r="AH1390" s="103"/>
+      <c r="B1390" s="98"/>
+      <c r="C1390" s="98"/>
+      <c r="D1390" s="98"/>
+      <c r="E1390" s="98"/>
+      <c r="F1390" s="98"/>
+      <c r="G1390" s="98"/>
+      <c r="H1390" s="98"/>
+      <c r="I1390" s="98"/>
+      <c r="J1390" s="98"/>
+      <c r="K1390" s="98"/>
+      <c r="L1390" s="98"/>
+      <c r="M1390" s="98"/>
+      <c r="N1390" s="98"/>
+      <c r="O1390" s="98"/>
+      <c r="P1390" s="98"/>
+      <c r="Q1390" s="98"/>
+      <c r="R1390" s="98"/>
+      <c r="S1390" s="98"/>
+      <c r="T1390" s="98"/>
+      <c r="U1390" s="98"/>
+      <c r="V1390" s="98"/>
+      <c r="W1390" s="98"/>
+      <c r="X1390" s="98"/>
+      <c r="Y1390" s="98"/>
+      <c r="Z1390" s="98"/>
+      <c r="AA1390" s="98"/>
+      <c r="AB1390" s="98"/>
+      <c r="AC1390" s="98"/>
+      <c r="AD1390" s="98"/>
+      <c r="AE1390" s="98"/>
+      <c r="AF1390" s="98"/>
+      <c r="AG1390" s="98"/>
+      <c r="AH1390" s="98"/>
     </row>
     <row r="1502" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1502" s="103"/>
-      <c r="C1502" s="103"/>
-      <c r="D1502" s="103"/>
-      <c r="E1502" s="103"/>
-      <c r="F1502" s="103"/>
-      <c r="G1502" s="103"/>
-      <c r="H1502" s="103"/>
-      <c r="I1502" s="103"/>
-      <c r="J1502" s="103"/>
-      <c r="K1502" s="103"/>
-      <c r="L1502" s="103"/>
-      <c r="M1502" s="103"/>
-      <c r="N1502" s="103"/>
-      <c r="O1502" s="103"/>
-      <c r="P1502" s="103"/>
-      <c r="Q1502" s="103"/>
-      <c r="R1502" s="103"/>
-      <c r="S1502" s="103"/>
-      <c r="T1502" s="103"/>
-      <c r="U1502" s="103"/>
-      <c r="V1502" s="103"/>
-      <c r="W1502" s="103"/>
-      <c r="X1502" s="103"/>
-      <c r="Y1502" s="103"/>
-      <c r="Z1502" s="103"/>
-      <c r="AA1502" s="103"/>
-      <c r="AB1502" s="103"/>
-      <c r="AC1502" s="103"/>
-      <c r="AD1502" s="103"/>
-      <c r="AE1502" s="103"/>
-      <c r="AF1502" s="103"/>
-      <c r="AG1502" s="103"/>
-      <c r="AH1502" s="103"/>
+      <c r="B1502" s="98"/>
+      <c r="C1502" s="98"/>
+      <c r="D1502" s="98"/>
+      <c r="E1502" s="98"/>
+      <c r="F1502" s="98"/>
+      <c r="G1502" s="98"/>
+      <c r="H1502" s="98"/>
+      <c r="I1502" s="98"/>
+      <c r="J1502" s="98"/>
+      <c r="K1502" s="98"/>
+      <c r="L1502" s="98"/>
+      <c r="M1502" s="98"/>
+      <c r="N1502" s="98"/>
+      <c r="O1502" s="98"/>
+      <c r="P1502" s="98"/>
+      <c r="Q1502" s="98"/>
+      <c r="R1502" s="98"/>
+      <c r="S1502" s="98"/>
+      <c r="T1502" s="98"/>
+      <c r="U1502" s="98"/>
+      <c r="V1502" s="98"/>
+      <c r="W1502" s="98"/>
+      <c r="X1502" s="98"/>
+      <c r="Y1502" s="98"/>
+      <c r="Z1502" s="98"/>
+      <c r="AA1502" s="98"/>
+      <c r="AB1502" s="98"/>
+      <c r="AC1502" s="98"/>
+      <c r="AD1502" s="98"/>
+      <c r="AE1502" s="98"/>
+      <c r="AF1502" s="98"/>
+      <c r="AG1502" s="98"/>
+      <c r="AH1502" s="98"/>
     </row>
     <row r="1604" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1604" s="103"/>
-      <c r="C1604" s="103"/>
-      <c r="D1604" s="103"/>
-      <c r="E1604" s="103"/>
-      <c r="F1604" s="103"/>
-      <c r="G1604" s="103"/>
-      <c r="H1604" s="103"/>
-      <c r="I1604" s="103"/>
-      <c r="J1604" s="103"/>
-      <c r="K1604" s="103"/>
-      <c r="L1604" s="103"/>
-      <c r="M1604" s="103"/>
-      <c r="N1604" s="103"/>
-      <c r="O1604" s="103"/>
-      <c r="P1604" s="103"/>
-      <c r="Q1604" s="103"/>
-      <c r="R1604" s="103"/>
-      <c r="S1604" s="103"/>
-      <c r="T1604" s="103"/>
-      <c r="U1604" s="103"/>
-      <c r="V1604" s="103"/>
-      <c r="W1604" s="103"/>
-      <c r="X1604" s="103"/>
-      <c r="Y1604" s="103"/>
-      <c r="Z1604" s="103"/>
-      <c r="AA1604" s="103"/>
-      <c r="AB1604" s="103"/>
-      <c r="AC1604" s="103"/>
-      <c r="AD1604" s="103"/>
-      <c r="AE1604" s="103"/>
-      <c r="AF1604" s="103"/>
-      <c r="AG1604" s="103"/>
-      <c r="AH1604" s="103"/>
+      <c r="B1604" s="98"/>
+      <c r="C1604" s="98"/>
+      <c r="D1604" s="98"/>
+      <c r="E1604" s="98"/>
+      <c r="F1604" s="98"/>
+      <c r="G1604" s="98"/>
+      <c r="H1604" s="98"/>
+      <c r="I1604" s="98"/>
+      <c r="J1604" s="98"/>
+      <c r="K1604" s="98"/>
+      <c r="L1604" s="98"/>
+      <c r="M1604" s="98"/>
+      <c r="N1604" s="98"/>
+      <c r="O1604" s="98"/>
+      <c r="P1604" s="98"/>
+      <c r="Q1604" s="98"/>
+      <c r="R1604" s="98"/>
+      <c r="S1604" s="98"/>
+      <c r="T1604" s="98"/>
+      <c r="U1604" s="98"/>
+      <c r="V1604" s="98"/>
+      <c r="W1604" s="98"/>
+      <c r="X1604" s="98"/>
+      <c r="Y1604" s="98"/>
+      <c r="Z1604" s="98"/>
+      <c r="AA1604" s="98"/>
+      <c r="AB1604" s="98"/>
+      <c r="AC1604" s="98"/>
+      <c r="AD1604" s="98"/>
+      <c r="AE1604" s="98"/>
+      <c r="AF1604" s="98"/>
+      <c r="AG1604" s="98"/>
+      <c r="AH1604" s="98"/>
     </row>
     <row r="1698" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1698" s="103"/>
-      <c r="C1698" s="103"/>
-      <c r="D1698" s="103"/>
-      <c r="E1698" s="103"/>
-      <c r="F1698" s="103"/>
-      <c r="G1698" s="103"/>
-      <c r="H1698" s="103"/>
-      <c r="I1698" s="103"/>
-      <c r="J1698" s="103"/>
-      <c r="K1698" s="103"/>
-      <c r="L1698" s="103"/>
-      <c r="M1698" s="103"/>
-      <c r="N1698" s="103"/>
-      <c r="O1698" s="103"/>
-      <c r="P1698" s="103"/>
-      <c r="Q1698" s="103"/>
-      <c r="R1698" s="103"/>
-      <c r="S1698" s="103"/>
-      <c r="T1698" s="103"/>
-      <c r="U1698" s="103"/>
-      <c r="V1698" s="103"/>
-      <c r="W1698" s="103"/>
-      <c r="X1698" s="103"/>
-      <c r="Y1698" s="103"/>
-      <c r="Z1698" s="103"/>
-      <c r="AA1698" s="103"/>
-      <c r="AB1698" s="103"/>
-      <c r="AC1698" s="103"/>
-      <c r="AD1698" s="103"/>
-      <c r="AE1698" s="103"/>
-      <c r="AF1698" s="103"/>
-      <c r="AG1698" s="103"/>
-      <c r="AH1698" s="103"/>
+      <c r="B1698" s="98"/>
+      <c r="C1698" s="98"/>
+      <c r="D1698" s="98"/>
+      <c r="E1698" s="98"/>
+      <c r="F1698" s="98"/>
+      <c r="G1698" s="98"/>
+      <c r="H1698" s="98"/>
+      <c r="I1698" s="98"/>
+      <c r="J1698" s="98"/>
+      <c r="K1698" s="98"/>
+      <c r="L1698" s="98"/>
+      <c r="M1698" s="98"/>
+      <c r="N1698" s="98"/>
+      <c r="O1698" s="98"/>
+      <c r="P1698" s="98"/>
+      <c r="Q1698" s="98"/>
+      <c r="R1698" s="98"/>
+      <c r="S1698" s="98"/>
+      <c r="T1698" s="98"/>
+      <c r="U1698" s="98"/>
+      <c r="V1698" s="98"/>
+      <c r="W1698" s="98"/>
+      <c r="X1698" s="98"/>
+      <c r="Y1698" s="98"/>
+      <c r="Z1698" s="98"/>
+      <c r="AA1698" s="98"/>
+      <c r="AB1698" s="98"/>
+      <c r="AC1698" s="98"/>
+      <c r="AD1698" s="98"/>
+      <c r="AE1698" s="98"/>
+      <c r="AF1698" s="98"/>
+      <c r="AG1698" s="98"/>
+      <c r="AH1698" s="98"/>
     </row>
     <row r="1945" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1945" s="103"/>
-      <c r="C1945" s="103"/>
-      <c r="D1945" s="103"/>
-      <c r="E1945" s="103"/>
-      <c r="F1945" s="103"/>
-      <c r="G1945" s="103"/>
-      <c r="H1945" s="103"/>
-      <c r="I1945" s="103"/>
-      <c r="J1945" s="103"/>
-      <c r="K1945" s="103"/>
-      <c r="L1945" s="103"/>
-      <c r="M1945" s="103"/>
-      <c r="N1945" s="103"/>
-      <c r="O1945" s="103"/>
-      <c r="P1945" s="103"/>
-      <c r="Q1945" s="103"/>
-      <c r="R1945" s="103"/>
-      <c r="S1945" s="103"/>
-      <c r="T1945" s="103"/>
-      <c r="U1945" s="103"/>
-      <c r="V1945" s="103"/>
-      <c r="W1945" s="103"/>
-      <c r="X1945" s="103"/>
-      <c r="Y1945" s="103"/>
-      <c r="Z1945" s="103"/>
-      <c r="AA1945" s="103"/>
-      <c r="AB1945" s="103"/>
-      <c r="AC1945" s="103"/>
-      <c r="AD1945" s="103"/>
-      <c r="AE1945" s="103"/>
-      <c r="AF1945" s="103"/>
-      <c r="AG1945" s="103"/>
-      <c r="AH1945" s="103"/>
+      <c r="B1945" s="98"/>
+      <c r="C1945" s="98"/>
+      <c r="D1945" s="98"/>
+      <c r="E1945" s="98"/>
+      <c r="F1945" s="98"/>
+      <c r="G1945" s="98"/>
+      <c r="H1945" s="98"/>
+      <c r="I1945" s="98"/>
+      <c r="J1945" s="98"/>
+      <c r="K1945" s="98"/>
+      <c r="L1945" s="98"/>
+      <c r="M1945" s="98"/>
+      <c r="N1945" s="98"/>
+      <c r="O1945" s="98"/>
+      <c r="P1945" s="98"/>
+      <c r="Q1945" s="98"/>
+      <c r="R1945" s="98"/>
+      <c r="S1945" s="98"/>
+      <c r="T1945" s="98"/>
+      <c r="U1945" s="98"/>
+      <c r="V1945" s="98"/>
+      <c r="W1945" s="98"/>
+      <c r="X1945" s="98"/>
+      <c r="Y1945" s="98"/>
+      <c r="Z1945" s="98"/>
+      <c r="AA1945" s="98"/>
+      <c r="AB1945" s="98"/>
+      <c r="AC1945" s="98"/>
+      <c r="AD1945" s="98"/>
+      <c r="AE1945" s="98"/>
+      <c r="AF1945" s="98"/>
+      <c r="AG1945" s="98"/>
+      <c r="AH1945" s="98"/>
     </row>
     <row r="2031" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2031" s="103"/>
-      <c r="C2031" s="103"/>
-      <c r="D2031" s="103"/>
-      <c r="E2031" s="103"/>
-      <c r="F2031" s="103"/>
-      <c r="G2031" s="103"/>
-      <c r="H2031" s="103"/>
-      <c r="I2031" s="103"/>
-      <c r="J2031" s="103"/>
-      <c r="K2031" s="103"/>
-      <c r="L2031" s="103"/>
-      <c r="M2031" s="103"/>
-      <c r="N2031" s="103"/>
-      <c r="O2031" s="103"/>
-      <c r="P2031" s="103"/>
-      <c r="Q2031" s="103"/>
-      <c r="R2031" s="103"/>
-      <c r="S2031" s="103"/>
-      <c r="T2031" s="103"/>
-      <c r="U2031" s="103"/>
-      <c r="V2031" s="103"/>
-      <c r="W2031" s="103"/>
-      <c r="X2031" s="103"/>
-      <c r="Y2031" s="103"/>
-      <c r="Z2031" s="103"/>
-      <c r="AA2031" s="103"/>
-      <c r="AB2031" s="103"/>
-      <c r="AC2031" s="103"/>
-      <c r="AD2031" s="103"/>
-      <c r="AE2031" s="103"/>
-      <c r="AF2031" s="103"/>
-      <c r="AG2031" s="103"/>
-      <c r="AH2031" s="103"/>
+      <c r="B2031" s="98"/>
+      <c r="C2031" s="98"/>
+      <c r="D2031" s="98"/>
+      <c r="E2031" s="98"/>
+      <c r="F2031" s="98"/>
+      <c r="G2031" s="98"/>
+      <c r="H2031" s="98"/>
+      <c r="I2031" s="98"/>
+      <c r="J2031" s="98"/>
+      <c r="K2031" s="98"/>
+      <c r="L2031" s="98"/>
+      <c r="M2031" s="98"/>
+      <c r="N2031" s="98"/>
+      <c r="O2031" s="98"/>
+      <c r="P2031" s="98"/>
+      <c r="Q2031" s="98"/>
+      <c r="R2031" s="98"/>
+      <c r="S2031" s="98"/>
+      <c r="T2031" s="98"/>
+      <c r="U2031" s="98"/>
+      <c r="V2031" s="98"/>
+      <c r="W2031" s="98"/>
+      <c r="X2031" s="98"/>
+      <c r="Y2031" s="98"/>
+      <c r="Z2031" s="98"/>
+      <c r="AA2031" s="98"/>
+      <c r="AB2031" s="98"/>
+      <c r="AC2031" s="98"/>
+      <c r="AD2031" s="98"/>
+      <c r="AE2031" s="98"/>
+      <c r="AF2031" s="98"/>
+      <c r="AG2031" s="98"/>
+      <c r="AH2031" s="98"/>
     </row>
     <row r="2153" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2153" s="103"/>
-      <c r="C2153" s="103"/>
-      <c r="D2153" s="103"/>
-      <c r="E2153" s="103"/>
-      <c r="F2153" s="103"/>
-      <c r="G2153" s="103"/>
-      <c r="H2153" s="103"/>
-      <c r="I2153" s="103"/>
-      <c r="J2153" s="103"/>
-      <c r="K2153" s="103"/>
-      <c r="L2153" s="103"/>
-      <c r="M2153" s="103"/>
-      <c r="N2153" s="103"/>
-      <c r="O2153" s="103"/>
-      <c r="P2153" s="103"/>
-      <c r="Q2153" s="103"/>
-      <c r="R2153" s="103"/>
-      <c r="S2153" s="103"/>
-      <c r="T2153" s="103"/>
-      <c r="U2153" s="103"/>
-      <c r="V2153" s="103"/>
-      <c r="W2153" s="103"/>
-      <c r="X2153" s="103"/>
-      <c r="Y2153" s="103"/>
-      <c r="Z2153" s="103"/>
-      <c r="AA2153" s="103"/>
-      <c r="AB2153" s="103"/>
-      <c r="AC2153" s="103"/>
-      <c r="AD2153" s="103"/>
-      <c r="AE2153" s="103"/>
-      <c r="AF2153" s="103"/>
-      <c r="AG2153" s="103"/>
-      <c r="AH2153" s="103"/>
+      <c r="B2153" s="98"/>
+      <c r="C2153" s="98"/>
+      <c r="D2153" s="98"/>
+      <c r="E2153" s="98"/>
+      <c r="F2153" s="98"/>
+      <c r="G2153" s="98"/>
+      <c r="H2153" s="98"/>
+      <c r="I2153" s="98"/>
+      <c r="J2153" s="98"/>
+      <c r="K2153" s="98"/>
+      <c r="L2153" s="98"/>
+      <c r="M2153" s="98"/>
+      <c r="N2153" s="98"/>
+      <c r="O2153" s="98"/>
+      <c r="P2153" s="98"/>
+      <c r="Q2153" s="98"/>
+      <c r="R2153" s="98"/>
+      <c r="S2153" s="98"/>
+      <c r="T2153" s="98"/>
+      <c r="U2153" s="98"/>
+      <c r="V2153" s="98"/>
+      <c r="W2153" s="98"/>
+      <c r="X2153" s="98"/>
+      <c r="Y2153" s="98"/>
+      <c r="Z2153" s="98"/>
+      <c r="AA2153" s="98"/>
+      <c r="AB2153" s="98"/>
+      <c r="AC2153" s="98"/>
+      <c r="AD2153" s="98"/>
+      <c r="AE2153" s="98"/>
+      <c r="AF2153" s="98"/>
+      <c r="AG2153" s="98"/>
+      <c r="AH2153" s="98"/>
     </row>
     <row r="2317" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2317" s="103"/>
-      <c r="C2317" s="103"/>
-      <c r="D2317" s="103"/>
-      <c r="E2317" s="103"/>
-      <c r="F2317" s="103"/>
-      <c r="G2317" s="103"/>
-      <c r="H2317" s="103"/>
-      <c r="I2317" s="103"/>
-      <c r="J2317" s="103"/>
-      <c r="K2317" s="103"/>
-      <c r="L2317" s="103"/>
-      <c r="M2317" s="103"/>
-      <c r="N2317" s="103"/>
-      <c r="O2317" s="103"/>
-      <c r="P2317" s="103"/>
-      <c r="Q2317" s="103"/>
-      <c r="R2317" s="103"/>
-      <c r="S2317" s="103"/>
-      <c r="T2317" s="103"/>
-      <c r="U2317" s="103"/>
-      <c r="V2317" s="103"/>
-      <c r="W2317" s="103"/>
-      <c r="X2317" s="103"/>
-      <c r="Y2317" s="103"/>
-      <c r="Z2317" s="103"/>
-      <c r="AA2317" s="103"/>
-      <c r="AB2317" s="103"/>
-      <c r="AC2317" s="103"/>
-      <c r="AD2317" s="103"/>
-      <c r="AE2317" s="103"/>
-      <c r="AF2317" s="103"/>
-      <c r="AG2317" s="103"/>
-      <c r="AH2317" s="103"/>
+      <c r="B2317" s="98"/>
+      <c r="C2317" s="98"/>
+      <c r="D2317" s="98"/>
+      <c r="E2317" s="98"/>
+      <c r="F2317" s="98"/>
+      <c r="G2317" s="98"/>
+      <c r="H2317" s="98"/>
+      <c r="I2317" s="98"/>
+      <c r="J2317" s="98"/>
+      <c r="K2317" s="98"/>
+      <c r="L2317" s="98"/>
+      <c r="M2317" s="98"/>
+      <c r="N2317" s="98"/>
+      <c r="O2317" s="98"/>
+      <c r="P2317" s="98"/>
+      <c r="Q2317" s="98"/>
+      <c r="R2317" s="98"/>
+      <c r="S2317" s="98"/>
+      <c r="T2317" s="98"/>
+      <c r="U2317" s="98"/>
+      <c r="V2317" s="98"/>
+      <c r="W2317" s="98"/>
+      <c r="X2317" s="98"/>
+      <c r="Y2317" s="98"/>
+      <c r="Z2317" s="98"/>
+      <c r="AA2317" s="98"/>
+      <c r="AB2317" s="98"/>
+      <c r="AC2317" s="98"/>
+      <c r="AD2317" s="98"/>
+      <c r="AE2317" s="98"/>
+      <c r="AF2317" s="98"/>
+      <c r="AG2317" s="98"/>
+      <c r="AH2317" s="98"/>
     </row>
     <row r="2419" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2419" s="103"/>
-      <c r="C2419" s="103"/>
-      <c r="D2419" s="103"/>
-      <c r="E2419" s="103"/>
-      <c r="F2419" s="103"/>
-      <c r="G2419" s="103"/>
-      <c r="H2419" s="103"/>
-      <c r="I2419" s="103"/>
-      <c r="J2419" s="103"/>
-      <c r="K2419" s="103"/>
-      <c r="L2419" s="103"/>
-      <c r="M2419" s="103"/>
-      <c r="N2419" s="103"/>
-      <c r="O2419" s="103"/>
-      <c r="P2419" s="103"/>
-      <c r="Q2419" s="103"/>
-      <c r="R2419" s="103"/>
-      <c r="S2419" s="103"/>
-      <c r="T2419" s="103"/>
-      <c r="U2419" s="103"/>
-      <c r="V2419" s="103"/>
-      <c r="W2419" s="103"/>
-      <c r="X2419" s="103"/>
-      <c r="Y2419" s="103"/>
-      <c r="Z2419" s="103"/>
-      <c r="AA2419" s="103"/>
-      <c r="AB2419" s="103"/>
-      <c r="AC2419" s="103"/>
-      <c r="AD2419" s="103"/>
-      <c r="AE2419" s="103"/>
-      <c r="AF2419" s="103"/>
-      <c r="AG2419" s="103"/>
-      <c r="AH2419" s="103"/>
+      <c r="B2419" s="98"/>
+      <c r="C2419" s="98"/>
+      <c r="D2419" s="98"/>
+      <c r="E2419" s="98"/>
+      <c r="F2419" s="98"/>
+      <c r="G2419" s="98"/>
+      <c r="H2419" s="98"/>
+      <c r="I2419" s="98"/>
+      <c r="J2419" s="98"/>
+      <c r="K2419" s="98"/>
+      <c r="L2419" s="98"/>
+      <c r="M2419" s="98"/>
+      <c r="N2419" s="98"/>
+      <c r="O2419" s="98"/>
+      <c r="P2419" s="98"/>
+      <c r="Q2419" s="98"/>
+      <c r="R2419" s="98"/>
+      <c r="S2419" s="98"/>
+      <c r="T2419" s="98"/>
+      <c r="U2419" s="98"/>
+      <c r="V2419" s="98"/>
+      <c r="W2419" s="98"/>
+      <c r="X2419" s="98"/>
+      <c r="Y2419" s="98"/>
+      <c r="Z2419" s="98"/>
+      <c r="AA2419" s="98"/>
+      <c r="AB2419" s="98"/>
+      <c r="AC2419" s="98"/>
+      <c r="AD2419" s="98"/>
+      <c r="AE2419" s="98"/>
+      <c r="AF2419" s="98"/>
+      <c r="AG2419" s="98"/>
+      <c r="AH2419" s="98"/>
     </row>
     <row r="2509" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2509" s="103"/>
-      <c r="C2509" s="103"/>
-      <c r="D2509" s="103"/>
-      <c r="E2509" s="103"/>
-      <c r="F2509" s="103"/>
-      <c r="G2509" s="103"/>
-      <c r="H2509" s="103"/>
-      <c r="I2509" s="103"/>
-      <c r="J2509" s="103"/>
-      <c r="K2509" s="103"/>
-      <c r="L2509" s="103"/>
-      <c r="M2509" s="103"/>
-      <c r="N2509" s="103"/>
-      <c r="O2509" s="103"/>
-      <c r="P2509" s="103"/>
-      <c r="Q2509" s="103"/>
-      <c r="R2509" s="103"/>
-      <c r="S2509" s="103"/>
-      <c r="T2509" s="103"/>
-      <c r="U2509" s="103"/>
-      <c r="V2509" s="103"/>
-      <c r="W2509" s="103"/>
-      <c r="X2509" s="103"/>
-      <c r="Y2509" s="103"/>
-      <c r="Z2509" s="103"/>
-      <c r="AA2509" s="103"/>
-      <c r="AB2509" s="103"/>
-      <c r="AC2509" s="103"/>
-      <c r="AD2509" s="103"/>
-      <c r="AE2509" s="103"/>
-      <c r="AF2509" s="103"/>
-      <c r="AG2509" s="103"/>
-      <c r="AH2509" s="103"/>
+      <c r="B2509" s="98"/>
+      <c r="C2509" s="98"/>
+      <c r="D2509" s="98"/>
+      <c r="E2509" s="98"/>
+      <c r="F2509" s="98"/>
+      <c r="G2509" s="98"/>
+      <c r="H2509" s="98"/>
+      <c r="I2509" s="98"/>
+      <c r="J2509" s="98"/>
+      <c r="K2509" s="98"/>
+      <c r="L2509" s="98"/>
+      <c r="M2509" s="98"/>
+      <c r="N2509" s="98"/>
+      <c r="O2509" s="98"/>
+      <c r="P2509" s="98"/>
+      <c r="Q2509" s="98"/>
+      <c r="R2509" s="98"/>
+      <c r="S2509" s="98"/>
+      <c r="T2509" s="98"/>
+      <c r="U2509" s="98"/>
+      <c r="V2509" s="98"/>
+      <c r="W2509" s="98"/>
+      <c r="X2509" s="98"/>
+      <c r="Y2509" s="98"/>
+      <c r="Z2509" s="98"/>
+      <c r="AA2509" s="98"/>
+      <c r="AB2509" s="98"/>
+      <c r="AC2509" s="98"/>
+      <c r="AD2509" s="98"/>
+      <c r="AE2509" s="98"/>
+      <c r="AF2509" s="98"/>
+      <c r="AG2509" s="98"/>
+      <c r="AH2509" s="98"/>
     </row>
     <row r="2598" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2598" s="103"/>
-      <c r="C2598" s="103"/>
-      <c r="D2598" s="103"/>
-      <c r="E2598" s="103"/>
-      <c r="F2598" s="103"/>
-      <c r="G2598" s="103"/>
-      <c r="H2598" s="103"/>
-      <c r="I2598" s="103"/>
-      <c r="J2598" s="103"/>
-      <c r="K2598" s="103"/>
-      <c r="L2598" s="103"/>
-      <c r="M2598" s="103"/>
-      <c r="N2598" s="103"/>
-      <c r="O2598" s="103"/>
-      <c r="P2598" s="103"/>
-      <c r="Q2598" s="103"/>
-      <c r="R2598" s="103"/>
-      <c r="S2598" s="103"/>
-      <c r="T2598" s="103"/>
-      <c r="U2598" s="103"/>
-      <c r="V2598" s="103"/>
-      <c r="W2598" s="103"/>
-      <c r="X2598" s="103"/>
-      <c r="Y2598" s="103"/>
-      <c r="Z2598" s="103"/>
-      <c r="AA2598" s="103"/>
-      <c r="AB2598" s="103"/>
-      <c r="AC2598" s="103"/>
-      <c r="AD2598" s="103"/>
-      <c r="AE2598" s="103"/>
-      <c r="AF2598" s="103"/>
-      <c r="AG2598" s="103"/>
-      <c r="AH2598" s="103"/>
+      <c r="B2598" s="98"/>
+      <c r="C2598" s="98"/>
+      <c r="D2598" s="98"/>
+      <c r="E2598" s="98"/>
+      <c r="F2598" s="98"/>
+      <c r="G2598" s="98"/>
+      <c r="H2598" s="98"/>
+      <c r="I2598" s="98"/>
+      <c r="J2598" s="98"/>
+      <c r="K2598" s="98"/>
+      <c r="L2598" s="98"/>
+      <c r="M2598" s="98"/>
+      <c r="N2598" s="98"/>
+      <c r="O2598" s="98"/>
+      <c r="P2598" s="98"/>
+      <c r="Q2598" s="98"/>
+      <c r="R2598" s="98"/>
+      <c r="S2598" s="98"/>
+      <c r="T2598" s="98"/>
+      <c r="U2598" s="98"/>
+      <c r="V2598" s="98"/>
+      <c r="W2598" s="98"/>
+      <c r="X2598" s="98"/>
+      <c r="Y2598" s="98"/>
+      <c r="Z2598" s="98"/>
+      <c r="AA2598" s="98"/>
+      <c r="AB2598" s="98"/>
+      <c r="AC2598" s="98"/>
+      <c r="AD2598" s="98"/>
+      <c r="AE2598" s="98"/>
+      <c r="AF2598" s="98"/>
+      <c r="AG2598" s="98"/>
+      <c r="AH2598" s="98"/>
     </row>
     <row r="2719" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2719" s="103"/>
-      <c r="C2719" s="103"/>
-      <c r="D2719" s="103"/>
-      <c r="E2719" s="103"/>
-      <c r="F2719" s="103"/>
-      <c r="G2719" s="103"/>
-      <c r="H2719" s="103"/>
-      <c r="I2719" s="103"/>
-      <c r="J2719" s="103"/>
-      <c r="K2719" s="103"/>
-      <c r="L2719" s="103"/>
-      <c r="M2719" s="103"/>
-      <c r="N2719" s="103"/>
-      <c r="O2719" s="103"/>
-      <c r="P2719" s="103"/>
-      <c r="Q2719" s="103"/>
-      <c r="R2719" s="103"/>
-      <c r="S2719" s="103"/>
-      <c r="T2719" s="103"/>
-      <c r="U2719" s="103"/>
-      <c r="V2719" s="103"/>
-      <c r="W2719" s="103"/>
-      <c r="X2719" s="103"/>
-      <c r="Y2719" s="103"/>
-      <c r="Z2719" s="103"/>
-      <c r="AA2719" s="103"/>
-      <c r="AB2719" s="103"/>
-      <c r="AC2719" s="103"/>
-      <c r="AD2719" s="103"/>
-      <c r="AE2719" s="103"/>
-      <c r="AF2719" s="103"/>
-      <c r="AG2719" s="103"/>
-      <c r="AH2719" s="103"/>
+      <c r="B2719" s="98"/>
+      <c r="C2719" s="98"/>
+      <c r="D2719" s="98"/>
+      <c r="E2719" s="98"/>
+      <c r="F2719" s="98"/>
+      <c r="G2719" s="98"/>
+      <c r="H2719" s="98"/>
+      <c r="I2719" s="98"/>
+      <c r="J2719" s="98"/>
+      <c r="K2719" s="98"/>
+      <c r="L2719" s="98"/>
+      <c r="M2719" s="98"/>
+      <c r="N2719" s="98"/>
+      <c r="O2719" s="98"/>
+      <c r="P2719" s="98"/>
+      <c r="Q2719" s="98"/>
+      <c r="R2719" s="98"/>
+      <c r="S2719" s="98"/>
+      <c r="T2719" s="98"/>
+      <c r="U2719" s="98"/>
+      <c r="V2719" s="98"/>
+      <c r="W2719" s="98"/>
+      <c r="X2719" s="98"/>
+      <c r="Y2719" s="98"/>
+      <c r="Z2719" s="98"/>
+      <c r="AA2719" s="98"/>
+      <c r="AB2719" s="98"/>
+      <c r="AC2719" s="98"/>
+      <c r="AD2719" s="98"/>
+      <c r="AE2719" s="98"/>
+      <c r="AF2719" s="98"/>
+      <c r="AG2719" s="98"/>
+      <c r="AH2719" s="98"/>
     </row>
     <row r="2837" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2837" s="103"/>
-      <c r="C2837" s="103"/>
-      <c r="D2837" s="103"/>
-      <c r="E2837" s="103"/>
-      <c r="F2837" s="103"/>
-      <c r="G2837" s="103"/>
-      <c r="H2837" s="103"/>
-      <c r="I2837" s="103"/>
-      <c r="J2837" s="103"/>
-      <c r="K2837" s="103"/>
-      <c r="L2837" s="103"/>
-      <c r="M2837" s="103"/>
-      <c r="N2837" s="103"/>
-      <c r="O2837" s="103"/>
-      <c r="P2837" s="103"/>
-      <c r="Q2837" s="103"/>
-      <c r="R2837" s="103"/>
-      <c r="S2837" s="103"/>
-      <c r="T2837" s="103"/>
-      <c r="U2837" s="103"/>
-      <c r="V2837" s="103"/>
-      <c r="W2837" s="103"/>
-      <c r="X2837" s="103"/>
-      <c r="Y2837" s="103"/>
-      <c r="Z2837" s="103"/>
-      <c r="AA2837" s="103"/>
-      <c r="AB2837" s="103"/>
-      <c r="AC2837" s="103"/>
-      <c r="AD2837" s="103"/>
-      <c r="AE2837" s="103"/>
-      <c r="AF2837" s="103"/>
-      <c r="AG2837" s="103"/>
-      <c r="AH2837" s="103"/>
+      <c r="B2837" s="98"/>
+      <c r="C2837" s="98"/>
+      <c r="D2837" s="98"/>
+      <c r="E2837" s="98"/>
+      <c r="F2837" s="98"/>
+      <c r="G2837" s="98"/>
+      <c r="H2837" s="98"/>
+      <c r="I2837" s="98"/>
+      <c r="J2837" s="98"/>
+      <c r="K2837" s="98"/>
+      <c r="L2837" s="98"/>
+      <c r="M2837" s="98"/>
+      <c r="N2837" s="98"/>
+      <c r="O2837" s="98"/>
+      <c r="P2837" s="98"/>
+      <c r="Q2837" s="98"/>
+      <c r="R2837" s="98"/>
+      <c r="S2837" s="98"/>
+      <c r="T2837" s="98"/>
+      <c r="U2837" s="98"/>
+      <c r="V2837" s="98"/>
+      <c r="W2837" s="98"/>
+      <c r="X2837" s="98"/>
+      <c r="Y2837" s="98"/>
+      <c r="Z2837" s="98"/>
+      <c r="AA2837" s="98"/>
+      <c r="AB2837" s="98"/>
+      <c r="AC2837" s="98"/>
+      <c r="AD2837" s="98"/>
+      <c r="AE2837" s="98"/>
+      <c r="AF2837" s="98"/>
+      <c r="AG2837" s="98"/>
+      <c r="AH2837" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B112:AH112"/>
-    <mergeCell ref="B122:AG122"/>
-    <mergeCell ref="B308:AH308"/>
-    <mergeCell ref="B511:AH511"/>
-    <mergeCell ref="B712:AH712"/>
-    <mergeCell ref="B887:AH887"/>
-    <mergeCell ref="B1100:AH1100"/>
-    <mergeCell ref="B1227:AH1227"/>
-    <mergeCell ref="B1390:AH1390"/>
-    <mergeCell ref="B1502:AH1502"/>
-    <mergeCell ref="B1604:AH1604"/>
-    <mergeCell ref="B1698:AH1698"/>
-    <mergeCell ref="B1945:AH1945"/>
-    <mergeCell ref="B2031:AH2031"/>
-    <mergeCell ref="B2719:AH2719"/>
     <mergeCell ref="B2837:AH2837"/>
     <mergeCell ref="B2153:AH2153"/>
     <mergeCell ref="B2317:AH2317"/>
     <mergeCell ref="B2419:AH2419"/>
     <mergeCell ref="B2509:AH2509"/>
     <mergeCell ref="B2598:AH2598"/>
+    <mergeCell ref="B1604:AH1604"/>
+    <mergeCell ref="B1698:AH1698"/>
+    <mergeCell ref="B1945:AH1945"/>
+    <mergeCell ref="B2031:AH2031"/>
+    <mergeCell ref="B2719:AH2719"/>
+    <mergeCell ref="B887:AH887"/>
+    <mergeCell ref="B1100:AH1100"/>
+    <mergeCell ref="B1227:AH1227"/>
+    <mergeCell ref="B1390:AH1390"/>
+    <mergeCell ref="B1502:AH1502"/>
+    <mergeCell ref="B112:AH112"/>
+    <mergeCell ref="B122:AG122"/>
+    <mergeCell ref="B308:AH308"/>
+    <mergeCell ref="B511:AH511"/>
+    <mergeCell ref="B712:AH712"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
@@ -55933,8 +56002,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD5C4245-EB16-4977-B50E-7C05C1E95418}">
-  <dimension ref="A1:AG14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B1F055-65F7-45E1-A7A7-497252B17989}">
+  <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
@@ -55942,35 +56011,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41" style="90" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="90" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="90" customWidth="1"/>
-    <col min="4" max="33" width="9.140625" style="90" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="90"/>
+    <col min="1" max="1" width="41" style="97" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="97" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="97" customWidth="1"/>
+    <col min="4" max="33" width="9.140625" style="97" customWidth="1"/>
+    <col min="34" max="16384" width="9.140625" style="97"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="97" t="s">
         <v>645</v>
       </c>
+      <c r="B1" s="97">
+        <v>3412.14</v>
+      </c>
+      <c r="C1" s="97" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="97" t="s">
         <v>646</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="97" t="s">
         <v>647</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="97" t="s">
         <v>648</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" s="90" t="s">
+      <c r="A6" s="97" t="s">
         <v>649</v>
       </c>
     </row>
@@ -56082,7 +56157,7 @@
       <c r="A10" s="93" t="s">
         <v>651</v>
       </c>
-      <c r="B10" s="94">
+      <c r="B10" s="114">
         <v>327892000</v>
       </c>
       <c r="C10" s="94">
@@ -56181,10 +56256,11 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="93" t="s">
-        <v>652</v>
-      </c>
-      <c r="B11" s="94">
-        <v>309326295</v>
+        <v>656</v>
+      </c>
+      <c r="B11" s="114">
+        <f>282200000</f>
+        <v>282200000</v>
       </c>
       <c r="C11" s="95"/>
       <c r="D11" s="95"/>
@@ -56218,12 +56294,13 @@
       <c r="AF11" s="95"/>
       <c r="AG11" s="95"/>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="93" t="s">
-        <v>653</v>
-      </c>
-      <c r="B12" s="95">
-        <v>210</v>
+        <v>657</v>
+      </c>
+      <c r="B12" s="97">
+        <f>123450*10^6</f>
+        <v>123450000000</v>
       </c>
       <c r="C12" s="96"/>
       <c r="D12" s="96"/>
@@ -56257,272 +56334,186 @@
       <c r="AF12" s="95"/>
       <c r="AG12" s="95"/>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="93" t="s">
-        <v>654</v>
-      </c>
-      <c r="B13" s="96">
-        <f>$B12*(B$10/$B11)</f>
-        <v>222.604159791847</v>
-      </c>
-      <c r="C13" s="96">
-        <f t="shared" ref="C13:AG13" si="0">$B12*(C$10/$B11)</f>
-        <v>224.21789263017553</v>
-      </c>
-      <c r="D13" s="96">
+        <v>658</v>
+      </c>
+      <c r="B13" s="97">
+        <f>B12*B1</f>
+        <v>421228683000000</v>
+      </c>
+      <c r="C13" s="96"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="96"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="96"/>
+      <c r="H13" s="96"/>
+      <c r="I13" s="96"/>
+      <c r="J13" s="96"/>
+      <c r="K13" s="96"/>
+      <c r="L13" s="96"/>
+      <c r="M13" s="96"/>
+      <c r="N13" s="96"/>
+      <c r="O13" s="96"/>
+      <c r="P13" s="96"/>
+      <c r="Q13" s="96"/>
+      <c r="R13" s="96"/>
+      <c r="S13" s="96"/>
+      <c r="T13" s="96"/>
+      <c r="U13" s="96"/>
+      <c r="V13" s="96"/>
+      <c r="W13" s="96"/>
+      <c r="X13" s="96"/>
+      <c r="Y13" s="96"/>
+      <c r="Z13" s="96"/>
+      <c r="AA13" s="95"/>
+      <c r="AB13" s="95"/>
+      <c r="AC13" s="95"/>
+      <c r="AD13" s="95"/>
+      <c r="AE13" s="95"/>
+      <c r="AF13" s="95"/>
+      <c r="AG13" s="95"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" s="93" t="s">
+        <v>652</v>
+      </c>
+      <c r="B14" s="115">
+        <f>$B$13*(B$10/$B11)</f>
+        <v>489431308739319.69</v>
+      </c>
+      <c r="C14" s="115">
+        <f t="shared" ref="C14:AG14" si="0">$B$13*(C$10/$B11)</f>
+        <v>492979361820435.88</v>
+      </c>
+      <c r="D14" s="115">
         <f t="shared" si="0"/>
-        <v>225.8268732052023</v>
-      </c>
-      <c r="E13" s="96">
+        <v>496516966280783.13</v>
+      </c>
+      <c r="E14" s="115">
         <f t="shared" si="0"/>
-        <v>227.4283859378977</v>
-      </c>
-      <c r="F13" s="96">
+        <v>500038151479922.06</v>
+      </c>
+      <c r="F14" s="115">
         <f t="shared" si="0"/>
-        <v>229.01971524923221</v>
-      </c>
-      <c r="G13" s="96">
+        <v>503536946777413.25</v>
+      </c>
+      <c r="G14" s="115">
         <f t="shared" si="0"/>
-        <v>230.59678777066139</v>
-      </c>
-      <c r="H13" s="96">
+        <v>507004396212597.5</v>
+      </c>
+      <c r="H14" s="115">
         <f t="shared" si="0"/>
-        <v>232.15688792315569</v>
-      </c>
-      <c r="I13" s="96">
+        <v>510434529145035.38</v>
+      </c>
+      <c r="I14" s="115">
         <f t="shared" si="0"/>
-        <v>233.69865791720036</v>
-      </c>
-      <c r="J13" s="96">
+        <v>513824360254507.5</v>
+      </c>
+      <c r="J14" s="115">
         <f t="shared" si="0"/>
-        <v>235.22413443706751</v>
-      </c>
-      <c r="K13" s="96">
+        <v>517178367521343</v>
+      </c>
+      <c r="K14" s="115">
         <f t="shared" si="0"/>
-        <v>236.72720742994062</v>
-      </c>
-      <c r="L13" s="96">
+        <v>520483117004553.5</v>
+      </c>
+      <c r="L14" s="115">
         <f t="shared" si="0"/>
-        <v>238.20516131679011</v>
-      </c>
-      <c r="M13" s="96">
+        <v>523732638063699.56</v>
+      </c>
+      <c r="M14" s="115">
         <f t="shared" si="0"/>
-        <v>239.65528051858635</v>
-      </c>
-      <c r="N13" s="96">
+        <v>526920960058341.63</v>
+      </c>
+      <c r="N14" s="115">
         <f t="shared" si="0"/>
-        <v>241.07620724581463</v>
-      </c>
-      <c r="O13" s="96">
+        <v>530045097668260.06</v>
+      </c>
+      <c r="O14" s="115">
         <f t="shared" si="0"/>
-        <v>242.46522591944534</v>
-      </c>
-      <c r="P13" s="96">
+        <v>533099080253015.56</v>
+      </c>
+      <c r="P14" s="115">
         <f t="shared" si="0"/>
-        <v>243.82301543423588</v>
-      </c>
-      <c r="Q13" s="96">
+        <v>536084400472717.94</v>
+      </c>
+      <c r="Q14" s="115">
         <f t="shared" si="0"/>
-        <v>245.14821800067142</v>
-      </c>
-      <c r="R13" s="96">
+        <v>538998073007147.38</v>
+      </c>
+      <c r="R14" s="115">
         <f t="shared" si="0"/>
-        <v>246.44083361875201</v>
-      </c>
-      <c r="S13" s="96">
+        <v>541840097856304.06</v>
+      </c>
+      <c r="S14" s="115">
         <f t="shared" si="0"/>
-        <v>247.70289897274981</v>
-      </c>
-      <c r="T13" s="96">
+        <v>544614953000517.38</v>
+      </c>
+      <c r="T14" s="115">
         <f t="shared" si="0"/>
-        <v>248.93441406266481</v>
-      </c>
-      <c r="U13" s="96">
+        <v>547322638439787.38</v>
+      </c>
+      <c r="U14" s="115">
         <f t="shared" si="0"/>
-        <v>250.13741557276919</v>
-      </c>
-      <c r="V13" s="96">
+        <v>549967632154443.63</v>
+      </c>
+      <c r="V14" s="115">
         <f t="shared" si="0"/>
-        <v>251.31258239782036</v>
-      </c>
-      <c r="W13" s="96">
+        <v>552551426804596</v>
+      </c>
+      <c r="W14" s="115">
         <f t="shared" si="0"/>
-        <v>252.46127232733318</v>
-      </c>
-      <c r="X13" s="96">
+        <v>555077007710464.19</v>
+      </c>
+      <c r="X14" s="115">
         <f t="shared" si="0"/>
-        <v>253.58620094033714</v>
-      </c>
-      <c r="Y13" s="96">
+        <v>557550345512487.56</v>
+      </c>
+      <c r="Y14" s="115">
         <f t="shared" si="0"/>
-        <v>254.68872602634704</v>
-      </c>
-      <c r="Z13" s="96">
+        <v>559974425530885.94</v>
+      </c>
+      <c r="Z14" s="115">
         <f t="shared" si="0"/>
-        <v>255.7708842696351</v>
-      </c>
-      <c r="AA13" s="96">
+        <v>562353725745988.63</v>
+      </c>
+      <c r="AA14" s="115">
         <f t="shared" si="0"/>
-        <v>256.83539124923084</v>
-      </c>
-      <c r="AB13" s="96">
+        <v>564694216798235.25</v>
+      </c>
+      <c r="AB14" s="115">
         <f t="shared" si="0"/>
-        <v>257.88564143892131</v>
-      </c>
-      <c r="AC13" s="96">
+        <v>567003361988175</v>
+      </c>
+      <c r="AC14" s="115">
         <f t="shared" si="0"/>
-        <v>258.92367152297868</v>
-      </c>
-      <c r="AD13" s="96">
+        <v>569285639296137.5</v>
+      </c>
+      <c r="AD14" s="115">
         <f t="shared" si="0"/>
-        <v>259.95355486994731</v>
-      </c>
-      <c r="AE13" s="96">
+        <v>571550004682781.75</v>
+      </c>
+      <c r="AE14" s="115">
         <f t="shared" si="0"/>
-        <v>260.97732816409933</v>
-      </c>
-      <c r="AF13" s="96">
+        <v>573800936128437.25</v>
+      </c>
+      <c r="AF14" s="115">
         <f t="shared" si="0"/>
-        <v>261.9977069844644</v>
-      </c>
-      <c r="AG13" s="96">
+        <v>576044404273543.63</v>
+      </c>
+      <c r="AG14" s="115">
         <f t="shared" si="0"/>
-        <v>263.0167280153147</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B14" s="97">
-        <f>B13*10^12</f>
-        <v>222604159791847</v>
-      </c>
-      <c r="C14" s="97">
-        <f t="shared" ref="C14:AG14" si="1">C13*10^12</f>
-        <v>224217892630175.53</v>
-      </c>
-      <c r="D14" s="97">
-        <f t="shared" si="1"/>
-        <v>225826873205202.31</v>
-      </c>
-      <c r="E14" s="97">
-        <f t="shared" si="1"/>
-        <v>227428385937897.69</v>
-      </c>
-      <c r="F14" s="97">
-        <f t="shared" si="1"/>
-        <v>229019715249232.22</v>
-      </c>
-      <c r="G14" s="97">
-        <f t="shared" si="1"/>
-        <v>230596787770661.41</v>
-      </c>
-      <c r="H14" s="97">
-        <f t="shared" si="1"/>
-        <v>232156887923155.69</v>
-      </c>
-      <c r="I14" s="97">
-        <f t="shared" si="1"/>
-        <v>233698657917200.38</v>
-      </c>
-      <c r="J14" s="97">
-        <f t="shared" si="1"/>
-        <v>235224134437067.5</v>
-      </c>
-      <c r="K14" s="97">
-        <f t="shared" si="1"/>
-        <v>236727207429940.63</v>
-      </c>
-      <c r="L14" s="97">
-        <f t="shared" si="1"/>
-        <v>238205161316790.13</v>
-      </c>
-      <c r="M14" s="97">
-        <f t="shared" si="1"/>
-        <v>239655280518586.34</v>
-      </c>
-      <c r="N14" s="97">
-        <f t="shared" si="1"/>
-        <v>241076207245814.63</v>
-      </c>
-      <c r="O14" s="97">
-        <f t="shared" si="1"/>
-        <v>242465225919445.34</v>
-      </c>
-      <c r="P14" s="97">
-        <f t="shared" si="1"/>
-        <v>243823015434235.88</v>
-      </c>
-      <c r="Q14" s="97">
-        <f t="shared" si="1"/>
-        <v>245148218000671.41</v>
-      </c>
-      <c r="R14" s="97">
-        <f t="shared" si="1"/>
-        <v>246440833618752</v>
-      </c>
-      <c r="S14" s="97">
-        <f t="shared" si="1"/>
-        <v>247702898972749.81</v>
-      </c>
-      <c r="T14" s="97">
-        <f t="shared" si="1"/>
-        <v>248934414062664.81</v>
-      </c>
-      <c r="U14" s="97">
-        <f t="shared" si="1"/>
-        <v>250137415572769.19</v>
-      </c>
-      <c r="V14" s="97">
-        <f t="shared" si="1"/>
-        <v>251312582397820.38</v>
-      </c>
-      <c r="W14" s="97">
-        <f t="shared" si="1"/>
-        <v>252461272327333.19</v>
-      </c>
-      <c r="X14" s="97">
-        <f t="shared" si="1"/>
-        <v>253586200940337.13</v>
-      </c>
-      <c r="Y14" s="97">
-        <f t="shared" si="1"/>
-        <v>254688726026347.03</v>
-      </c>
-      <c r="Z14" s="97">
-        <f t="shared" si="1"/>
-        <v>255770884269635.09</v>
-      </c>
-      <c r="AA14" s="97">
-        <f t="shared" si="1"/>
-        <v>256835391249230.84</v>
-      </c>
-      <c r="AB14" s="97">
-        <f t="shared" si="1"/>
-        <v>257885641438921.31</v>
-      </c>
-      <c r="AC14" s="97">
-        <f t="shared" si="1"/>
-        <v>258923671522978.69</v>
-      </c>
-      <c r="AD14" s="97">
-        <f t="shared" si="1"/>
-        <v>259953554869947.31</v>
-      </c>
-      <c r="AE14" s="97">
-        <f t="shared" si="1"/>
-        <v>260977328164099.34</v>
-      </c>
-      <c r="AF14" s="97">
-        <f t="shared" si="1"/>
-        <v>261997706984464.41</v>
-      </c>
-      <c r="AG14" s="97">
-        <f t="shared" si="1"/>
-        <v>263016728015314.69</v>
-      </c>
+        <v>578284887098430.13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AG15" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>